<commit_message>
Data for 1000 column
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631EDEEF-43FE-4378-A96A-AFB211EFED03}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B179D-D9B4-4774-B6B4-B8581E66657C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
   <si>
     <t>Input Size</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Java Default Sort</t>
-  </si>
-  <si>
-    <t>Randomness Sort</t>
   </si>
   <si>
     <t>Trump Sort</t>
@@ -536,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
-  <dimension ref="B2:H68"/>
+  <dimension ref="B2:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,7 +584,9 @@
       <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>14</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -600,7 +599,9 @@
       <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>12</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -613,7 +614,9 @@
       <c r="D6" s="15">
         <v>2</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="15">
+        <v>5</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -626,7 +629,9 @@
       <c r="D7" s="15">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="15">
+        <v>4</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -639,7 +644,9 @@
       <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -654,7 +661,9 @@
       <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7">
+        <v>17</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -667,7 +676,9 @@
       <c r="D10" s="15">
         <v>1</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="15">
+        <v>13</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -680,7 +691,9 @@
       <c r="D11" s="15">
         <v>1</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="15">
+        <v>4</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -693,7 +706,9 @@
       <c r="D12" s="15">
         <v>2</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="15">
+        <v>3</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -706,7 +721,9 @@
       <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5">
+        <v>2</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -721,7 +738,9 @@
       <c r="D14" s="7">
         <v>5</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7">
+        <v>21</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -734,7 +753,9 @@
       <c r="D15" s="15">
         <v>1</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="15">
+        <v>6</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -747,7 +768,9 @@
       <c r="D16" s="15">
         <v>1</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="15">
+        <v>4</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -760,7 +783,9 @@
       <c r="D17" s="15">
         <v>1</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="15">
+        <v>2</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -773,7 +798,9 @@
       <c r="D18" s="5">
         <v>0</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5">
+        <v>2</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -788,7 +815,9 @@
       <c r="D19" s="7">
         <v>5</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7">
+        <v>4</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -801,7 +830,9 @@
       <c r="D20" s="15">
         <v>0</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -814,7 +845,9 @@
       <c r="D21" s="15">
         <v>1</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -827,7 +860,9 @@
       <c r="D22" s="15">
         <v>0</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -840,7 +875,9 @@
       <c r="D23" s="5">
         <v>1</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -855,7 +892,9 @@
       <c r="D24" s="7">
         <v>8</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7">
+        <v>33</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -868,7 +907,9 @@
       <c r="D25" s="15">
         <v>5</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="15">
+        <v>69</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -881,7 +922,9 @@
       <c r="D26" s="15">
         <v>4</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="15">
+        <v>62</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -894,7 +937,9 @@
       <c r="D27" s="15">
         <v>3</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="15">
+        <v>2</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -907,7 +952,9 @@
       <c r="D28" s="5">
         <v>4</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -922,7 +969,9 @@
       <c r="D29" s="7">
         <v>2</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="7">
+        <v>2</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -935,7 +984,9 @@
       <c r="D30" s="15">
         <v>1</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="15">
+        <v>3</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -948,7 +999,9 @@
       <c r="D31" s="15">
         <v>1</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="15">
+        <v>1</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -961,7 +1014,9 @@
       <c r="D32" s="15">
         <v>1</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="E32" s="15">
+        <v>2</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -974,7 +1029,9 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -987,9 +1044,11 @@
         <v>2</v>
       </c>
       <c r="D34" s="7">
-        <v>8028</v>
-      </c>
-      <c r="E34" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E34" s="7">
+        <v>12</v>
+      </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -1000,9 +1059,11 @@
         <v>3</v>
       </c>
       <c r="D35" s="15">
-        <v>8091</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="E35" s="15">
+        <v>6</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1013,9 +1074,11 @@
         <v>4</v>
       </c>
       <c r="D36" s="15">
-        <v>8012</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E36" s="15">
+        <v>9</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1026,9 +1089,11 @@
         <v>5</v>
       </c>
       <c r="D37" s="15">
-        <v>8218</v>
-      </c>
-      <c r="E37" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="15">
+        <v>3</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1039,9 +1104,11 @@
         <v>6</v>
       </c>
       <c r="D38" s="5">
-        <v>7987</v>
-      </c>
-      <c r="E38" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="5">
+        <v>4</v>
+      </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
@@ -1054,9 +1121,11 @@
         <v>2</v>
       </c>
       <c r="D39" s="7">
-        <v>2</v>
-      </c>
-      <c r="E39" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -1067,9 +1136,11 @@
         <v>3</v>
       </c>
       <c r="D40" s="15">
-        <v>2</v>
-      </c>
-      <c r="E40" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="15">
+        <v>1</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -1080,9 +1151,11 @@
         <v>4</v>
       </c>
       <c r="D41" s="15">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="15">
+        <v>1</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -1093,9 +1166,11 @@
         <v>5</v>
       </c>
       <c r="D42" s="15">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="15">
+        <v>1</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -1108,7 +1183,9 @@
       <c r="D43" s="5">
         <v>1</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="E43" s="5">
+        <v>1</v>
+      </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
@@ -1121,9 +1198,11 @@
         <v>2</v>
       </c>
       <c r="D44" s="7">
-        <v>1</v>
-      </c>
-      <c r="E44" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1</v>
+      </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
@@ -1136,7 +1215,9 @@
       <c r="D45" s="15">
         <v>1</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="15">
+        <v>1</v>
+      </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -1149,7 +1230,9 @@
       <c r="D46" s="15">
         <v>0</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="E46" s="15">
+        <v>1</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -1162,7 +1245,9 @@
       <c r="D47" s="15">
         <v>0</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="E47" s="15">
+        <v>1</v>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -1173,9 +1258,11 @@
         <v>6</v>
       </c>
       <c r="D48" s="5">
-        <v>1</v>
-      </c>
-      <c r="E48" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="5">
+        <v>1</v>
+      </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
@@ -1188,9 +1275,11 @@
         <v>2</v>
       </c>
       <c r="D49" s="7">
-        <v>2</v>
-      </c>
-      <c r="E49" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="7">
+        <v>2</v>
+      </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -1203,7 +1292,9 @@
       <c r="D50" s="15">
         <v>1</v>
       </c>
-      <c r="E50" s="3"/>
+      <c r="E50" s="15">
+        <v>2</v>
+      </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -1216,7 +1307,9 @@
       <c r="D51" s="15">
         <v>0</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="E51" s="15">
+        <v>3</v>
+      </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -1229,7 +1322,9 @@
       <c r="D52" s="15">
         <v>0</v>
       </c>
-      <c r="E52" s="3"/>
+      <c r="E52" s="15">
+        <v>2</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -1242,7 +1337,9 @@
       <c r="D53" s="5">
         <v>0</v>
       </c>
-      <c r="E53" s="5"/>
+      <c r="E53" s="5">
+        <v>1</v>
+      </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
@@ -1257,7 +1354,9 @@
       <c r="D54" s="7">
         <v>1</v>
       </c>
-      <c r="E54" s="7"/>
+      <c r="E54" s="7">
+        <v>2</v>
+      </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -1270,7 +1369,9 @@
       <c r="D55" s="15">
         <v>1</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="15">
+        <v>1</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -1281,9 +1382,11 @@
         <v>4</v>
       </c>
       <c r="D56" s="15">
-        <v>0</v>
-      </c>
-      <c r="E56" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="15">
+        <v>1</v>
+      </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -1294,9 +1397,11 @@
         <v>5</v>
       </c>
       <c r="D57" s="15">
-        <v>0</v>
-      </c>
-      <c r="E57" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="15">
+        <v>1</v>
+      </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -1307,9 +1412,11 @@
         <v>6</v>
       </c>
       <c r="D58" s="5">
+        <v>1</v>
+      </c>
+      <c r="E58" s="5">
         <v>0</v>
       </c>
-      <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
@@ -1322,9 +1429,11 @@
         <v>2</v>
       </c>
       <c r="D59" s="7">
-        <v>1</v>
-      </c>
-      <c r="E59" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E59" s="7">
+        <v>1</v>
+      </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -1337,7 +1446,9 @@
       <c r="D60" s="15">
         <v>1</v>
       </c>
-      <c r="E60" s="3"/>
+      <c r="E60" s="15">
+        <v>1</v>
+      </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -1350,7 +1461,9 @@
       <c r="D61" s="15">
         <v>1</v>
       </c>
-      <c r="E61" s="3"/>
+      <c r="E61" s="15">
+        <v>1</v>
+      </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -1363,94 +1476,31 @@
       <c r="D62" s="15">
         <v>1</v>
       </c>
-      <c r="E62" s="3"/>
+      <c r="E62" s="15">
+        <v>0</v>
+      </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="12"/>
-      <c r="C63" s="4" t="s">
+      <c r="B63" s="13"/>
+      <c r="C63" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="5">
-        <v>1</v>
-      </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-    </row>
-    <row r="64" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" s="7">
-        <v>2</v>
-      </c>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="11"/>
-      <c r="C65" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="15">
-        <v>1</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="11"/>
-      <c r="C66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="15">
-        <v>1</v>
-      </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="11"/>
-      <c r="C67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="15">
-        <v>1</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="13"/>
-      <c r="C68" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="9">
-        <v>1</v>
-      </c>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
+      <c r="D63" s="9">
+        <v>1</v>
+      </c>
+      <c r="E63" s="9">
+        <v>1</v>
+      </c>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B39:B43"/>
+  <mergeCells count="13">
+    <mergeCell ref="B34:B38"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B9:B13"/>
@@ -1458,12 +1508,11 @@
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B39:B43"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="B49:B53"/>
     <mergeCell ref="B54:B58"/>
     <mergeCell ref="B59:B63"/>
-    <mergeCell ref="B64:B68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data for 100000 inputs
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920CFB87-5EDF-4D1B-AECB-FB39FFFD15CE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F174E-AD15-416C-A156-92C261017878}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B2:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,7 +590,9 @@
       <c r="F4" s="3">
         <v>511</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="15">
+        <v>61759</v>
+      </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
@@ -607,7 +609,9 @@
       <c r="F5" s="3">
         <v>502</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="15">
+        <v>60918</v>
+      </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
@@ -624,7 +628,9 @@
       <c r="F6" s="15">
         <v>444</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="15">
+        <v>54164</v>
+      </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
@@ -641,7 +647,9 @@
       <c r="F7" s="15">
         <v>534</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="15">
+        <v>52958</v>
+      </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -658,7 +666,9 @@
       <c r="F8" s="5">
         <v>504</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5">
+        <v>52913</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -677,7 +687,9 @@
       <c r="F9" s="7">
         <v>424</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7">
+        <v>56672</v>
+      </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
@@ -694,7 +706,9 @@
       <c r="F10" s="15">
         <v>420</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="15">
+        <v>56947</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
@@ -711,7 +725,9 @@
       <c r="F11" s="15">
         <v>288</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="15">
+        <v>58195</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
@@ -728,7 +744,9 @@
       <c r="F12" s="15">
         <v>285</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="15">
+        <v>57720</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -745,7 +763,9 @@
       <c r="F13" s="5">
         <v>322</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="5">
+        <v>58964</v>
+      </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -764,7 +784,9 @@
       <c r="F14" s="7">
         <v>249</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7">
+        <v>20797</v>
+      </c>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
@@ -781,7 +803,9 @@
       <c r="F15" s="15">
         <v>172</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="15">
+        <v>20644</v>
+      </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
@@ -798,7 +822,9 @@
       <c r="F16" s="15">
         <v>133</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="15">
+        <v>20445</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
@@ -815,7 +841,9 @@
       <c r="F17" s="15">
         <v>135</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="15">
+        <v>20424</v>
+      </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -832,7 +860,9 @@
       <c r="F18" s="5">
         <v>136</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="5">
+        <v>20371</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -851,7 +881,9 @@
       <c r="F19" s="7">
         <v>12</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="7">
+        <v>57</v>
+      </c>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
@@ -868,7 +900,9 @@
       <c r="F20" s="15">
         <v>7</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="15">
+        <v>25</v>
+      </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
@@ -885,7 +919,9 @@
       <c r="F21" s="15">
         <v>3</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="15">
+        <v>22</v>
+      </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
@@ -902,7 +938,9 @@
       <c r="F22" s="15">
         <v>2</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="15">
+        <v>22</v>
+      </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -919,7 +957,9 @@
       <c r="F23" s="5">
         <v>3</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5">
+        <v>26</v>
+      </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -938,7 +978,9 @@
       <c r="F24" s="7">
         <v>167</v>
       </c>
-      <c r="G24" s="7"/>
+      <c r="G24" s="7">
+        <v>317</v>
+      </c>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
@@ -955,7 +997,9 @@
       <c r="F25" s="15">
         <v>4</v>
       </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="15">
+        <v>65</v>
+      </c>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
@@ -972,7 +1016,9 @@
       <c r="F26" s="15">
         <v>19</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="15">
+        <v>46</v>
+      </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
@@ -989,7 +1035,9 @@
       <c r="F27" s="15">
         <v>4</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="15">
+        <v>58</v>
+      </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1006,7 +1054,9 @@
       <c r="F28" s="5">
         <v>4</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="5">
+        <v>60</v>
+      </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1025,7 +1075,9 @@
       <c r="F29" s="7">
         <v>15</v>
       </c>
-      <c r="G29" s="7"/>
+      <c r="G29" s="7">
+        <v>78</v>
+      </c>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
@@ -1042,7 +1094,9 @@
       <c r="F30" s="15">
         <v>4</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="15">
+        <v>224</v>
+      </c>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
@@ -1059,7 +1113,9 @@
       <c r="F31" s="15">
         <v>9</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="15">
+        <v>130</v>
+      </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
@@ -1076,7 +1132,9 @@
       <c r="F32" s="15">
         <v>11</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="15">
+        <v>78</v>
+      </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1093,7 +1151,9 @@
       <c r="F33" s="5">
         <v>20</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5">
+        <v>115</v>
+      </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1112,7 +1172,9 @@
       <c r="F34" s="7">
         <v>226</v>
       </c>
-      <c r="G34" s="7"/>
+      <c r="G34" s="7">
+        <v>17778</v>
+      </c>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.35">
@@ -1129,7 +1191,9 @@
       <c r="F35" s="15">
         <v>218</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="15">
+        <v>19389</v>
+      </c>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
@@ -1146,7 +1210,9 @@
       <c r="F36" s="15">
         <v>173</v>
       </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="15">
+        <v>23968</v>
+      </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.35">
@@ -1163,7 +1229,9 @@
       <c r="F37" s="15">
         <v>168</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="G37" s="15">
+        <v>23653</v>
+      </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1180,7 +1248,9 @@
       <c r="F38" s="5">
         <v>168</v>
       </c>
-      <c r="G38" s="5"/>
+      <c r="G38" s="5">
+        <v>24275</v>
+      </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1199,7 +1269,9 @@
       <c r="F39" s="7">
         <v>5</v>
       </c>
-      <c r="G39" s="7"/>
+      <c r="G39" s="7">
+        <v>7</v>
+      </c>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
@@ -1216,7 +1288,9 @@
       <c r="F40" s="15">
         <v>2</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="15">
+        <v>4</v>
+      </c>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
@@ -1233,7 +1307,9 @@
       <c r="F41" s="15">
         <v>2</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="15">
+        <v>2</v>
+      </c>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.35">
@@ -1250,7 +1326,9 @@
       <c r="F42" s="15">
         <v>1</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="15">
+        <v>2</v>
+      </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1267,7 +1345,9 @@
       <c r="F43" s="5">
         <v>1</v>
       </c>
-      <c r="G43" s="5"/>
+      <c r="G43" s="5">
+        <v>2</v>
+      </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1286,7 +1366,9 @@
       <c r="F44" s="7">
         <v>2</v>
       </c>
-      <c r="G44" s="7"/>
+      <c r="G44" s="7">
+        <v>3</v>
+      </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.35">
@@ -1303,7 +1385,9 @@
       <c r="F45" s="15">
         <v>1</v>
       </c>
-      <c r="G45" s="3"/>
+      <c r="G45" s="15">
+        <v>2</v>
+      </c>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.35">
@@ -1320,7 +1404,9 @@
       <c r="F46" s="15">
         <v>1</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="15">
+        <v>1</v>
+      </c>
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.35">
@@ -1337,7 +1423,9 @@
       <c r="F47" s="15">
         <v>0</v>
       </c>
-      <c r="G47" s="3"/>
+      <c r="G47" s="15">
+        <v>1</v>
+      </c>
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1354,7 +1442,9 @@
       <c r="F48" s="5">
         <v>1</v>
       </c>
-      <c r="G48" s="5"/>
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1373,7 +1463,9 @@
       <c r="F49" s="7">
         <v>13</v>
       </c>
-      <c r="G49" s="7"/>
+      <c r="G49" s="7">
+        <v>33</v>
+      </c>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
@@ -1390,7 +1482,9 @@
       <c r="F50" s="15">
         <v>5</v>
       </c>
-      <c r="G50" s="3"/>
+      <c r="G50" s="15">
+        <v>11</v>
+      </c>
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.35">
@@ -1407,7 +1501,9 @@
       <c r="F51" s="15">
         <v>2</v>
       </c>
-      <c r="G51" s="3"/>
+      <c r="G51" s="15">
+        <v>20</v>
+      </c>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.35">
@@ -1424,7 +1520,9 @@
       <c r="F52" s="15">
         <v>2</v>
       </c>
-      <c r="G52" s="3"/>
+      <c r="G52" s="15">
+        <v>19</v>
+      </c>
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1441,7 +1539,9 @@
       <c r="F53" s="5">
         <v>1</v>
       </c>
-      <c r="G53" s="5"/>
+      <c r="G53" s="5">
+        <v>18</v>
+      </c>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1460,7 +1560,9 @@
       <c r="F54" s="7">
         <v>4</v>
       </c>
-      <c r="G54" s="7"/>
+      <c r="G54" s="7">
+        <v>10</v>
+      </c>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.35">
@@ -1477,7 +1579,9 @@
       <c r="F55" s="15">
         <v>2</v>
       </c>
-      <c r="G55" s="3"/>
+      <c r="G55" s="15">
+        <v>14</v>
+      </c>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.35">
@@ -1494,7 +1598,9 @@
       <c r="F56" s="15">
         <v>3</v>
       </c>
-      <c r="G56" s="3"/>
+      <c r="G56" s="15">
+        <v>4</v>
+      </c>
       <c r="H56" s="3"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.35">
@@ -1511,7 +1617,9 @@
       <c r="F57" s="15">
         <v>2</v>
       </c>
-      <c r="G57" s="3"/>
+      <c r="G57" s="15">
+        <v>3</v>
+      </c>
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1528,7 +1636,9 @@
       <c r="F58" s="5">
         <v>1</v>
       </c>
-      <c r="G58" s="5"/>
+      <c r="G58" s="5">
+        <v>3</v>
+      </c>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1547,7 +1657,9 @@
       <c r="F59" s="7">
         <v>5</v>
       </c>
-      <c r="G59" s="7"/>
+      <c r="G59" s="7">
+        <v>11</v>
+      </c>
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.35">
@@ -1564,7 +1676,9 @@
       <c r="F60" s="15">
         <v>2</v>
       </c>
-      <c r="G60" s="3"/>
+      <c r="G60" s="15">
+        <v>17</v>
+      </c>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.35">
@@ -1581,7 +1695,9 @@
       <c r="F61" s="15">
         <v>2</v>
       </c>
-      <c r="G61" s="3"/>
+      <c r="G61" s="15">
+        <v>6</v>
+      </c>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.35">
@@ -1598,7 +1714,9 @@
       <c r="F62" s="15">
         <v>1</v>
       </c>
-      <c r="G62" s="3"/>
+      <c r="G62" s="15">
+        <v>3</v>
+      </c>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1615,7 +1733,9 @@
       <c r="F63" s="9">
         <v>1</v>
       </c>
-      <c r="G63" s="9"/>
+      <c r="G63" s="9">
+        <v>3</v>
+      </c>
       <c r="H63" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 1000000 inputs
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F174E-AD15-416C-A156-92C261017878}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF88BB-344A-42C7-93D5-355F73E2E547}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="19">
   <si>
     <t>Input Size</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Counting Sort</t>
+  </si>
+  <si>
+    <t>Unmeasureable</t>
   </si>
 </sst>
 </file>
@@ -535,13 +538,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B2:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
@@ -593,7 +597,9 @@
       <c r="G4" s="15">
         <v>61759</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
@@ -612,7 +618,9 @@
       <c r="G5" s="15">
         <v>60918</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
@@ -631,7 +639,9 @@
       <c r="G6" s="15">
         <v>54164</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="11"/>
@@ -650,7 +660,9 @@
       <c r="G7" s="15">
         <v>52958</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="12"/>
@@ -669,7 +681,9 @@
       <c r="G8" s="5">
         <v>52913</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -690,7 +704,9 @@
       <c r="G9" s="7">
         <v>56672</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
@@ -709,7 +725,9 @@
       <c r="G10" s="15">
         <v>56947</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
@@ -728,7 +746,9 @@
       <c r="G11" s="15">
         <v>58195</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
@@ -747,7 +767,9 @@
       <c r="G12" s="15">
         <v>57720</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="12"/>
@@ -766,7 +788,9 @@
       <c r="G13" s="5">
         <v>58964</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
@@ -787,7 +811,9 @@
       <c r="G14" s="7">
         <v>20797</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
@@ -806,7 +832,9 @@
       <c r="G15" s="15">
         <v>20644</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="11"/>
@@ -825,7 +853,9 @@
       <c r="G16" s="15">
         <v>20445</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="11"/>
@@ -844,7 +874,9 @@
       <c r="G17" s="15">
         <v>20424</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="12"/>
@@ -863,7 +895,9 @@
       <c r="G18" s="5">
         <v>20371</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10" t="s">
@@ -884,7 +918,9 @@
       <c r="G19" s="7">
         <v>57</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7">
+        <v>590</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="11"/>
@@ -903,7 +939,9 @@
       <c r="G20" s="15">
         <v>25</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="15">
+        <v>527</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="11"/>
@@ -922,7 +960,9 @@
       <c r="G21" s="15">
         <v>22</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="15">
+        <v>530</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
@@ -941,7 +981,9 @@
       <c r="G22" s="15">
         <v>22</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="15">
+        <v>522</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="12"/>
@@ -960,7 +1002,9 @@
       <c r="G23" s="5">
         <v>26</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5">
+        <v>542</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B24" s="10" t="s">
@@ -981,7 +1025,9 @@
       <c r="G24" s="7">
         <v>317</v>
       </c>
-      <c r="H24" s="7"/>
+      <c r="H24" s="7">
+        <v>920</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="11"/>
@@ -1000,7 +1046,9 @@
       <c r="G25" s="15">
         <v>65</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="15">
+        <v>820</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="11"/>
@@ -1019,7 +1067,9 @@
       <c r="G26" s="15">
         <v>46</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="15">
+        <v>741</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="11"/>
@@ -1038,7 +1088,9 @@
       <c r="G27" s="15">
         <v>58</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="15">
+        <v>941</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="12"/>
@@ -1057,7 +1109,9 @@
       <c r="G28" s="5">
         <v>60</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="5">
+        <v>941</v>
+      </c>
     </row>
     <row r="29" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10" t="s">
@@ -1078,7 +1132,9 @@
       <c r="G29" s="7">
         <v>78</v>
       </c>
-      <c r="H29" s="7"/>
+      <c r="H29" s="7">
+        <v>876</v>
+      </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="11"/>
@@ -1097,7 +1153,9 @@
       <c r="G30" s="15">
         <v>224</v>
       </c>
-      <c r="H30" s="3"/>
+      <c r="H30" s="15">
+        <v>618</v>
+      </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="11"/>
@@ -1116,7 +1174,9 @@
       <c r="G31" s="15">
         <v>130</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" s="15">
+        <v>467</v>
+      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="11"/>
@@ -1135,7 +1195,9 @@
       <c r="G32" s="15">
         <v>78</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="H32" s="15">
+        <v>467</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="12"/>
@@ -1154,7 +1216,9 @@
       <c r="G33" s="5">
         <v>115</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="5">
+        <v>509</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10" t="s">
@@ -1175,7 +1239,9 @@
       <c r="G34" s="7">
         <v>17778</v>
       </c>
-      <c r="H34" s="7"/>
+      <c r="H34" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="11"/>
@@ -1194,7 +1260,9 @@
       <c r="G35" s="15">
         <v>19389</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" s="11"/>
@@ -1213,7 +1281,9 @@
       <c r="G36" s="15">
         <v>23968</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="11"/>
@@ -1232,7 +1302,9 @@
       <c r="G37" s="15">
         <v>23653</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="H37" s="15" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="12"/>
@@ -1251,7 +1323,9 @@
       <c r="G38" s="5">
         <v>24275</v>
       </c>
-      <c r="H38" s="5"/>
+      <c r="H38" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B39" s="10" t="s">
@@ -1272,7 +1346,9 @@
       <c r="G39" s="7">
         <v>7</v>
       </c>
-      <c r="H39" s="7"/>
+      <c r="H39" s="7">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="11"/>
@@ -1291,7 +1367,9 @@
       <c r="G40" s="15">
         <v>4</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="15">
+        <v>45</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="11"/>
@@ -1310,7 +1388,9 @@
       <c r="G41" s="15">
         <v>2</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="15">
+        <v>35</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" s="11"/>
@@ -1329,7 +1409,9 @@
       <c r="G42" s="15">
         <v>2</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="15">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="12"/>
@@ -1348,7 +1430,9 @@
       <c r="G43" s="5">
         <v>2</v>
       </c>
-      <c r="H43" s="5"/>
+      <c r="H43" s="5">
+        <v>43</v>
+      </c>
     </row>
     <row r="44" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B44" s="10" t="s">
@@ -1369,7 +1453,9 @@
       <c r="G44" s="7">
         <v>3</v>
       </c>
-      <c r="H44" s="7"/>
+      <c r="H44" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="11"/>
@@ -1388,7 +1474,9 @@
       <c r="G45" s="15">
         <v>2</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="11"/>
@@ -1407,7 +1495,9 @@
       <c r="G46" s="15">
         <v>1</v>
       </c>
-      <c r="H46" s="3"/>
+      <c r="H46" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="11"/>
@@ -1426,7 +1516,9 @@
       <c r="G47" s="15">
         <v>1</v>
       </c>
-      <c r="H47" s="3"/>
+      <c r="H47" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="48" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="12"/>
@@ -1445,7 +1537,9 @@
       <c r="G48" s="5">
         <v>1</v>
       </c>
-      <c r="H48" s="5"/>
+      <c r="H48" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B49" s="10" t="s">
@@ -1466,7 +1560,9 @@
       <c r="G49" s="7">
         <v>33</v>
       </c>
-      <c r="H49" s="7"/>
+      <c r="H49" s="7">
+        <v>313</v>
+      </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B50" s="11"/>
@@ -1485,7 +1581,9 @@
       <c r="G50" s="15">
         <v>11</v>
       </c>
-      <c r="H50" s="3"/>
+      <c r="H50" s="15">
+        <v>257</v>
+      </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B51" s="11"/>
@@ -1504,7 +1602,9 @@
       <c r="G51" s="15">
         <v>20</v>
       </c>
-      <c r="H51" s="3"/>
+      <c r="H51" s="15">
+        <v>259</v>
+      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B52" s="11"/>
@@ -1523,7 +1623,9 @@
       <c r="G52" s="15">
         <v>19</v>
       </c>
-      <c r="H52" s="3"/>
+      <c r="H52" s="15">
+        <v>406</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B53" s="12"/>
@@ -1542,7 +1644,9 @@
       <c r="G53" s="5">
         <v>18</v>
       </c>
-      <c r="H53" s="5"/>
+      <c r="H53" s="5">
+        <v>295</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B54" s="10" t="s">
@@ -1563,7 +1667,9 @@
       <c r="G54" s="7">
         <v>10</v>
       </c>
-      <c r="H54" s="7"/>
+      <c r="H54" s="7">
+        <v>58</v>
+      </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B55" s="11"/>
@@ -1582,7 +1688,9 @@
       <c r="G55" s="15">
         <v>14</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="15">
+        <v>125</v>
+      </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56" s="11"/>
@@ -1601,7 +1709,9 @@
       <c r="G56" s="15">
         <v>4</v>
       </c>
-      <c r="H56" s="3"/>
+      <c r="H56" s="15">
+        <v>46</v>
+      </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B57" s="11"/>
@@ -1620,7 +1730,9 @@
       <c r="G57" s="15">
         <v>3</v>
       </c>
-      <c r="H57" s="3"/>
+      <c r="H57" s="15">
+        <v>39</v>
+      </c>
     </row>
     <row r="58" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="12"/>
@@ -1639,7 +1751,9 @@
       <c r="G58" s="5">
         <v>3</v>
       </c>
-      <c r="H58" s="5"/>
+      <c r="H58" s="5">
+        <v>34</v>
+      </c>
     </row>
     <row r="59" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
@@ -1660,7 +1774,9 @@
       <c r="G59" s="7">
         <v>11</v>
       </c>
-      <c r="H59" s="7"/>
+      <c r="H59" s="7">
+        <v>153</v>
+      </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B60" s="11"/>
@@ -1679,7 +1795,9 @@
       <c r="G60" s="15">
         <v>17</v>
       </c>
-      <c r="H60" s="3"/>
+      <c r="H60" s="15">
+        <v>146</v>
+      </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B61" s="11"/>
@@ -1698,7 +1816,9 @@
       <c r="G61" s="15">
         <v>6</v>
       </c>
-      <c r="H61" s="3"/>
+      <c r="H61" s="15">
+        <v>191</v>
+      </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B62" s="11"/>
@@ -1717,7 +1837,9 @@
       <c r="G62" s="15">
         <v>3</v>
       </c>
-      <c r="H62" s="3"/>
+      <c r="H62" s="15">
+        <v>107</v>
+      </c>
     </row>
     <row r="63" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B63" s="13"/>
@@ -1736,7 +1858,9 @@
       <c r="G63" s="9">
         <v>3</v>
       </c>
-      <c r="H63" s="9"/>
+      <c r="H63" s="9">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Data for 10000000 inputs
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF88BB-344A-42C7-93D5-355F73E2E547}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D4FEE7-62EB-4AA4-B516-E45150959A74}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="19">
   <si>
     <t>Input Size</t>
   </si>
@@ -536,19 +536,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
-  <dimension ref="B2:H63"/>
+  <dimension ref="B2:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="14" t="s">
@@ -559,7 +559,7 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1">
@@ -577,8 +577,11 @@
       <c r="H3" s="1">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -600,8 +603,11 @@
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -621,8 +627,11 @@
       <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>4</v>
@@ -642,8 +651,11 @@
       <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -663,8 +675,11 @@
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>6</v>
@@ -684,8 +699,11 @@
       <c r="H8" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
@@ -707,8 +725,11 @@
       <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
         <v>3</v>
@@ -728,8 +749,11 @@
       <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
         <v>4</v>
@@ -749,8 +773,11 @@
       <c r="H11" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -770,8 +797,11 @@
       <c r="H12" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="12"/>
       <c r="C13" s="4" t="s">
         <v>6</v>
@@ -788,11 +818,14 @@
       <c r="G13" s="5">
         <v>58964</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
@@ -814,8 +847,11 @@
       <c r="H14" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
@@ -835,8 +871,11 @@
       <c r="H15" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="11"/>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -856,8 +895,11 @@
       <c r="H16" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="11"/>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -877,8 +919,11 @@
       <c r="H17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>6</v>
@@ -898,8 +943,11 @@
       <c r="H18" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
@@ -921,8 +969,11 @@
       <c r="H19" s="7">
         <v>590</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I19" s="15">
+        <v>7922</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="11"/>
       <c r="C20" s="2" t="s">
         <v>3</v>
@@ -942,8 +993,11 @@
       <c r="H20" s="15">
         <v>527</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="15">
+        <v>8560</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="11"/>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -963,8 +1017,11 @@
       <c r="H21" s="15">
         <v>530</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="15">
+        <v>8649</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
       <c r="C22" s="2" t="s">
         <v>5</v>
@@ -984,8 +1041,11 @@
       <c r="H22" s="15">
         <v>522</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I22" s="15">
+        <v>8448</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="12"/>
       <c r="C23" s="4" t="s">
         <v>6</v>
@@ -1005,8 +1065,11 @@
       <c r="H23" s="5">
         <v>542</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="5">
+        <v>8416</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B24" s="10" t="s">
         <v>10</v>
       </c>
@@ -1028,8 +1091,11 @@
       <c r="H24" s="7">
         <v>920</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="15">
+        <v>13203</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="11"/>
       <c r="C25" s="2" t="s">
         <v>3</v>
@@ -1049,8 +1115,11 @@
       <c r="H25" s="15">
         <v>820</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="15">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="11"/>
       <c r="C26" s="2" t="s">
         <v>4</v>
@@ -1070,8 +1139,11 @@
       <c r="H26" s="15">
         <v>741</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I26" s="15">
+        <v>11544</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="11"/>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1091,8 +1163,11 @@
       <c r="H27" s="15">
         <v>941</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="15">
+        <v>11184</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="12"/>
       <c r="C28" s="4" t="s">
         <v>6</v>
@@ -1112,8 +1187,11 @@
       <c r="H28" s="5">
         <v>941</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="5">
+        <v>11648</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10" t="s">
         <v>11</v>
       </c>
@@ -1135,8 +1213,11 @@
       <c r="H29" s="7">
         <v>876</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I29" s="15">
+        <v>8678</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="11"/>
       <c r="C30" s="2" t="s">
         <v>3</v>
@@ -1156,8 +1237,11 @@
       <c r="H30" s="15">
         <v>618</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="15">
+        <v>8168</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="11"/>
       <c r="C31" s="2" t="s">
         <v>4</v>
@@ -1177,8 +1261,11 @@
       <c r="H31" s="15">
         <v>467</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I31" s="15">
+        <v>8512</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="11"/>
       <c r="C32" s="2" t="s">
         <v>5</v>
@@ -1198,8 +1285,11 @@
       <c r="H32" s="15">
         <v>467</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I32" s="15">
+        <v>7909</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="12"/>
       <c r="C33" s="4" t="s">
         <v>6</v>
@@ -1219,8 +1309,11 @@
       <c r="H33" s="5">
         <v>509</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I33" s="5">
+        <v>7723</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10" t="s">
         <v>12</v>
       </c>
@@ -1242,8 +1335,11 @@
       <c r="H34" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I34" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="11"/>
       <c r="C35" s="2" t="s">
         <v>3</v>
@@ -1263,8 +1359,11 @@
       <c r="H35" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I35" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="11"/>
       <c r="C36" s="2" t="s">
         <v>4</v>
@@ -1284,8 +1383,11 @@
       <c r="H36" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I36" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="11"/>
       <c r="C37" s="2" t="s">
         <v>5</v>
@@ -1305,8 +1407,11 @@
       <c r="H37" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I37" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="12"/>
       <c r="C38" s="4" t="s">
         <v>6</v>
@@ -1326,8 +1431,11 @@
       <c r="H38" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I38" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B39" s="10" t="s">
         <v>13</v>
       </c>
@@ -1349,8 +1457,11 @@
       <c r="H39" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I39" s="15">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="11"/>
       <c r="C40" s="2" t="s">
         <v>3</v>
@@ -1370,8 +1481,11 @@
       <c r="H40" s="15">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I40" s="15">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="11"/>
       <c r="C41" s="2" t="s">
         <v>4</v>
@@ -1391,8 +1505,11 @@
       <c r="H41" s="15">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I41" s="15">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="11"/>
       <c r="C42" s="2" t="s">
         <v>5</v>
@@ -1412,8 +1529,11 @@
       <c r="H42" s="15">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I42" s="15">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="12"/>
       <c r="C43" s="4" t="s">
         <v>6</v>
@@ -1433,8 +1553,11 @@
       <c r="H43" s="5">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I43" s="5">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B44" s="10" t="s">
         <v>14</v>
       </c>
@@ -1456,8 +1579,11 @@
       <c r="H44" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I44" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="11"/>
       <c r="C45" s="2" t="s">
         <v>3</v>
@@ -1477,8 +1603,11 @@
       <c r="H45" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I45" s="15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="11"/>
       <c r="C46" s="2" t="s">
         <v>4</v>
@@ -1498,8 +1627,11 @@
       <c r="H46" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I46" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="11"/>
       <c r="C47" s="2" t="s">
         <v>5</v>
@@ -1519,8 +1651,11 @@
       <c r="H47" s="15">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I47" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="12"/>
       <c r="C48" s="4" t="s">
         <v>6</v>
@@ -1540,8 +1675,11 @@
       <c r="H48" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I48" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B49" s="10" t="s">
         <v>15</v>
       </c>
@@ -1563,8 +1701,11 @@
       <c r="H49" s="7">
         <v>313</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I49" s="15">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" s="11"/>
       <c r="C50" s="2" t="s">
         <v>3</v>
@@ -1584,8 +1725,11 @@
       <c r="H50" s="15">
         <v>257</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I50" s="15">
+        <v>4360</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" s="11"/>
       <c r="C51" s="2" t="s">
         <v>4</v>
@@ -1605,8 +1749,11 @@
       <c r="H51" s="15">
         <v>259</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I51" s="15">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="11"/>
       <c r="C52" s="2" t="s">
         <v>5</v>
@@ -1626,8 +1773,11 @@
       <c r="H52" s="15">
         <v>406</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I52" s="15">
+        <v>4857</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B53" s="12"/>
       <c r="C53" s="4" t="s">
         <v>6</v>
@@ -1647,8 +1797,11 @@
       <c r="H53" s="5">
         <v>295</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I53" s="5">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B54" s="10" t="s">
         <v>16</v>
       </c>
@@ -1670,8 +1823,11 @@
       <c r="H54" s="7">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I54" s="15">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" s="11"/>
       <c r="C55" s="2" t="s">
         <v>3</v>
@@ -1691,8 +1847,11 @@
       <c r="H55" s="15">
         <v>125</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I55" s="15">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="11"/>
       <c r="C56" s="2" t="s">
         <v>4</v>
@@ -1712,8 +1871,11 @@
       <c r="H56" s="15">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I56" s="15">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="11"/>
       <c r="C57" s="2" t="s">
         <v>5</v>
@@ -1733,8 +1895,11 @@
       <c r="H57" s="15">
         <v>39</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I57" s="15">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="12"/>
       <c r="C58" s="4" t="s">
         <v>6</v>
@@ -1754,8 +1919,11 @@
       <c r="H58" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I58" s="5">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
         <v>17</v>
       </c>
@@ -1777,8 +1945,11 @@
       <c r="H59" s="7">
         <v>153</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I59" s="15">
+        <v>12638</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="11"/>
       <c r="C60" s="2" t="s">
         <v>3</v>
@@ -1798,8 +1969,11 @@
       <c r="H60" s="15">
         <v>146</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I60" s="15">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="11"/>
       <c r="C61" s="2" t="s">
         <v>4</v>
@@ -1819,8 +1993,11 @@
       <c r="H61" s="15">
         <v>191</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I61" s="15">
+        <v>5037</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="11"/>
       <c r="C62" s="2" t="s">
         <v>5</v>
@@ -1840,8 +2017,11 @@
       <c r="H62" s="15">
         <v>107</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I62" s="15">
+        <v>12883</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B63" s="13"/>
       <c r="C63" s="8" t="s">
         <v>6</v>
@@ -1860,6 +2040,9 @@
       </c>
       <c r="H63" s="9">
         <v>119</v>
+      </c>
+      <c r="I63" s="9">
+        <v>11523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert from Comparable to int
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F37B73-2F53-4FA8-8985-0A907C6394E3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA1B6D6-0599-4077-BD7F-D8CAC89E44F3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
New data for 100
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA1B6D6-0599-4077-BD7F-D8CAC89E44F3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80D9DA1-EFC6-442A-B989-2EDAE540D43E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="10">
         <v>2</v>
@@ -735,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11" s="7">
         <v>17</v>
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="10">
         <v>13</v>
@@ -807,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="10">
         <v>3</v>
@@ -831,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="5">
         <v>2</v>
@@ -857,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="7">
         <v>6</v>
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="10">
         <v>18</v>
@@ -979,7 +979,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21" s="7">
         <v>4</v>
@@ -1003,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="10">
         <v>1</v>
@@ -1051,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="10">
         <v>1</v>
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -1101,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E26" s="7">
         <v>33</v>
@@ -1125,7 +1125,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E27" s="10">
         <v>69</v>
@@ -1149,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E28" s="10">
         <v>62</v>
@@ -1173,7 +1173,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E29" s="10">
         <v>2</v>
@@ -1197,7 +1197,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
@@ -1223,7 +1223,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="7">
         <v>2</v>
@@ -1345,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="7">
         <v>12</v>
@@ -1369,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="D37" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="10">
         <v>6</v>
@@ -1515,7 +1515,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="10">
         <v>1</v>
@@ -1539,7 +1539,7 @@
         <v>5</v>
       </c>
       <c r="D44" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="10">
         <v>1</v>
@@ -1589,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="7">
         <v>1</v>
@@ -1637,7 +1637,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="10">
         <v>1</v>
@@ -1661,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="10">
         <v>1</v>
@@ -1759,7 +1759,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="10">
         <v>3</v>
@@ -1783,7 +1783,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="10">
         <v>2</v>
@@ -1881,7 +1881,7 @@
         <v>4</v>
       </c>
       <c r="D58" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" s="10">
         <v>1</v>
@@ -1955,7 +1955,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" s="7">
         <v>1</v>
@@ -2027,7 +2027,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
Add Shell Sort to spreadsheet
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5609C14-6A5F-41EB-8086-94F32049AA45}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8421E5E3-4EF8-45EB-AD19-FB2479EA8DC0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
   <si>
     <t>Input Size</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Written in Java. No multithreading used. Application was closed and re-opened every time sorting method or input size was changed.</t>
+  </si>
+  <si>
+    <t>Shell Sort</t>
+  </si>
+  <si>
+    <t>Trial 6</t>
+  </si>
+  <si>
+    <t>Trial 7</t>
+  </si>
+  <si>
+    <t>Trial 8</t>
+  </si>
+  <si>
+    <t>Trial 9</t>
+  </si>
+  <si>
+    <t>Trial 10</t>
   </si>
 </sst>
 </file>
@@ -105,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -171,31 +189,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -204,8 +202,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -222,9 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
-  <dimension ref="B1:I65"/>
+  <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,33 +546,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
@@ -603,7 +597,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -614,12 +608,12 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
@@ -628,40 +622,40 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="14"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
@@ -675,7 +669,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -691,49 +685,49 @@
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="8">
         <v>0</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="14"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
         <v>6</v>
       </c>
@@ -747,7 +741,7 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -763,49 +757,49 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="10">
-        <v>1</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="10">
-        <v>1</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="10">
-        <v>1</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="14"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4" t="s">
         <v>6</v>
       </c>
@@ -819,70 +813,70 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="12" t="s">
-        <v>9</v>
+      <c r="B21" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="10"/>
+      <c r="I21" s="14"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="13"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="10">
-        <v>1</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="10">
-        <v>1</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="14"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -891,71 +885,61 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="12" t="s">
-        <v>10</v>
+      <c r="B26" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="7">
-        <v>11</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="10"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="10">
-        <v>9</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="10">
-        <v>5</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="10">
-        <v>7</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="14"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="5">
-        <v>3</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -963,70 +947,70 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="12" t="s">
-        <v>11</v>
+      <c r="B31" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="10"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="10">
-        <v>1</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B33" s="13"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="10">
-        <v>1</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
+      <c r="D33" s="8">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="13"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
     </row>
     <row r="35" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="14"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1035,70 +1019,70 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="12" t="s">
-        <v>12</v>
+      <c r="B36" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
+      <c r="I36" s="8"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B37" s="13"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="10">
-        <v>1</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="D37" s="8">
+        <v>9</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B38" s="13"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="10">
-        <v>1</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="D38" s="8">
+        <v>5</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B39" s="13"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="10">
-        <v>1</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
+      <c r="D39" s="8">
+        <v>7</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="14"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1107,8 +1091,8 @@
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="12" t="s">
-        <v>13</v>
+      <c r="B41" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>2</v>
@@ -1120,52 +1104,52 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
-      <c r="I41" s="10"/>
+      <c r="I41" s="8"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B42" s="13"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="10">
-        <v>1</v>
-      </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="D42" s="8">
+        <v>1</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B43" s="13"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="10">
-        <v>1</v>
-      </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
+      <c r="D43" s="8">
+        <v>1</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B44" s="13"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="10">
-        <v>1</v>
-      </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
+      <c r="D44" s="8">
+        <v>1</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
     </row>
     <row r="45" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="14"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="4" t="s">
         <v>6</v>
       </c>
@@ -1179,8 +1163,8 @@
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="12" t="s">
-        <v>14</v>
+      <c r="B46" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>2</v>
@@ -1192,57 +1176,57 @@
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
-      <c r="I46" s="10"/>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B47" s="13"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="10">
-        <v>1</v>
-      </c>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
+      <c r="D47" s="8">
+        <v>1</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B48" s="13"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="10">
-        <v>1</v>
-      </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
+      <c r="D48" s="8">
+        <v>1</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B49" s="13"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="10">
-        <v>1</v>
-      </c>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
+      <c r="D49" s="8">
+        <v>1</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
     </row>
     <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="14"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -1251,8 +1235,8 @@
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="12" t="s">
-        <v>15</v>
+      <c r="B51" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>2</v>
@@ -1264,57 +1248,57 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="10"/>
+      <c r="I51" s="8"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B52" s="13"/>
+      <c r="B52" s="11"/>
       <c r="C52" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="10">
-        <v>1</v>
-      </c>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
+      <c r="D52" s="8">
+        <v>1</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B53" s="13"/>
+      <c r="B53" s="11"/>
       <c r="C53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="10">
-        <v>1</v>
-      </c>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
+      <c r="D53" s="8">
+        <v>1</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B54" s="13"/>
+      <c r="B54" s="11"/>
       <c r="C54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="10">
-        <v>1</v>
-      </c>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
+      <c r="D54" s="8">
+        <v>1</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
     </row>
     <row r="55" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="14"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -1323,8 +1307,8 @@
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="12" t="s">
-        <v>16</v>
+      <c r="B56" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>2</v>
@@ -1336,57 +1320,57 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
-      <c r="I56" s="10"/>
+      <c r="I56" s="8"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B57" s="13"/>
+      <c r="B57" s="11"/>
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="10">
-        <v>1</v>
-      </c>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
+      <c r="D57" s="8">
+        <v>1</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B58" s="13"/>
+      <c r="B58" s="11"/>
       <c r="C58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="10">
-        <v>0</v>
-      </c>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
+      <c r="D58" s="8">
+        <v>1</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B59" s="13"/>
+      <c r="B59" s="11"/>
       <c r="C59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="10">
-        <v>1</v>
-      </c>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
+      <c r="D59" s="8">
+        <v>1</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
     </row>
     <row r="60" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="14"/>
+      <c r="B60" s="12"/>
       <c r="C60" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -1395,8 +1379,8 @@
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="12" t="s">
-        <v>17</v>
+      <c r="B61" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>2</v>
@@ -1408,80 +1392,154 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
-      <c r="I61" s="10"/>
+      <c r="I61" s="8"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B62" s="13"/>
+      <c r="B62" s="11"/>
       <c r="C62" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="10">
-        <v>1</v>
-      </c>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
+      <c r="D62" s="8">
+        <v>1</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B63" s="13"/>
+      <c r="B63" s="11"/>
       <c r="C63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="10">
-        <v>1</v>
-      </c>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
+      <c r="D63" s="8">
+        <v>1</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B64" s="13"/>
+      <c r="B64" s="11"/>
       <c r="C64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="8">
+        <v>1</v>
+      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+    </row>
+    <row r="65" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="12"/>
+      <c r="C65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="5">
         <v>0</v>
       </c>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-    </row>
-    <row r="65" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="16"/>
-      <c r="C65" s="8" t="s">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="7">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="8"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B67" s="11"/>
+      <c r="C67" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="8">
+        <v>1</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B68" s="11"/>
+      <c r="C68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="8">
+        <v>0</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B69" s="11"/>
+      <c r="C69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="8">
+        <v>1</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+    </row>
+    <row r="70" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="12"/>
+      <c r="C70" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="9">
-        <v>1</v>
-      </c>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-    </row>
+      <c r="D70" s="5">
+        <v>1</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B50"/>
+  <mergeCells count="15">
+    <mergeCell ref="B26:B30"/>
     <mergeCell ref="B51:B55"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="B21:B25"/>
     <mergeCell ref="D1:I2"/>
-    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B46:B50"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B30"/>
     <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B41:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add all new algorithms
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8421E5E3-4EF8-45EB-AD19-FB2479EA8DC0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37F0984-0428-4630-B272-B7C2779BA17E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
   <si>
     <t>Input Size</t>
   </si>
@@ -87,19 +87,13 @@
     <t>Shell Sort</t>
   </si>
   <si>
-    <t>Trial 6</t>
-  </si>
-  <si>
-    <t>Trial 7</t>
-  </si>
-  <si>
-    <t>Trial 8</t>
-  </si>
-  <si>
-    <t>Trial 9</t>
-  </si>
-  <si>
-    <t>Trial 10</t>
+    <t>Heap Sort</t>
+  </si>
+  <si>
+    <t>Comb Sort</t>
+  </si>
+  <si>
+    <t>Pigeonhole Sort</t>
   </si>
 </sst>
 </file>
@@ -203,9 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -215,10 +207,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
-  <dimension ref="B1:I71"/>
+  <dimension ref="B1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,33 +540,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
@@ -592,7 +586,7 @@
       <c r="H5" s="1">
         <v>1000000</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>10000000</v>
       </c>
     </row>
@@ -669,18 +663,16 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7">
-        <v>2</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="B11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
@@ -689,11 +681,9 @@
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="8"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -703,9 +693,7 @@
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
+      <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -717,9 +705,7 @@
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -731,9 +717,7 @@
       <c r="C15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -742,7 +726,7 @@
     </row>
     <row r="16" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>2</v>
@@ -762,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -804,80 +788,70 @@
         <v>6</v>
       </c>
       <c r="D20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="7">
-        <v>1</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="14"/>
+      <c r="B21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="8">
-        <v>1</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="8">
-        <v>1</v>
-      </c>
+      <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="8">
-        <v>0</v>
-      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -886,90 +860,96 @@
     </row>
     <row r="26" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B26" s="10" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="11"/>
       <c r="C27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="11"/>
       <c r="C28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="11"/>
       <c r="C29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="12"/>
       <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B31" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="7">
-        <v>2</v>
-      </c>
+      <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="11"/>
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="8">
-        <v>1</v>
-      </c>
+      <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -981,9 +961,7 @@
       <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="8">
-        <v>1</v>
-      </c>
+      <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -995,9 +973,7 @@
       <c r="C34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="8">
-        <v>1</v>
-      </c>
+      <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -1009,9 +985,7 @@
       <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1020,13 +994,13 @@
     </row>
     <row r="36" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="7">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -1040,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="D37" s="8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1054,7 +1028,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1068,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1082,7 +1056,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1092,13 +1066,13 @@
     </row>
     <row r="41" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="7">
         <v>11</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="7">
-        <v>1</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -1112,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -1126,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1140,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="D44" s="8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1154,7 +1128,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -1164,7 +1138,7 @@
     </row>
     <row r="46" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B46" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>2</v>
@@ -1176,7 +1150,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="11"/>
@@ -1189,8 +1163,8 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" s="11"/>
@@ -1203,8 +1177,8 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="11"/>
@@ -1236,7 +1210,7 @@
     </row>
     <row r="51" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B51" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>2</v>
@@ -1248,7 +1222,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="8"/>
+      <c r="I51" s="7"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="11"/>
@@ -1261,8 +1235,8 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="11"/>
@@ -1275,8 +1249,8 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="11"/>
@@ -1308,7 +1282,7 @@
     </row>
     <row r="56" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B56" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>2</v>
@@ -1370,7 +1344,7 @@
         <v>6</v>
       </c>
       <c r="D60" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -1380,7 +1354,7 @@
     </row>
     <row r="61" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B61" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>2</v>
@@ -1452,7 +1426,7 @@
     </row>
     <row r="66" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B66" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>2</v>
@@ -1486,7 +1460,7 @@
         <v>4</v>
       </c>
       <c r="D68" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
@@ -1514,7 +1488,7 @@
         <v>6</v>
       </c>
       <c r="D70" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -1522,24 +1496,223 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1</v>
+      </c>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="8"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B72" s="11"/>
+      <c r="C72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="8">
+        <v>1</v>
+      </c>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B73" s="11"/>
+      <c r="C73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="8">
+        <v>0</v>
+      </c>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B74" s="11"/>
+      <c r="C74" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="8">
+        <v>1</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+    </row>
+    <row r="75" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="12"/>
+      <c r="C75" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="5">
+        <v>1</v>
+      </c>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="8"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B77" s="11"/>
+      <c r="C77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B78" s="11"/>
+      <c r="C78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B79" s="11"/>
+      <c r="C79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+    </row>
+    <row r="80" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B80" s="12"/>
+      <c r="C80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="8"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B82" s="11"/>
+      <c r="C82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B83" s="11"/>
+      <c r="C83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B84" s="11"/>
+      <c r="C84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+    </row>
+    <row r="85" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B85" s="12"/>
+      <c r="C85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="18">
+    <mergeCell ref="B81:B85"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="D1:I2"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B16:B20"/>
     <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B21:B25"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B61:B65"/>
     <mergeCell ref="B66:B70"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="D1:I2"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="B76:B80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Third column of data
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A3F2C8-0BC8-470A-B34D-7DAE8AE32A0C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3EEA7B-E6CB-4981-A94C-ED826BF7B285}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,7 +603,9 @@
       <c r="E6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <v>78</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -619,7 +621,9 @@
       <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>76</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -635,7 +639,9 @@
       <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>33</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -651,7 +657,9 @@
       <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8">
+        <v>34</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -667,7 +675,9 @@
       <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>33</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -685,7 +695,9 @@
       <c r="E11" s="8">
         <v>5</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="8">
+        <v>10</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -701,7 +713,9 @@
       <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="8">
+        <v>3</v>
+      </c>
       <c r="G12" s="8"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -717,7 +731,9 @@
       <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8">
+        <v>3</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -733,7 +749,9 @@
       <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -749,7 +767,9 @@
       <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>3</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -767,7 +787,9 @@
       <c r="E16" s="7">
         <v>9</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>178</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -783,7 +805,9 @@
       <c r="E17" s="8">
         <v>6</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8">
+        <v>186</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -799,7 +823,9 @@
       <c r="E18" s="8">
         <v>2</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8">
+        <v>125</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -815,7 +841,9 @@
       <c r="E19" s="8">
         <v>1</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8">
+        <v>173</v>
+      </c>
       <c r="G19" s="8"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -831,7 +859,9 @@
       <c r="E20" s="5">
         <v>2</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="5">
+        <v>168</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -849,7 +879,9 @@
       <c r="E21" s="8">
         <v>2</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="8">
+        <v>10</v>
+      </c>
       <c r="G21" s="8"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -865,7 +897,9 @@
       <c r="E22" s="8">
         <v>2</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="8">
+        <v>2</v>
+      </c>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -881,7 +915,9 @@
       <c r="E23" s="8">
         <v>1</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8">
+        <v>2</v>
+      </c>
       <c r="G23" s="8"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -897,7 +933,9 @@
       <c r="E24" s="8">
         <v>0</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
       <c r="G24" s="8"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -913,7 +951,9 @@
       <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -931,7 +971,9 @@
       <c r="E26" s="7">
         <v>4</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>33</v>
+      </c>
       <c r="G26" s="7"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -947,7 +989,9 @@
       <c r="E27" s="8">
         <v>2</v>
       </c>
-      <c r="F27" s="8"/>
+      <c r="F27" s="8">
+        <v>17</v>
+      </c>
       <c r="G27" s="8"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -963,7 +1007,9 @@
       <c r="E28" s="8">
         <v>1</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8">
+        <v>21</v>
+      </c>
       <c r="G28" s="8"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -979,7 +1025,9 @@
       <c r="E29" s="8">
         <v>1</v>
       </c>
-      <c r="F29" s="8"/>
+      <c r="F29" s="8">
+        <v>20</v>
+      </c>
       <c r="G29" s="8"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -995,7 +1043,9 @@
       <c r="E30" s="5">
         <v>1</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5">
+        <v>22</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
@@ -1013,7 +1063,9 @@
       <c r="E31" s="7">
         <v>2</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7">
+        <v>11</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="9"/>
@@ -1029,7 +1081,9 @@
       <c r="E32" s="8">
         <v>1</v>
       </c>
-      <c r="F32" s="8"/>
+      <c r="F32" s="8">
+        <v>3</v>
+      </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1045,7 +1099,9 @@
       <c r="E33" s="8">
         <v>1</v>
       </c>
-      <c r="F33" s="8"/>
+      <c r="F33" s="8">
+        <v>2</v>
+      </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -1061,7 +1117,9 @@
       <c r="E34" s="8">
         <v>1</v>
       </c>
-      <c r="F34" s="8"/>
+      <c r="F34" s="8">
+        <v>2</v>
+      </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -1077,7 +1135,9 @@
       <c r="E35" s="5">
         <v>1</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="5">
+        <v>2</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1095,7 +1155,9 @@
       <c r="E36" s="7">
         <v>4</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7">
+        <v>13</v>
+      </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="8"/>
@@ -1111,7 +1173,9 @@
       <c r="E37" s="8">
         <v>6</v>
       </c>
-      <c r="F37" s="8"/>
+      <c r="F37" s="8">
+        <v>11</v>
+      </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -1127,7 +1191,9 @@
       <c r="E38" s="8">
         <v>2</v>
       </c>
-      <c r="F38" s="8"/>
+      <c r="F38" s="8">
+        <v>2</v>
+      </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
@@ -1143,7 +1209,9 @@
       <c r="E39" s="8">
         <v>1</v>
       </c>
-      <c r="F39" s="8"/>
+      <c r="F39" s="8">
+        <v>1</v>
+      </c>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
@@ -1159,7 +1227,9 @@
       <c r="E40" s="5">
         <v>1</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -1177,7 +1247,9 @@
       <c r="E41" s="7">
         <v>39</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="7">
+        <v>144</v>
+      </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="8"/>
@@ -1193,7 +1265,9 @@
       <c r="E42" s="8">
         <v>49</v>
       </c>
-      <c r="F42" s="8"/>
+      <c r="F42" s="8">
+        <v>3</v>
+      </c>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
@@ -1209,7 +1283,9 @@
       <c r="E43" s="8">
         <v>60</v>
       </c>
-      <c r="F43" s="8"/>
+      <c r="F43" s="8">
+        <v>3</v>
+      </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
@@ -1225,7 +1301,9 @@
       <c r="E44" s="8">
         <v>2</v>
       </c>
-      <c r="F44" s="8"/>
+      <c r="F44" s="8">
+        <v>3</v>
+      </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
@@ -1241,7 +1319,9 @@
       <c r="E45" s="5">
         <v>1</v>
       </c>
-      <c r="F45" s="5"/>
+      <c r="F45" s="5">
+        <v>3</v>
+      </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -1259,7 +1339,9 @@
       <c r="E46" s="7">
         <v>2</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7">
+        <v>7</v>
+      </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
@@ -1275,7 +1357,9 @@
       <c r="E47" s="8">
         <v>1</v>
       </c>
-      <c r="F47" s="8"/>
+      <c r="F47" s="8">
+        <v>2</v>
+      </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
@@ -1291,7 +1375,9 @@
       <c r="E48" s="8">
         <v>1</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F48" s="8">
+        <v>2</v>
+      </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
@@ -1307,7 +1393,9 @@
       <c r="E49" s="8">
         <v>1</v>
       </c>
-      <c r="F49" s="8"/>
+      <c r="F49" s="8">
+        <v>1</v>
+      </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
@@ -1323,7 +1411,9 @@
       <c r="E50" s="5">
         <v>1</v>
       </c>
-      <c r="F50" s="5"/>
+      <c r="F50" s="5">
+        <v>1</v>
+      </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -1341,7 +1431,9 @@
       <c r="E51" s="7">
         <v>2</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="7">
+        <v>3</v>
+      </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -1357,7 +1449,9 @@
       <c r="E52" s="8">
         <v>0</v>
       </c>
-      <c r="F52" s="8"/>
+      <c r="F52" s="8">
+        <v>2</v>
+      </c>
       <c r="G52" s="8"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -1373,7 +1467,9 @@
       <c r="E53" s="8">
         <v>4</v>
       </c>
-      <c r="F53" s="8"/>
+      <c r="F53" s="8">
+        <v>1</v>
+      </c>
       <c r="G53" s="8"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -1389,7 +1485,9 @@
       <c r="E54" s="8">
         <v>1</v>
       </c>
-      <c r="F54" s="8"/>
+      <c r="F54" s="8">
+        <v>2</v>
+      </c>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
@@ -1405,7 +1503,9 @@
       <c r="E55" s="5">
         <v>0</v>
       </c>
-      <c r="F55" s="5"/>
+      <c r="F55" s="5">
+        <v>2</v>
+      </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -1423,7 +1523,9 @@
       <c r="E56" s="7">
         <v>4</v>
       </c>
-      <c r="F56" s="7"/>
+      <c r="F56" s="7">
+        <v>3</v>
+      </c>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="8"/>
@@ -1439,7 +1541,9 @@
       <c r="E57" s="8">
         <v>1</v>
       </c>
-      <c r="F57" s="8"/>
+      <c r="F57" s="8">
+        <v>1</v>
+      </c>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
@@ -1455,7 +1559,9 @@
       <c r="E58" s="8">
         <v>0</v>
       </c>
-      <c r="F58" s="8"/>
+      <c r="F58" s="8">
+        <v>4</v>
+      </c>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
@@ -1471,7 +1577,9 @@
       <c r="E59" s="8">
         <v>0</v>
       </c>
-      <c r="F59" s="8"/>
+      <c r="F59" s="8">
+        <v>1</v>
+      </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
@@ -1487,7 +1595,9 @@
       <c r="E60" s="5">
         <v>0</v>
       </c>
-      <c r="F60" s="5"/>
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
@@ -1505,7 +1615,9 @@
       <c r="E61" s="7">
         <v>4</v>
       </c>
-      <c r="F61" s="7"/>
+      <c r="F61" s="7">
+        <v>1</v>
+      </c>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="8"/>
@@ -1521,7 +1633,9 @@
       <c r="E62" s="8">
         <v>0</v>
       </c>
-      <c r="F62" s="8"/>
+      <c r="F62" s="8">
+        <v>1</v>
+      </c>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
@@ -1537,7 +1651,9 @@
       <c r="E63" s="8">
         <v>1</v>
       </c>
-      <c r="F63" s="8"/>
+      <c r="F63" s="8">
+        <v>1</v>
+      </c>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
@@ -1553,7 +1669,9 @@
       <c r="E64" s="8">
         <v>1</v>
       </c>
-      <c r="F64" s="8"/>
+      <c r="F64" s="8">
+        <v>1</v>
+      </c>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
@@ -1569,7 +1687,9 @@
       <c r="E65" s="5">
         <v>0</v>
       </c>
-      <c r="F65" s="5"/>
+      <c r="F65" s="5">
+        <v>1</v>
+      </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -1587,7 +1707,9 @@
       <c r="E66" s="7">
         <v>2</v>
       </c>
-      <c r="F66" s="7"/>
+      <c r="F66" s="7">
+        <v>11</v>
+      </c>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="8"/>
@@ -1603,7 +1725,9 @@
       <c r="E67" s="8">
         <v>1</v>
       </c>
-      <c r="F67" s="8"/>
+      <c r="F67" s="8">
+        <v>2</v>
+      </c>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
@@ -1619,7 +1743,9 @@
       <c r="E68" s="8">
         <v>1</v>
       </c>
-      <c r="F68" s="8"/>
+      <c r="F68" s="8">
+        <v>1</v>
+      </c>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
@@ -1635,7 +1761,9 @@
       <c r="E69" s="8">
         <v>1</v>
       </c>
-      <c r="F69" s="8"/>
+      <c r="F69" s="8">
+        <v>2</v>
+      </c>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
@@ -1651,7 +1779,9 @@
       <c r="E70" s="5">
         <v>1</v>
       </c>
-      <c r="F70" s="5"/>
+      <c r="F70" s="5">
+        <v>2</v>
+      </c>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
@@ -1669,7 +1799,9 @@
       <c r="E71" s="7">
         <v>2</v>
       </c>
-      <c r="F71" s="7"/>
+      <c r="F71" s="7">
+        <v>6</v>
+      </c>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
       <c r="I71" s="8"/>
@@ -1685,7 +1817,9 @@
       <c r="E72" s="8">
         <v>1</v>
       </c>
-      <c r="F72" s="8"/>
+      <c r="F72" s="8">
+        <v>1</v>
+      </c>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
@@ -1701,7 +1835,9 @@
       <c r="E73" s="8">
         <v>1</v>
       </c>
-      <c r="F73" s="8"/>
+      <c r="F73" s="8">
+        <v>1</v>
+      </c>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
@@ -1717,7 +1853,9 @@
       <c r="E74" s="8">
         <v>1</v>
       </c>
-      <c r="F74" s="8"/>
+      <c r="F74" s="8">
+        <v>1</v>
+      </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
@@ -1733,7 +1871,9 @@
       <c r="E75" s="5">
         <v>1</v>
       </c>
-      <c r="F75" s="5"/>
+      <c r="F75" s="5">
+        <v>2</v>
+      </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -1751,7 +1891,9 @@
       <c r="E76" s="7">
         <v>4</v>
       </c>
-      <c r="F76" s="7"/>
+      <c r="F76" s="7">
+        <v>5</v>
+      </c>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
       <c r="I76" s="8"/>
@@ -1767,7 +1909,9 @@
       <c r="E77" s="8">
         <v>0</v>
       </c>
-      <c r="F77" s="8"/>
+      <c r="F77" s="8">
+        <v>2</v>
+      </c>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
@@ -1783,7 +1927,9 @@
       <c r="E78" s="8">
         <v>1</v>
       </c>
-      <c r="F78" s="8"/>
+      <c r="F78" s="8">
+        <v>2</v>
+      </c>
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
@@ -1799,7 +1945,9 @@
       <c r="E79" s="8">
         <v>1</v>
       </c>
-      <c r="F79" s="8"/>
+      <c r="F79" s="8">
+        <v>8</v>
+      </c>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
@@ -1815,7 +1963,9 @@
       <c r="E80" s="5">
         <v>0</v>
       </c>
-      <c r="F80" s="5"/>
+      <c r="F80" s="5">
+        <v>10</v>
+      </c>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
@@ -1833,7 +1983,9 @@
       <c r="E81" s="7">
         <v>4</v>
       </c>
-      <c r="F81" s="7"/>
+      <c r="F81" s="7">
+        <v>3</v>
+      </c>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="8"/>
@@ -1849,7 +2001,9 @@
       <c r="E82" s="8">
         <v>0</v>
       </c>
-      <c r="F82" s="8"/>
+      <c r="F82" s="8">
+        <v>2</v>
+      </c>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
@@ -1865,7 +2019,9 @@
       <c r="E83" s="8">
         <v>1</v>
       </c>
-      <c r="F83" s="8"/>
+      <c r="F83" s="8">
+        <v>1</v>
+      </c>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
@@ -1881,7 +2037,9 @@
       <c r="E84" s="8">
         <v>1</v>
       </c>
-      <c r="F84" s="8"/>
+      <c r="F84" s="8">
+        <v>1</v>
+      </c>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
@@ -1897,7 +2055,9 @@
       <c r="E85" s="5">
         <v>1</v>
       </c>
-      <c r="F85" s="5"/>
+      <c r="F85" s="5">
+        <v>1</v>
+      </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>

</xml_diff>

<commit_message>
Fourth column of data
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3EEA7B-E6CB-4981-A94C-ED826BF7B285}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ED1CC1-90D6-4E69-95DD-B454777C6585}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,7 +606,9 @@
       <c r="F6" s="3">
         <v>78</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8">
+        <v>5775</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
@@ -624,7 +626,9 @@
       <c r="F7" s="3">
         <v>76</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8">
+        <v>5828</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
@@ -642,7 +646,9 @@
       <c r="F8" s="8">
         <v>33</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8">
+        <v>3250</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
@@ -660,7 +666,9 @@
       <c r="F9" s="8">
         <v>34</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8">
+        <v>3214</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
@@ -678,7 +686,9 @@
       <c r="F10" s="5">
         <v>33</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5">
+        <v>3199</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
@@ -698,7 +708,9 @@
       <c r="F11" s="8">
         <v>10</v>
       </c>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8">
+        <v>22</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
@@ -716,7 +728,9 @@
       <c r="F12" s="8">
         <v>3</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8">
+        <v>22</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
@@ -734,7 +748,9 @@
       <c r="F13" s="8">
         <v>3</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8">
+        <v>19</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
@@ -752,7 +768,9 @@
       <c r="F14" s="8">
         <v>3</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8">
+        <v>16</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
@@ -770,7 +788,9 @@
       <c r="F15" s="5">
         <v>3</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="5">
+        <v>17</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
@@ -790,7 +810,9 @@
       <c r="F16" s="7">
         <v>178</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7">
+        <v>24234</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
@@ -808,7 +830,9 @@
       <c r="F17" s="8">
         <v>186</v>
       </c>
-      <c r="G17" s="8"/>
+      <c r="G17" s="8">
+        <v>24313</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
@@ -826,7 +850,9 @@
       <c r="F18" s="8">
         <v>125</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8">
+        <v>12675</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
@@ -844,7 +870,9 @@
       <c r="F19" s="8">
         <v>173</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="8">
+        <v>12459</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
@@ -862,7 +890,9 @@
       <c r="F20" s="5">
         <v>168</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="5">
+        <v>12523</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
@@ -882,7 +912,9 @@
       <c r="F21" s="8">
         <v>10</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="8">
+        <v>20</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
@@ -900,7 +932,9 @@
       <c r="F22" s="8">
         <v>2</v>
       </c>
-      <c r="G22" s="8"/>
+      <c r="G22" s="8">
+        <v>22</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
@@ -918,7 +952,9 @@
       <c r="F23" s="8">
         <v>2</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="G23" s="8">
+        <v>14</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
@@ -936,7 +972,9 @@
       <c r="F24" s="8">
         <v>1</v>
       </c>
-      <c r="G24" s="8"/>
+      <c r="G24" s="8">
+        <v>12</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
@@ -954,7 +992,9 @@
       <c r="F25" s="5">
         <v>1</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="5">
+        <v>12</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
@@ -974,7 +1014,9 @@
       <c r="F26" s="7">
         <v>33</v>
       </c>
-      <c r="G26" s="7"/>
+      <c r="G26" s="7">
+        <v>1280</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
@@ -992,7 +1034,9 @@
       <c r="F27" s="8">
         <v>17</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="8">
+        <v>1206</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
@@ -1010,7 +1054,9 @@
       <c r="F28" s="8">
         <v>21</v>
       </c>
-      <c r="G28" s="8"/>
+      <c r="G28" s="8">
+        <v>2125</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
@@ -1028,7 +1074,9 @@
       <c r="F29" s="8">
         <v>20</v>
       </c>
-      <c r="G29" s="8"/>
+      <c r="G29" s="8">
+        <v>2371</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
@@ -1046,7 +1094,9 @@
       <c r="F30" s="5">
         <v>22</v>
       </c>
-      <c r="G30" s="5"/>
+      <c r="G30" s="5">
+        <v>2461</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
@@ -1066,7 +1116,9 @@
       <c r="F31" s="7">
         <v>11</v>
       </c>
-      <c r="G31" s="7"/>
+      <c r="G31" s="7">
+        <v>28</v>
+      </c>
       <c r="H31" s="7"/>
       <c r="I31" s="9"/>
     </row>
@@ -1084,7 +1136,9 @@
       <c r="F32" s="8">
         <v>3</v>
       </c>
-      <c r="G32" s="8"/>
+      <c r="G32" s="8">
+        <v>21</v>
+      </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
     </row>
@@ -1102,7 +1156,9 @@
       <c r="F33" s="8">
         <v>2</v>
       </c>
-      <c r="G33" s="8"/>
+      <c r="G33" s="8">
+        <v>19</v>
+      </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
     </row>
@@ -1120,7 +1176,9 @@
       <c r="F34" s="8">
         <v>2</v>
       </c>
-      <c r="G34" s="8"/>
+      <c r="G34" s="8">
+        <v>17</v>
+      </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
     </row>
@@ -1138,7 +1196,9 @@
       <c r="F35" s="5">
         <v>2</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="G35" s="5">
+        <v>18</v>
+      </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
     </row>
@@ -1158,7 +1218,9 @@
       <c r="F36" s="7">
         <v>13</v>
       </c>
-      <c r="G36" s="7"/>
+      <c r="G36" s="7">
+        <v>22</v>
+      </c>
       <c r="H36" s="7"/>
       <c r="I36" s="8"/>
     </row>
@@ -1176,7 +1238,9 @@
       <c r="F37" s="8">
         <v>11</v>
       </c>
-      <c r="G37" s="8"/>
+      <c r="G37" s="8">
+        <v>15</v>
+      </c>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
     </row>
@@ -1194,7 +1258,9 @@
       <c r="F38" s="8">
         <v>2</v>
       </c>
-      <c r="G38" s="8"/>
+      <c r="G38" s="8">
+        <v>10</v>
+      </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
     </row>
@@ -1212,7 +1278,9 @@
       <c r="F39" s="8">
         <v>1</v>
       </c>
-      <c r="G39" s="8"/>
+      <c r="G39" s="8">
+        <v>10</v>
+      </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
     </row>
@@ -1230,7 +1298,9 @@
       <c r="F40" s="5">
         <v>1</v>
       </c>
-      <c r="G40" s="5"/>
+      <c r="G40" s="5">
+        <v>11</v>
+      </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
@@ -1250,7 +1320,9 @@
       <c r="F41" s="7">
         <v>144</v>
       </c>
-      <c r="G41" s="7"/>
+      <c r="G41" s="7">
+        <v>234</v>
+      </c>
       <c r="H41" s="7"/>
       <c r="I41" s="8"/>
     </row>
@@ -1268,7 +1340,9 @@
       <c r="F42" s="8">
         <v>3</v>
       </c>
-      <c r="G42" s="8"/>
+      <c r="G42" s="8">
+        <v>34</v>
+      </c>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
     </row>
@@ -1286,7 +1360,9 @@
       <c r="F43" s="8">
         <v>3</v>
       </c>
-      <c r="G43" s="8"/>
+      <c r="G43" s="8">
+        <v>37</v>
+      </c>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
     </row>
@@ -1304,7 +1380,9 @@
       <c r="F44" s="8">
         <v>3</v>
       </c>
-      <c r="G44" s="8"/>
+      <c r="G44" s="8">
+        <v>40</v>
+      </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
     </row>
@@ -1322,7 +1400,9 @@
       <c r="F45" s="5">
         <v>3</v>
       </c>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5">
+        <v>41</v>
+      </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
@@ -1342,7 +1422,9 @@
       <c r="F46" s="7">
         <v>7</v>
       </c>
-      <c r="G46" s="7"/>
+      <c r="G46" s="7">
+        <v>41</v>
+      </c>
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
     </row>
@@ -1360,7 +1442,9 @@
       <c r="F47" s="8">
         <v>2</v>
       </c>
-      <c r="G47" s="8"/>
+      <c r="G47" s="8">
+        <v>18</v>
+      </c>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
     </row>
@@ -1378,7 +1462,9 @@
       <c r="F48" s="8">
         <v>2</v>
       </c>
-      <c r="G48" s="8"/>
+      <c r="G48" s="8">
+        <v>16</v>
+      </c>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
     </row>
@@ -1396,7 +1482,9 @@
       <c r="F49" s="8">
         <v>1</v>
       </c>
-      <c r="G49" s="8"/>
+      <c r="G49" s="8">
+        <v>10</v>
+      </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
     </row>
@@ -1414,7 +1502,9 @@
       <c r="F50" s="5">
         <v>1</v>
       </c>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5">
+        <v>9</v>
+      </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
     </row>
@@ -1434,7 +1524,9 @@
       <c r="F51" s="7">
         <v>3</v>
       </c>
-      <c r="G51" s="7"/>
+      <c r="G51" s="7">
+        <v>6</v>
+      </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
     </row>
@@ -1452,7 +1544,9 @@
       <c r="F52" s="8">
         <v>2</v>
       </c>
-      <c r="G52" s="8"/>
+      <c r="G52" s="8">
+        <v>2</v>
+      </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
@@ -1470,7 +1564,9 @@
       <c r="F53" s="8">
         <v>1</v>
       </c>
-      <c r="G53" s="8"/>
+      <c r="G53" s="8">
+        <v>1</v>
+      </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
@@ -1488,7 +1584,9 @@
       <c r="F54" s="8">
         <v>2</v>
       </c>
-      <c r="G54" s="8"/>
+      <c r="G54" s="8">
+        <v>0</v>
+      </c>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
     </row>
@@ -1506,7 +1604,9 @@
       <c r="F55" s="5">
         <v>2</v>
       </c>
-      <c r="G55" s="5"/>
+      <c r="G55" s="5">
+        <v>1</v>
+      </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
     </row>
@@ -1526,7 +1626,9 @@
       <c r="F56" s="7">
         <v>3</v>
       </c>
-      <c r="G56" s="7"/>
+      <c r="G56" s="7">
+        <v>3</v>
+      </c>
       <c r="H56" s="7"/>
       <c r="I56" s="8"/>
     </row>
@@ -1544,7 +1646,9 @@
       <c r="F57" s="8">
         <v>1</v>
       </c>
-      <c r="G57" s="8"/>
+      <c r="G57" s="8">
+        <v>2</v>
+      </c>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
     </row>
@@ -1562,7 +1666,9 @@
       <c r="F58" s="8">
         <v>4</v>
       </c>
-      <c r="G58" s="8"/>
+      <c r="G58" s="8">
+        <v>1</v>
+      </c>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
     </row>
@@ -1580,7 +1686,9 @@
       <c r="F59" s="8">
         <v>1</v>
       </c>
-      <c r="G59" s="8"/>
+      <c r="G59" s="8">
+        <v>1</v>
+      </c>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
     </row>
@@ -1598,7 +1706,9 @@
       <c r="F60" s="5">
         <v>0</v>
       </c>
-      <c r="G60" s="5"/>
+      <c r="G60" s="5">
+        <v>1</v>
+      </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
     </row>
@@ -1618,7 +1728,9 @@
       <c r="F61" s="7">
         <v>1</v>
       </c>
-      <c r="G61" s="7"/>
+      <c r="G61" s="7">
+        <v>3</v>
+      </c>
       <c r="H61" s="7"/>
       <c r="I61" s="8"/>
     </row>
@@ -1636,7 +1748,9 @@
       <c r="F62" s="8">
         <v>1</v>
       </c>
-      <c r="G62" s="8"/>
+      <c r="G62" s="8">
+        <v>0</v>
+      </c>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
     </row>
@@ -1654,7 +1768,9 @@
       <c r="F63" s="8">
         <v>1</v>
       </c>
-      <c r="G63" s="8"/>
+      <c r="G63" s="8">
+        <v>1</v>
+      </c>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
     </row>
@@ -1672,7 +1788,9 @@
       <c r="F64" s="8">
         <v>1</v>
       </c>
-      <c r="G64" s="8"/>
+      <c r="G64" s="8">
+        <v>1</v>
+      </c>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
     </row>
@@ -1690,7 +1808,9 @@
       <c r="F65" s="5">
         <v>1</v>
       </c>
-      <c r="G65" s="5"/>
+      <c r="G65" s="5">
+        <v>0</v>
+      </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
     </row>
@@ -1710,7 +1830,9 @@
       <c r="F66" s="7">
         <v>11</v>
       </c>
-      <c r="G66" s="7"/>
+      <c r="G66" s="7">
+        <v>20</v>
+      </c>
       <c r="H66" s="7"/>
       <c r="I66" s="8"/>
     </row>
@@ -1728,7 +1850,9 @@
       <c r="F67" s="8">
         <v>2</v>
       </c>
-      <c r="G67" s="8"/>
+      <c r="G67" s="8">
+        <v>13</v>
+      </c>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
     </row>
@@ -1746,7 +1870,9 @@
       <c r="F68" s="8">
         <v>1</v>
       </c>
-      <c r="G68" s="8"/>
+      <c r="G68" s="8">
+        <v>11</v>
+      </c>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
     </row>
@@ -1764,7 +1890,9 @@
       <c r="F69" s="8">
         <v>2</v>
       </c>
-      <c r="G69" s="8"/>
+      <c r="G69" s="8">
+        <v>10</v>
+      </c>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
     </row>
@@ -1782,7 +1910,9 @@
       <c r="F70" s="5">
         <v>2</v>
       </c>
-      <c r="G70" s="5"/>
+      <c r="G70" s="5">
+        <v>10</v>
+      </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
     </row>
@@ -1802,7 +1932,9 @@
       <c r="F71" s="7">
         <v>6</v>
       </c>
-      <c r="G71" s="7"/>
+      <c r="G71" s="7">
+        <v>8</v>
+      </c>
       <c r="H71" s="7"/>
       <c r="I71" s="8"/>
     </row>
@@ -1820,7 +1952,9 @@
       <c r="F72" s="8">
         <v>1</v>
       </c>
-      <c r="G72" s="8"/>
+      <c r="G72" s="8">
+        <v>8</v>
+      </c>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
     </row>
@@ -1838,7 +1972,9 @@
       <c r="F73" s="8">
         <v>1</v>
       </c>
-      <c r="G73" s="8"/>
+      <c r="G73" s="8">
+        <v>2</v>
+      </c>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
     </row>
@@ -1856,7 +1992,9 @@
       <c r="F74" s="8">
         <v>1</v>
       </c>
-      <c r="G74" s="8"/>
+      <c r="G74" s="8">
+        <v>2</v>
+      </c>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
     </row>
@@ -1874,7 +2012,9 @@
       <c r="F75" s="5">
         <v>2</v>
       </c>
-      <c r="G75" s="5"/>
+      <c r="G75" s="5">
+        <v>2</v>
+      </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
@@ -1894,7 +2034,9 @@
       <c r="F76" s="7">
         <v>5</v>
       </c>
-      <c r="G76" s="7"/>
+      <c r="G76" s="7">
+        <v>6</v>
+      </c>
       <c r="H76" s="7"/>
       <c r="I76" s="8"/>
     </row>
@@ -1912,7 +2054,9 @@
       <c r="F77" s="8">
         <v>2</v>
       </c>
-      <c r="G77" s="8"/>
+      <c r="G77" s="8">
+        <v>6</v>
+      </c>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
     </row>
@@ -1930,7 +2074,9 @@
       <c r="F78" s="8">
         <v>2</v>
       </c>
-      <c r="G78" s="8"/>
+      <c r="G78" s="8">
+        <v>2</v>
+      </c>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
     </row>
@@ -1948,7 +2094,9 @@
       <c r="F79" s="8">
         <v>8</v>
       </c>
-      <c r="G79" s="8"/>
+      <c r="G79" s="8">
+        <v>1</v>
+      </c>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
     </row>
@@ -1966,7 +2114,9 @@
       <c r="F80" s="5">
         <v>10</v>
       </c>
-      <c r="G80" s="5"/>
+      <c r="G80" s="5">
+        <v>2</v>
+      </c>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
     </row>
@@ -1986,7 +2136,9 @@
       <c r="F81" s="7">
         <v>3</v>
       </c>
-      <c r="G81" s="7"/>
+      <c r="G81" s="7">
+        <v>6</v>
+      </c>
       <c r="H81" s="7"/>
       <c r="I81" s="8"/>
     </row>
@@ -2004,7 +2156,9 @@
       <c r="F82" s="8">
         <v>2</v>
       </c>
-      <c r="G82" s="8"/>
+      <c r="G82" s="8">
+        <v>4</v>
+      </c>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
     </row>
@@ -2022,7 +2176,9 @@
       <c r="F83" s="8">
         <v>1</v>
       </c>
-      <c r="G83" s="8"/>
+      <c r="G83" s="8">
+        <v>2</v>
+      </c>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
     </row>
@@ -2040,7 +2196,9 @@
       <c r="F84" s="8">
         <v>1</v>
       </c>
-      <c r="G84" s="8"/>
+      <c r="G84" s="8">
+        <v>2</v>
+      </c>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
     </row>
@@ -2058,7 +2216,9 @@
       <c r="F85" s="5">
         <v>1</v>
       </c>
-      <c r="G85" s="5"/>
+      <c r="G85" s="5">
+        <v>2</v>
+      </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
     </row>

</xml_diff>

<commit_message>
Last column of data
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABA43F7-66E1-4D77-9CC7-5B28613E7E78}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F4B1FC-6347-499C-B7D8-68145A0B1139}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="24">
   <si>
     <t>Input Size</t>
   </si>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,7 +615,9 @@
       <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="11"/>
@@ -637,7 +639,9 @@
       <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="11"/>
@@ -659,7 +663,9 @@
       <c r="H8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="11"/>
@@ -681,7 +687,9 @@
       <c r="H9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="12"/>
@@ -703,7 +711,9 @@
       <c r="H10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
@@ -727,7 +737,9 @@
       <c r="H11" s="8">
         <v>221</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="8">
+        <v>3521</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
@@ -749,7 +761,9 @@
       <c r="H12" s="8">
         <v>216</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="8">
+        <v>3527</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
@@ -771,7 +785,9 @@
       <c r="H13" s="8">
         <v>221</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="8">
+        <v>3546</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
@@ -793,7 +809,9 @@
       <c r="H14" s="8">
         <v>223</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="8">
+        <v>3585</v>
+      </c>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="12"/>
@@ -815,7 +833,9 @@
       <c r="H15" s="5">
         <v>221</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5">
+        <v>3555</v>
+      </c>
     </row>
     <row r="16" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
@@ -839,7 +859,9 @@
       <c r="H16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="11"/>
@@ -861,7 +883,9 @@
       <c r="H17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="11"/>
@@ -883,7 +907,9 @@
       <c r="H18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="11"/>
@@ -905,7 +931,9 @@
       <c r="H19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="12"/>
@@ -927,7 +955,9 @@
       <c r="H20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B21" s="11" t="s">
@@ -951,7 +981,9 @@
       <c r="H21" s="8">
         <v>218</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="8">
+        <v>2597</v>
+      </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
@@ -973,7 +1005,9 @@
       <c r="H22" s="8">
         <v>218</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="8">
+        <v>2607</v>
+      </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="11"/>
@@ -995,7 +1029,9 @@
       <c r="H23" s="8">
         <v>139</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="8">
+        <v>1666</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
@@ -1017,7 +1053,9 @@
       <c r="H24" s="8">
         <v>140</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="8">
+        <v>1695</v>
+      </c>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="12"/>
@@ -1039,7 +1077,9 @@
       <c r="H25" s="5">
         <v>141</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5">
+        <v>1676</v>
+      </c>
     </row>
     <row r="26" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B26" s="10" t="s">
@@ -1063,7 +1103,9 @@
       <c r="H26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="11"/>
@@ -1085,7 +1127,9 @@
       <c r="H27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="11"/>
@@ -1107,7 +1151,9 @@
       <c r="H28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="11"/>
@@ -1129,7 +1175,9 @@
       <c r="H29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="3"/>
+      <c r="I29" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="12"/>
@@ -1151,7 +1199,9 @@
       <c r="H30" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I30" s="5"/>
+      <c r="I30" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B31" s="10" t="s">
@@ -1175,7 +1225,9 @@
       <c r="H31" s="7">
         <v>235</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="9">
+        <v>3373</v>
+      </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="11"/>
@@ -1197,7 +1249,9 @@
       <c r="H32" s="8">
         <v>229</v>
       </c>
-      <c r="I32" s="8"/>
+      <c r="I32" s="8">
+        <v>3296</v>
+      </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="11"/>
@@ -1219,7 +1273,9 @@
       <c r="H33" s="8">
         <v>239</v>
       </c>
-      <c r="I33" s="8"/>
+      <c r="I33" s="8">
+        <v>3280</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="11"/>
@@ -1241,7 +1297,9 @@
       <c r="H34" s="8">
         <v>230</v>
       </c>
-      <c r="I34" s="8"/>
+      <c r="I34" s="8">
+        <v>3287</v>
+      </c>
     </row>
     <row r="35" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="12"/>
@@ -1263,7 +1321,9 @@
       <c r="H35" s="5">
         <v>228</v>
       </c>
-      <c r="I35" s="5"/>
+      <c r="I35" s="5">
+        <v>3402</v>
+      </c>
     </row>
     <row r="36" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="10" t="s">
@@ -1287,7 +1347,9 @@
       <c r="H36" s="7">
         <v>127</v>
       </c>
-      <c r="I36" s="8"/>
+      <c r="I36" s="8">
+        <v>1441</v>
+      </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="11"/>
@@ -1309,7 +1371,9 @@
       <c r="H37" s="8">
         <v>119</v>
       </c>
-      <c r="I37" s="8"/>
+      <c r="I37" s="8">
+        <v>1332</v>
+      </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="11"/>
@@ -1331,7 +1395,9 @@
       <c r="H38" s="8">
         <v>122</v>
       </c>
-      <c r="I38" s="8"/>
+      <c r="I38" s="8">
+        <v>1322</v>
+      </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="11"/>
@@ -1353,7 +1419,9 @@
       <c r="H39" s="8">
         <v>120</v>
       </c>
-      <c r="I39" s="8"/>
+      <c r="I39" s="8">
+        <v>1350</v>
+      </c>
     </row>
     <row r="40" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="12"/>
@@ -1375,7 +1443,9 @@
       <c r="H40" s="5">
         <v>126</v>
       </c>
-      <c r="I40" s="5"/>
+      <c r="I40" s="5">
+        <v>1319</v>
+      </c>
     </row>
     <row r="41" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
@@ -1399,7 +1469,9 @@
       <c r="H41" s="7">
         <v>497</v>
       </c>
-      <c r="I41" s="8"/>
+      <c r="I41" s="8">
+        <v>3533</v>
+      </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="11"/>
@@ -1421,7 +1493,9 @@
       <c r="H42" s="8">
         <v>291</v>
       </c>
-      <c r="I42" s="8"/>
+      <c r="I42" s="8">
+        <v>3242</v>
+      </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" s="11"/>
@@ -1443,7 +1517,9 @@
       <c r="H43" s="8">
         <v>337</v>
       </c>
-      <c r="I43" s="8"/>
+      <c r="I43" s="8">
+        <v>3245</v>
+      </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44" s="11"/>
@@ -1465,7 +1541,9 @@
       <c r="H44" s="8">
         <v>299</v>
       </c>
-      <c r="I44" s="8"/>
+      <c r="I44" s="8">
+        <v>3263</v>
+      </c>
     </row>
     <row r="45" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="12"/>
@@ -1487,7 +1565,9 @@
       <c r="H45" s="5">
         <v>296</v>
       </c>
-      <c r="I45" s="5"/>
+      <c r="I45" s="5">
+        <v>3259</v>
+      </c>
     </row>
     <row r="46" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B46" s="10" t="s">
@@ -1511,7 +1591,9 @@
       <c r="H46" s="7">
         <v>282</v>
       </c>
-      <c r="I46" s="8"/>
+      <c r="I46" s="8">
+        <v>1232</v>
+      </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="11"/>
@@ -1533,7 +1615,9 @@
       <c r="H47" s="8">
         <v>106</v>
       </c>
-      <c r="I47" s="8"/>
+      <c r="I47" s="8">
+        <v>1165</v>
+      </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" s="11"/>
@@ -1555,7 +1639,9 @@
       <c r="H48" s="8">
         <v>105</v>
       </c>
-      <c r="I48" s="8"/>
+      <c r="I48" s="8">
+        <v>1178</v>
+      </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="11"/>
@@ -1577,7 +1663,9 @@
       <c r="H49" s="8">
         <v>107</v>
       </c>
-      <c r="I49" s="8"/>
+      <c r="I49" s="8">
+        <v>1176</v>
+      </c>
     </row>
     <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="12"/>
@@ -1599,7 +1687,9 @@
       <c r="H50" s="5">
         <v>103</v>
       </c>
-      <c r="I50" s="5"/>
+      <c r="I50" s="5">
+        <v>1185</v>
+      </c>
     </row>
     <row r="51" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B51" s="10" t="s">
@@ -1623,7 +1713,9 @@
       <c r="H51" s="7">
         <v>17</v>
       </c>
-      <c r="I51" s="7"/>
+      <c r="I51" s="7">
+        <v>65</v>
+      </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="11"/>
@@ -1645,7 +1737,9 @@
       <c r="H52" s="8">
         <v>11</v>
       </c>
-      <c r="I52" s="3"/>
+      <c r="I52" s="8">
+        <v>23</v>
+      </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="11"/>
@@ -1667,7 +1761,9 @@
       <c r="H53" s="8">
         <v>3</v>
       </c>
-      <c r="I53" s="3"/>
+      <c r="I53" s="8">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="11"/>
@@ -1689,7 +1785,9 @@
       <c r="H54" s="8">
         <v>2</v>
       </c>
-      <c r="I54" s="8"/>
+      <c r="I54" s="8">
+        <v>18</v>
+      </c>
     </row>
     <row r="55" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="12"/>
@@ -1711,7 +1809,9 @@
       <c r="H55" s="5">
         <v>2</v>
       </c>
-      <c r="I55" s="5"/>
+      <c r="I55" s="5">
+        <v>17</v>
+      </c>
     </row>
     <row r="56" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B56" s="10" t="s">
@@ -1735,7 +1835,9 @@
       <c r="H56" s="7">
         <v>9</v>
       </c>
-      <c r="I56" s="8"/>
+      <c r="I56" s="8">
+        <v>26</v>
+      </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="11"/>
@@ -1757,7 +1859,9 @@
       <c r="H57" s="8">
         <v>2</v>
       </c>
-      <c r="I57" s="8"/>
+      <c r="I57" s="8">
+        <v>16</v>
+      </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="11"/>
@@ -1779,7 +1883,9 @@
       <c r="H58" s="8">
         <v>2</v>
       </c>
-      <c r="I58" s="8"/>
+      <c r="I58" s="8">
+        <v>14</v>
+      </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="11"/>
@@ -1801,7 +1907,9 @@
       <c r="H59" s="8">
         <v>1</v>
       </c>
-      <c r="I59" s="8"/>
+      <c r="I59" s="8">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B60" s="12"/>
@@ -1823,7 +1931,9 @@
       <c r="H60" s="5">
         <v>2</v>
       </c>
-      <c r="I60" s="5"/>
+      <c r="I60" s="5">
+        <v>13</v>
+      </c>
     </row>
     <row r="61" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B61" s="10" t="s">
@@ -1847,7 +1957,9 @@
       <c r="H61" s="7">
         <v>6</v>
       </c>
-      <c r="I61" s="8"/>
+      <c r="I61" s="8">
+        <v>16</v>
+      </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="11"/>
@@ -1869,7 +1981,9 @@
       <c r="H62" s="8">
         <v>2</v>
       </c>
-      <c r="I62" s="8"/>
+      <c r="I62" s="8">
+        <v>11</v>
+      </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="11"/>
@@ -1891,7 +2005,9 @@
       <c r="H63" s="8">
         <v>2</v>
       </c>
-      <c r="I63" s="8"/>
+      <c r="I63" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" s="11"/>
@@ -1913,7 +2029,9 @@
       <c r="H64" s="8">
         <v>1</v>
       </c>
-      <c r="I64" s="8"/>
+      <c r="I64" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B65" s="12"/>
@@ -1935,7 +2053,9 @@
       <c r="H65" s="5">
         <v>1</v>
       </c>
-      <c r="I65" s="5"/>
+      <c r="I65" s="5">
+        <v>9</v>
+      </c>
     </row>
     <row r="66" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B66" s="10" t="s">
@@ -1959,7 +2079,9 @@
       <c r="H66" s="7">
         <v>167</v>
       </c>
-      <c r="I66" s="8"/>
+      <c r="I66" s="8">
+        <v>1387</v>
+      </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" s="11"/>
@@ -1981,7 +2103,9 @@
       <c r="H67" s="8">
         <v>132</v>
       </c>
-      <c r="I67" s="8"/>
+      <c r="I67" s="8">
+        <v>1183</v>
+      </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" s="11"/>
@@ -2003,7 +2127,9 @@
       <c r="H68" s="8">
         <v>141</v>
       </c>
-      <c r="I68" s="8"/>
+      <c r="I68" s="8">
+        <v>1344</v>
+      </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69" s="11"/>
@@ -2025,7 +2151,9 @@
       <c r="H69" s="8">
         <v>134</v>
       </c>
-      <c r="I69" s="8"/>
+      <c r="I69" s="8">
+        <v>1384</v>
+      </c>
     </row>
     <row r="70" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B70" s="12"/>
@@ -2047,7 +2175,9 @@
       <c r="H70" s="5">
         <v>139</v>
       </c>
-      <c r="I70" s="5"/>
+      <c r="I70" s="5">
+        <v>1373</v>
+      </c>
     </row>
     <row r="71" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B71" s="10" t="s">
@@ -2071,7 +2201,9 @@
       <c r="H71" s="7">
         <v>35</v>
       </c>
-      <c r="I71" s="8"/>
+      <c r="I71" s="8">
+        <v>319</v>
+      </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B72" s="11"/>
@@ -2093,7 +2225,9 @@
       <c r="H72" s="8">
         <v>33</v>
       </c>
-      <c r="I72" s="8"/>
+      <c r="I72" s="8">
+        <v>310</v>
+      </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" s="11"/>
@@ -2115,7 +2249,9 @@
       <c r="H73" s="8">
         <v>18</v>
       </c>
-      <c r="I73" s="8"/>
+      <c r="I73" s="8">
+        <v>350</v>
+      </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" s="11"/>
@@ -2137,7 +2273,9 @@
       <c r="H74" s="8">
         <v>18</v>
       </c>
-      <c r="I74" s="8"/>
+      <c r="I74" s="8">
+        <v>306</v>
+      </c>
     </row>
     <row r="75" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B75" s="12"/>
@@ -2159,7 +2297,9 @@
       <c r="H75" s="5">
         <v>29</v>
       </c>
-      <c r="I75" s="5"/>
+      <c r="I75" s="5">
+        <v>303</v>
+      </c>
     </row>
     <row r="76" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B76" s="10" t="s">
@@ -2183,7 +2323,9 @@
       <c r="H76" s="7">
         <v>75</v>
       </c>
-      <c r="I76" s="8"/>
+      <c r="I76" s="8">
+        <v>1438</v>
+      </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" s="11"/>
@@ -2205,7 +2347,9 @@
       <c r="H77" s="8">
         <v>99</v>
       </c>
-      <c r="I77" s="8"/>
+      <c r="I77" s="8">
+        <v>1419</v>
+      </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" s="11"/>
@@ -2227,7 +2371,9 @@
       <c r="H78" s="8">
         <v>90</v>
       </c>
-      <c r="I78" s="8"/>
+      <c r="I78" s="8">
+        <v>1445</v>
+      </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79" s="11"/>
@@ -2249,7 +2395,9 @@
       <c r="H79" s="8">
         <v>57</v>
       </c>
-      <c r="I79" s="8"/>
+      <c r="I79" s="8">
+        <v>1416</v>
+      </c>
     </row>
     <row r="80" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B80" s="12"/>
@@ -2271,7 +2419,9 @@
       <c r="H80" s="5">
         <v>52</v>
       </c>
-      <c r="I80" s="5"/>
+      <c r="I80" s="5">
+        <v>1415</v>
+      </c>
     </row>
     <row r="81" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B81" s="10" t="s">
@@ -2295,7 +2445,9 @@
       <c r="H81" s="7">
         <v>40</v>
       </c>
-      <c r="I81" s="8"/>
+      <c r="I81" s="8">
+        <v>322</v>
+      </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" s="11"/>
@@ -2317,7 +2469,9 @@
       <c r="H82" s="8">
         <v>42</v>
       </c>
-      <c r="I82" s="8"/>
+      <c r="I82" s="8">
+        <v>359</v>
+      </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B83" s="11"/>
@@ -2339,7 +2493,9 @@
       <c r="H83" s="8">
         <v>23</v>
       </c>
-      <c r="I83" s="8"/>
+      <c r="I83" s="8">
+        <v>300</v>
+      </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" s="11"/>
@@ -2361,7 +2517,9 @@
       <c r="H84" s="8">
         <v>21</v>
       </c>
-      <c r="I84" s="8"/>
+      <c r="I84" s="8">
+        <v>301</v>
+      </c>
     </row>
     <row r="85" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B85" s="12"/>
@@ -2383,7 +2541,9 @@
       <c r="H85" s="5">
         <v>22</v>
       </c>
-      <c r="I85" s="5"/>
+      <c r="I85" s="5">
+        <v>307</v>
+      </c>
     </row>
     <row r="86" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="D86" s="8"/>

</xml_diff>

<commit_message>
Move charts and data around
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A7A0F0-B841-415B-99E6-B48445EA59EF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACD9A8F-D275-4F92-A22B-825CC485E123}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -324,7 +324,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$7</c:f>
+              <c:f>Sheet1!$B$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -347,7 +347,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -374,7 +374,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$H$7</c:f>
+              <c:f>Sheet1!$C$35:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -411,7 +411,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$8</c:f>
+              <c:f>Sheet1!$B$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -434,7 +434,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -461,7 +461,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$H$8</c:f>
+              <c:f>Sheet1!$C$36:$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -498,7 +498,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$9</c:f>
+              <c:f>Sheet1!$B$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -521,7 +521,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -548,7 +548,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$H$9</c:f>
+              <c:f>Sheet1!$C$37:$H$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -585,7 +585,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$10</c:f>
+              <c:f>Sheet1!$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -608,7 +608,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -635,7 +635,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$H$10</c:f>
+              <c:f>Sheet1!$C$38:$H$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -672,7 +672,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$11</c:f>
+              <c:f>Sheet1!$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -695,7 +695,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -722,7 +722,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$11:$H$11</c:f>
+              <c:f>Sheet1!$C$39:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -759,7 +759,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$12</c:f>
+              <c:f>Sheet1!$B$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -782,7 +782,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -809,7 +809,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$H$12</c:f>
+              <c:f>Sheet1!$C$40:$H$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -846,7 +846,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$13</c:f>
+              <c:f>Sheet1!$B$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -871,7 +871,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -898,7 +898,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$13:$H$13</c:f>
+              <c:f>Sheet1!$C$41:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -935,7 +935,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$14</c:f>
+              <c:f>Sheet1!$B$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -960,7 +960,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -987,7 +987,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$H$14</c:f>
+              <c:f>Sheet1!$C$42:$H$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1024,7 +1024,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$15</c:f>
+              <c:f>Sheet1!$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1049,7 +1049,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1076,7 +1076,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$H$15</c:f>
+              <c:f>Sheet1!$C$43:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1113,7 +1113,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
+              <c:f>Sheet1!$B$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1138,7 +1138,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1165,7 +1165,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$H$16</c:f>
+              <c:f>Sheet1!$C$44:$H$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1202,7 +1202,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$17</c:f>
+              <c:f>Sheet1!$B$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1227,7 +1227,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1254,7 +1254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$H$17</c:f>
+              <c:f>Sheet1!$C$45:$H$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1291,7 +1291,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>Sheet1!$B$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1316,7 +1316,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1343,7 +1343,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$H$18</c:f>
+              <c:f>Sheet1!$C$46:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1380,7 +1380,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$19</c:f>
+              <c:f>Sheet1!$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1406,7 +1406,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1433,7 +1433,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$H$19</c:f>
+              <c:f>Sheet1!$C$47:$H$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1470,7 +1470,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
+              <c:f>Sheet1!$B$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1496,7 +1496,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1523,7 +1523,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$H$20</c:f>
+              <c:f>Sheet1!$C$48:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1560,7 +1560,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$21</c:f>
+              <c:f>Sheet1!$B$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1586,7 +1586,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1613,7 +1613,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$H$21</c:f>
+              <c:f>Sheet1!$C$49:$H$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1650,7 +1650,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$22</c:f>
+              <c:f>Sheet1!$B$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1676,7 +1676,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$H$6</c:f>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1703,7 +1703,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$22:$H$22</c:f>
+              <c:f>Sheet1!$C$50:$H$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2499,16 +2499,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>31749</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2833,20 +2833,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
-  <dimension ref="B1:S87"/>
+  <dimension ref="B1:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="16" t="s">
         <v>24</v>
       </c>
@@ -2860,8 +2860,10 @@
       <c r="I1" s="17"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B2" s="16"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2871,1882 +2873,1878 @@
       <c r="I2" s="17"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="16"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C5" s="14" t="s">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N5" s="15"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C6">
-        <f>N6</f>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="1">
         <v>100</v>
       </c>
-      <c r="D6">
-        <f>O6</f>
+      <c r="Q6" s="1">
         <v>1000</v>
       </c>
-      <c r="E6">
+      <c r="R6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="S6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="U6" s="1">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>5</v>
+      </c>
+      <c r="R7" s="3">
+        <v>78</v>
+      </c>
+      <c r="S7" s="8">
+        <v>5775</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N8" s="11"/>
+      <c r="O8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>2</v>
+      </c>
+      <c r="R8" s="3">
+        <v>76</v>
+      </c>
+      <c r="S8" s="8">
+        <v>5828</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N9" s="11"/>
+      <c r="O9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>2</v>
+      </c>
+      <c r="R9" s="8">
+        <v>33</v>
+      </c>
+      <c r="S9" s="8">
+        <v>3250</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N10" s="11"/>
+      <c r="O10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
+      <c r="R10" s="8">
+        <v>34</v>
+      </c>
+      <c r="S10" s="8">
+        <v>3214</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N11" s="12"/>
+      <c r="O11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>1</v>
+      </c>
+      <c r="R11" s="5">
+        <v>33</v>
+      </c>
+      <c r="S11" s="5">
+        <v>3199</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>5</v>
+      </c>
+      <c r="R12" s="8">
+        <v>10</v>
+      </c>
+      <c r="S12" s="8">
+        <v>22</v>
+      </c>
+      <c r="T12" s="8">
+        <v>221</v>
+      </c>
+      <c r="U12" s="8">
+        <v>3521</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N13" s="11"/>
+      <c r="O13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>1</v>
+      </c>
+      <c r="R13" s="8">
+        <v>3</v>
+      </c>
+      <c r="S13" s="8">
+        <v>22</v>
+      </c>
+      <c r="T13" s="8">
+        <v>216</v>
+      </c>
+      <c r="U13" s="8">
+        <v>3527</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N14" s="11"/>
+      <c r="O14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>3</v>
+      </c>
+      <c r="R14" s="8">
+        <v>3</v>
+      </c>
+      <c r="S14" s="8">
+        <v>19</v>
+      </c>
+      <c r="T14" s="8">
+        <v>221</v>
+      </c>
+      <c r="U14" s="8">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N15" s="11"/>
+      <c r="O15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>1</v>
+      </c>
+      <c r="R15" s="8">
+        <v>3</v>
+      </c>
+      <c r="S15" s="8">
+        <v>16</v>
+      </c>
+      <c r="T15" s="8">
+        <v>223</v>
+      </c>
+      <c r="U15" s="8">
+        <v>3585</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N16" s="12"/>
+      <c r="O16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>1</v>
+      </c>
+      <c r="R16" s="5">
+        <v>3</v>
+      </c>
+      <c r="S16" s="5">
+        <v>17</v>
+      </c>
+      <c r="T16" s="5">
+        <v>221</v>
+      </c>
+      <c r="U16" s="5">
+        <v>3555</v>
+      </c>
+    </row>
+    <row r="17" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>9</v>
+      </c>
+      <c r="R17" s="7">
+        <v>178</v>
+      </c>
+      <c r="S17" s="7">
+        <v>24234</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N18" s="11"/>
+      <c r="O18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>6</v>
+      </c>
+      <c r="R18" s="8">
+        <v>186</v>
+      </c>
+      <c r="S18" s="8">
+        <v>24313</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N19" s="11"/>
+      <c r="O19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>2</v>
+      </c>
+      <c r="R19" s="8">
+        <v>125</v>
+      </c>
+      <c r="S19" s="8">
+        <v>12675</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N20" s="11"/>
+      <c r="O20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>1</v>
+      </c>
+      <c r="R20" s="8">
+        <v>173</v>
+      </c>
+      <c r="S20" s="8">
+        <v>12459</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N21" s="12"/>
+      <c r="O21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P21" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>2</v>
+      </c>
+      <c r="R21" s="5">
+        <v>168</v>
+      </c>
+      <c r="S21" s="5">
+        <v>12523</v>
+      </c>
+      <c r="T21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U21" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P22" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>2</v>
+      </c>
+      <c r="R22" s="8">
+        <v>10</v>
+      </c>
+      <c r="S22" s="8">
+        <v>20</v>
+      </c>
+      <c r="T22" s="8">
+        <v>218</v>
+      </c>
+      <c r="U22" s="8">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="23" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N23" s="11"/>
+      <c r="O23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P23" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>2</v>
+      </c>
+      <c r="R23" s="8">
+        <v>2</v>
+      </c>
+      <c r="S23" s="8">
+        <v>22</v>
+      </c>
+      <c r="T23" s="8">
+        <v>218</v>
+      </c>
+      <c r="U23" s="8">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="24" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N24" s="11"/>
+      <c r="O24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P24" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>1</v>
+      </c>
+      <c r="R24" s="8">
+        <v>2</v>
+      </c>
+      <c r="S24" s="8">
+        <v>14</v>
+      </c>
+      <c r="T24" s="8">
+        <v>139</v>
+      </c>
+      <c r="U24" s="8">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="25" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N25" s="11"/>
+      <c r="O25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P25" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>0</v>
+      </c>
+      <c r="R25" s="8">
+        <v>1</v>
+      </c>
+      <c r="S25" s="8">
+        <v>12</v>
+      </c>
+      <c r="T25" s="8">
+        <v>140</v>
+      </c>
+      <c r="U25" s="8">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="26" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N26" s="12"/>
+      <c r="O26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>1</v>
+      </c>
+      <c r="R26" s="5">
+        <v>1</v>
+      </c>
+      <c r="S26" s="5">
+        <v>12</v>
+      </c>
+      <c r="T26" s="5">
+        <v>141</v>
+      </c>
+      <c r="U26" s="5">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="27" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>4</v>
+      </c>
+      <c r="R27" s="7">
+        <v>33</v>
+      </c>
+      <c r="S27" s="7">
+        <v>1280</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N28" s="11"/>
+      <c r="O28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P28" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>2</v>
+      </c>
+      <c r="R28" s="8">
+        <v>17</v>
+      </c>
+      <c r="S28" s="8">
+        <v>1206</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N29" s="11"/>
+      <c r="O29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>1</v>
+      </c>
+      <c r="R29" s="8">
+        <v>21</v>
+      </c>
+      <c r="S29" s="8">
+        <v>2125</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N30" s="11"/>
+      <c r="O30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P30" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>1</v>
+      </c>
+      <c r="R30" s="8">
+        <v>20</v>
+      </c>
+      <c r="S30" s="8">
+        <v>2371</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N31" s="12"/>
+      <c r="O31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P31" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>1</v>
+      </c>
+      <c r="R31" s="5">
+        <v>22</v>
+      </c>
+      <c r="S31" s="5">
+        <v>2461</v>
+      </c>
+      <c r="T31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U31" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N32" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P32" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>2</v>
+      </c>
+      <c r="R32" s="7">
+        <v>11</v>
+      </c>
+      <c r="S32" s="7">
+        <v>28</v>
+      </c>
+      <c r="T32" s="7">
+        <v>235</v>
+      </c>
+      <c r="U32" s="9">
+        <v>3373</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C33" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P33" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>1</v>
+      </c>
+      <c r="R33" s="8">
+        <v>3</v>
+      </c>
+      <c r="S33" s="8">
+        <v>21</v>
+      </c>
+      <c r="T33" s="8">
+        <v>229</v>
+      </c>
+      <c r="U33" s="8">
+        <v>3296</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C34">
         <f>P6</f>
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <f>Q6</f>
+        <v>1000</v>
+      </c>
+      <c r="E34">
+        <f>R6</f>
         <v>10000</v>
       </c>
-      <c r="F6">
-        <f>Q6</f>
+      <c r="F34">
+        <f>S6</f>
         <v>100000</v>
       </c>
-      <c r="G6">
-        <f>R6</f>
+      <c r="G34">
+        <f>T6</f>
         <v>1000000</v>
       </c>
-      <c r="H6">
-        <f>S6</f>
+      <c r="H34">
+        <f>U6</f>
         <v>10000000</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="1">
-        <v>100</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="P6" s="1">
-        <v>10000</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>100000</v>
-      </c>
-      <c r="R6" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="S6" s="1">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <f>AVERAGE(N7:N11)</f>
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <f>AVERAGE(O7:O11)</f>
+      <c r="N34" s="11"/>
+      <c r="O34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P34" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>1</v>
+      </c>
+      <c r="R34" s="8">
+        <v>2</v>
+      </c>
+      <c r="S34" s="8">
+        <v>19</v>
+      </c>
+      <c r="T34" s="8">
+        <v>239</v>
+      </c>
+      <c r="U34" s="8">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <f>AVERAGE(P7:P11)</f>
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>AVERAGE(Q7:Q11)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E7">
-        <f>AVERAGE(P7:P11)</f>
+      <c r="E35">
+        <f>AVERAGE(R7:R11)</f>
         <v>50.8</v>
       </c>
-      <c r="F7">
-        <f>AVERAGE(Q7:Q11)</f>
+      <c r="F35">
+        <f>AVERAGE(S7:S11)</f>
         <v>4253.2</v>
       </c>
-      <c r="G7">
+      <c r="G35">
         <v>999999</v>
       </c>
-      <c r="H7">
+      <c r="H35">
         <v>9999999</v>
       </c>
-      <c r="L7" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="3">
-        <v>2</v>
-      </c>
-      <c r="O7" s="3">
+      <c r="N35" s="11"/>
+      <c r="O35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P7" s="3">
-        <v>78</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>5775</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+      <c r="P35" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>1</v>
+      </c>
+      <c r="R35" s="8">
+        <v>2</v>
+      </c>
+      <c r="S35" s="8">
+        <v>17</v>
+      </c>
+      <c r="T35" s="8">
+        <v>230</v>
+      </c>
+      <c r="U35" s="8">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
-        <f>AVERAGE(N12:N16)</f>
+      <c r="C36">
+        <f>AVERAGE(P12:P16)</f>
         <v>0.6</v>
       </c>
-      <c r="D8">
-        <f>AVERAGE(O12:O16)</f>
+      <c r="D36">
+        <f>AVERAGE(Q12:Q16)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E8">
-        <f>AVERAGE(P12:P16)</f>
+      <c r="E36">
+        <f>AVERAGE(R12:R16)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="F8">
-        <f>AVERAGE(Q12:Q16)</f>
+      <c r="F36">
+        <f>AVERAGE(S12:S16)</f>
         <v>19.2</v>
       </c>
-      <c r="G8">
-        <f>AVERAGE(R12:R16)</f>
+      <c r="G36">
+        <f>AVERAGE(T12:T16)</f>
         <v>220.4</v>
       </c>
-      <c r="H8">
-        <f>AVERAGE(S12:S16)</f>
+      <c r="H36">
+        <f>AVERAGE(U12:U16)</f>
         <v>3546.8</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="2" t="s">
+      <c r="N36" s="12"/>
+      <c r="O36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P36" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>1</v>
+      </c>
+      <c r="R36" s="5">
+        <v>2</v>
+      </c>
+      <c r="S36" s="5">
+        <v>18</v>
+      </c>
+      <c r="T36" s="5">
+        <v>228</v>
+      </c>
+      <c r="U36" s="5">
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <f>AVERAGE(P17:P21)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D37">
+        <f>AVERAGE(Q17:Q21)</f>
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <f>AVERAGE(R17:R21)</f>
+        <v>166</v>
+      </c>
+      <c r="F37">
+        <f>AVERAGE(S17:S21)</f>
+        <v>17240.8</v>
+      </c>
+      <c r="G37">
+        <v>999999</v>
+      </c>
+      <c r="H37">
+        <v>9999999</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P37" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>4</v>
+      </c>
+      <c r="R37" s="7">
+        <v>13</v>
+      </c>
+      <c r="S37" s="7">
+        <v>22</v>
+      </c>
+      <c r="T37" s="7">
+        <v>127</v>
+      </c>
+      <c r="U37" s="8">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38">
+        <f>AVERAGE(P22:P26)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D38">
+        <f>AVERAGE(Q22:Q26)</f>
+        <v>1.2</v>
+      </c>
+      <c r="E38">
+        <f>AVERAGE(R22:R26)</f>
+        <v>3.2</v>
+      </c>
+      <c r="F38">
+        <f>AVERAGE(S22:S26)</f>
+        <v>16</v>
+      </c>
+      <c r="G38">
+        <f>AVERAGE(T22:T26)</f>
+        <v>171.2</v>
+      </c>
+      <c r="H38">
+        <f>AVERAGE(U22:U26)</f>
+        <v>2048.1999999999998</v>
+      </c>
+      <c r="N38" s="11"/>
+      <c r="O38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3">
-        <v>2</v>
-      </c>
-      <c r="P8" s="3">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>5828</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="P38" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>6</v>
+      </c>
+      <c r="R38" s="8">
+        <v>11</v>
+      </c>
+      <c r="S38" s="8">
+        <v>15</v>
+      </c>
+      <c r="T38" s="8">
+        <v>119</v>
+      </c>
+      <c r="U38" s="8">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <f>AVERAGE(P27:P31)</f>
+        <v>1.2</v>
+      </c>
+      <c r="D39">
+        <f>AVERAGE(Q27:Q31)</f>
+        <v>1.8</v>
+      </c>
+      <c r="E39">
+        <f>AVERAGE(R27:R31)</f>
+        <v>22.6</v>
+      </c>
+      <c r="F39">
+        <f>AVERAGE(S27:S31)</f>
+        <v>1888.6</v>
+      </c>
+      <c r="G39">
+        <v>999999</v>
+      </c>
+      <c r="H39">
+        <v>9999999</v>
+      </c>
+      <c r="N39" s="11"/>
+      <c r="O39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P39" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>2</v>
+      </c>
+      <c r="R39" s="8">
+        <v>2</v>
+      </c>
+      <c r="S39" s="8">
+        <v>10</v>
+      </c>
+      <c r="T39" s="8">
+        <v>122</v>
+      </c>
+      <c r="U39" s="8">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40">
+        <f>AVERAGE(P32:P36)</f>
+        <v>1.2</v>
+      </c>
+      <c r="D40">
+        <f>AVERAGE(Q32:Q36)</f>
+        <v>1.2</v>
+      </c>
+      <c r="E40">
+        <f>AVERAGE(R32:R36)</f>
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <f>AVERAGE(S32:S36)</f>
+        <v>20.6</v>
+      </c>
+      <c r="G40">
+        <f>AVERAGE(T32:T36)</f>
+        <v>232.2</v>
+      </c>
+      <c r="H40">
+        <f>AVERAGE(U32:U36)</f>
+        <v>3327.6</v>
+      </c>
+      <c r="N40" s="11"/>
+      <c r="O40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P40" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>1</v>
+      </c>
+      <c r="R40" s="8">
+        <v>1</v>
+      </c>
+      <c r="S40" s="8">
+        <v>10</v>
+      </c>
+      <c r="T40" s="8">
+        <v>120</v>
+      </c>
+      <c r="U40" s="8">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <f>AVERAGE(P37:P41)</f>
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <f>AVERAGE(Q37:Q41)</f>
+        <v>2.8</v>
+      </c>
+      <c r="E41">
+        <f>AVERAGE(R37:R41)</f>
+        <v>5.6</v>
+      </c>
+      <c r="F41">
+        <f>AVERAGE(S37:S41)</f>
+        <v>13.6</v>
+      </c>
+      <c r="G41">
+        <f>AVERAGE(T37:T41)</f>
+        <v>122.8</v>
+      </c>
+      <c r="H41">
+        <f>AVERAGE(U37:U41)</f>
+        <v>1352.8</v>
+      </c>
+      <c r="N41" s="12"/>
+      <c r="O41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P41" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>1</v>
+      </c>
+      <c r="R41" s="5">
+        <v>1</v>
+      </c>
+      <c r="S41" s="5">
+        <v>11</v>
+      </c>
+      <c r="T41" s="5">
+        <v>126</v>
+      </c>
+      <c r="U41" s="5">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <f>AVERAGE(P42:P46)</f>
         <v>7</v>
       </c>
-      <c r="C9">
-        <f>AVERAGE(N17:N21)</f>
+      <c r="D42">
+        <f>AVERAGE(Q42:Q46)</f>
+        <v>30.2</v>
+      </c>
+      <c r="E42">
+        <f>AVERAGE(R42:R46)</f>
+        <v>31.2</v>
+      </c>
+      <c r="F42">
+        <f>AVERAGE(S42:S46)</f>
+        <v>77.2</v>
+      </c>
+      <c r="G42">
+        <f>AVERAGE(T42:T46)</f>
+        <v>344</v>
+      </c>
+      <c r="H42">
+        <f>AVERAGE(U42:U46)</f>
+        <v>3308.4</v>
+      </c>
+      <c r="N42" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P42" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q42" s="7">
+        <v>39</v>
+      </c>
+      <c r="R42" s="7">
+        <v>144</v>
+      </c>
+      <c r="S42" s="7">
+        <v>234</v>
+      </c>
+      <c r="T42" s="7">
+        <v>497</v>
+      </c>
+      <c r="U42" s="8">
+        <v>3533</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <f>AVERAGE(P47:P51)</f>
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <f>AVERAGE(Q47:Q51)</f>
+        <v>1.2</v>
+      </c>
+      <c r="E43">
+        <f>AVERAGE(R47:R51)</f>
+        <v>2.6</v>
+      </c>
+      <c r="F43">
+        <f>AVERAGE(S47:S51)</f>
+        <v>18.8</v>
+      </c>
+      <c r="G43">
+        <f>AVERAGE(T47:T51)</f>
+        <v>140.6</v>
+      </c>
+      <c r="H43">
+        <f>AVERAGE(U47:U51)</f>
+        <v>1187.2</v>
+      </c>
+      <c r="N43" s="11"/>
+      <c r="O43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P43" s="8">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>49</v>
+      </c>
+      <c r="R43" s="8">
+        <v>3</v>
+      </c>
+      <c r="S43" s="8">
+        <v>34</v>
+      </c>
+      <c r="T43" s="8">
+        <v>291</v>
+      </c>
+      <c r="U43" s="8">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <f>AVERAGE(P52:P56)</f>
         <v>0.8</v>
       </c>
-      <c r="D9">
-        <f>AVERAGE(O17:O21)</f>
+      <c r="D44">
+        <f>AVERAGE(Q52:Q56)</f>
+        <v>1.4</v>
+      </c>
+      <c r="E44">
+        <f>AVERAGE(R52:R56)</f>
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <f>AVERAGE(S52:S56)</f>
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <f>AVERAGE(T52:T56)</f>
+        <v>7</v>
+      </c>
+      <c r="H44">
+        <f>AVERAGE(U52:U56)</f>
+        <v>29.4</v>
+      </c>
+      <c r="N44" s="11"/>
+      <c r="O44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9">
-        <f>AVERAGE(P17:P21)</f>
-        <v>166</v>
-      </c>
-      <c r="F9">
-        <f>AVERAGE(Q17:Q21)</f>
-        <v>17240.8</v>
-      </c>
-      <c r="G9">
-        <v>999999</v>
-      </c>
-      <c r="H9">
-        <v>9999999</v>
-      </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="8">
-        <v>1</v>
-      </c>
-      <c r="O9" s="8">
-        <v>2</v>
-      </c>
-      <c r="P9" s="8">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>3250</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <f>AVERAGE(N22:N26)</f>
+      <c r="P44" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>60</v>
+      </c>
+      <c r="R44" s="8">
+        <v>3</v>
+      </c>
+      <c r="S44" s="8">
+        <v>37</v>
+      </c>
+      <c r="T44" s="8">
+        <v>337</v>
+      </c>
+      <c r="U44" s="8">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <f>AVERAGE(P57:P61)</f>
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <f>AVERAGE(Q57:Q61)</f>
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f>AVERAGE(R57:R61)</f>
+        <v>1.8</v>
+      </c>
+      <c r="F45">
+        <f>AVERAGE(S57:S61)</f>
+        <v>1.6</v>
+      </c>
+      <c r="G45">
+        <f>AVERAGE(T57:T61)</f>
+        <v>3.2</v>
+      </c>
+      <c r="H45">
+        <f>AVERAGE(U57:U61)</f>
+        <v>16.2</v>
+      </c>
+      <c r="N45" s="11"/>
+      <c r="O45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P45" s="8">
+        <v>7</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>2</v>
+      </c>
+      <c r="R45" s="8">
+        <v>3</v>
+      </c>
+      <c r="S45" s="8">
+        <v>40</v>
+      </c>
+      <c r="T45" s="8">
+        <v>299</v>
+      </c>
+      <c r="U45" s="8">
+        <v>3263</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <f>AVERAGE(P62:P66)</f>
         <v>0.8</v>
       </c>
-      <c r="D10">
-        <f>AVERAGE(O22:O26)</f>
+      <c r="D46">
+        <f>AVERAGE(Q62:Q66)</f>
         <v>1.2</v>
       </c>
-      <c r="E10">
-        <f>AVERAGE(P22:P26)</f>
-        <v>3.2</v>
-      </c>
-      <c r="F10">
-        <f>AVERAGE(Q22:Q26)</f>
-        <v>16</v>
-      </c>
-      <c r="G10">
-        <f>AVERAGE(R22:R26)</f>
-        <v>171.2</v>
-      </c>
-      <c r="H10">
-        <f>AVERAGE(S22:S26)</f>
-        <v>2048.1999999999998</v>
-      </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="O10" s="8">
-        <v>1</v>
-      </c>
-      <c r="P10" s="8">
-        <v>34</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>3214</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <f>AVERAGE(N27:N31)</f>
-        <v>1.2</v>
-      </c>
-      <c r="D11">
-        <f>AVERAGE(O27:O31)</f>
-        <v>1.8</v>
-      </c>
-      <c r="E11">
-        <f>AVERAGE(P27:P31)</f>
-        <v>22.6</v>
-      </c>
-      <c r="F11">
-        <f>AVERAGE(Q27:Q31)</f>
-        <v>1888.6</v>
-      </c>
-      <c r="G11">
-        <v>999999</v>
-      </c>
-      <c r="H11">
-        <v>9999999</v>
-      </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="4" t="s">
+      <c r="E46">
+        <f>AVERAGE(R62:R66)</f>
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <f>AVERAGE(S62:S66)</f>
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <f>AVERAGE(T62:T66)</f>
+        <v>2.4</v>
+      </c>
+      <c r="H46">
+        <f>AVERAGE(U62:U66)</f>
+        <v>10.4</v>
+      </c>
+      <c r="N46" s="12"/>
+      <c r="O46" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="N11" s="5">
-        <v>1</v>
-      </c>
-      <c r="O11" s="5">
-        <v>1</v>
-      </c>
-      <c r="P11" s="5">
-        <v>33</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>3199</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <f>AVERAGE(N32:N36)</f>
-        <v>1.2</v>
-      </c>
-      <c r="D12">
-        <f>AVERAGE(O32:O36)</f>
-        <v>1.2</v>
-      </c>
-      <c r="E12">
-        <f>AVERAGE(P32:P36)</f>
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <f>AVERAGE(Q32:Q36)</f>
-        <v>20.6</v>
-      </c>
-      <c r="G12">
-        <f>AVERAGE(R32:R36)</f>
-        <v>232.2</v>
-      </c>
-      <c r="H12">
-        <f>AVERAGE(S32:S36)</f>
-        <v>3327.6</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N12" s="8">
-        <v>1</v>
-      </c>
-      <c r="O12" s="8">
-        <v>5</v>
-      </c>
-      <c r="P12" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>22</v>
-      </c>
-      <c r="R12" s="8">
-        <v>221</v>
-      </c>
-      <c r="S12" s="8">
-        <v>3521</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <f>AVERAGE(N37:N41)</f>
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <f>AVERAGE(O37:O41)</f>
-        <v>2.8</v>
-      </c>
-      <c r="E13">
-        <f>AVERAGE(P37:P41)</f>
-        <v>5.6</v>
-      </c>
-      <c r="F13">
-        <f>AVERAGE(Q37:Q41)</f>
-        <v>13.6</v>
-      </c>
-      <c r="G13">
-        <f>AVERAGE(R37:R41)</f>
-        <v>122.8</v>
-      </c>
-      <c r="H13">
-        <f>AVERAGE(S37:S41)</f>
-        <v>1352.8</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N13" s="8">
-        <v>1</v>
-      </c>
-      <c r="O13" s="8">
-        <v>1</v>
-      </c>
-      <c r="P13" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>22</v>
-      </c>
-      <c r="R13" s="8">
-        <v>216</v>
-      </c>
-      <c r="S13" s="8">
-        <v>3527</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <f>AVERAGE(N42:N46)</f>
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <f>AVERAGE(O42:O46)</f>
-        <v>30.2</v>
-      </c>
-      <c r="E14">
-        <f>AVERAGE(P42:P46)</f>
-        <v>31.2</v>
-      </c>
-      <c r="F14">
-        <f>AVERAGE(Q42:Q46)</f>
-        <v>77.2</v>
-      </c>
-      <c r="G14">
-        <f>AVERAGE(R42:R46)</f>
-        <v>344</v>
-      </c>
-      <c r="H14">
-        <f>AVERAGE(S42:S46)</f>
-        <v>3308.4</v>
-      </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8">
-        <v>3</v>
-      </c>
-      <c r="P14" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>19</v>
-      </c>
-      <c r="R14" s="8">
-        <v>221</v>
-      </c>
-      <c r="S14" s="8">
-        <v>3546</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <f>AVERAGE(N47:N51)</f>
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <f>AVERAGE(O47:O51)</f>
-        <v>1.2</v>
-      </c>
-      <c r="E15">
-        <f>AVERAGE(P47:P51)</f>
-        <v>2.6</v>
-      </c>
-      <c r="F15">
-        <f>AVERAGE(Q47:Q51)</f>
-        <v>18.8</v>
-      </c>
-      <c r="G15">
-        <f>AVERAGE(R47:R51)</f>
-        <v>140.6</v>
-      </c>
-      <c r="H15">
-        <f>AVERAGE(S47:S51)</f>
-        <v>1187.2</v>
-      </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N15" s="8">
-        <v>0</v>
-      </c>
-      <c r="O15" s="8">
-        <v>1</v>
-      </c>
-      <c r="P15" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>16</v>
-      </c>
-      <c r="R15" s="8">
-        <v>223</v>
-      </c>
-      <c r="S15" s="8">
-        <v>3585</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <f>AVERAGE(N52:N56)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D16">
-        <f>AVERAGE(O52:O56)</f>
-        <v>1.4</v>
-      </c>
-      <c r="E16">
-        <f>AVERAGE(P52:P56)</f>
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <f>AVERAGE(Q52:Q56)</f>
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <f>AVERAGE(R52:R56)</f>
-        <v>7</v>
-      </c>
-      <c r="H16">
-        <f>AVERAGE(S52:S56)</f>
-        <v>29.4</v>
-      </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16" s="5">
-        <v>1</v>
-      </c>
-      <c r="O16" s="5">
-        <v>1</v>
-      </c>
-      <c r="P16" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>17</v>
-      </c>
-      <c r="R16" s="5">
-        <v>221</v>
-      </c>
-      <c r="S16" s="5">
-        <v>3555</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17">
-        <f>AVERAGE(N57:N61)</f>
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <f>AVERAGE(O57:O61)</f>
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <f>AVERAGE(P57:P61)</f>
-        <v>1.8</v>
-      </c>
-      <c r="F17">
-        <f>AVERAGE(Q57:Q61)</f>
-        <v>1.6</v>
-      </c>
-      <c r="G17">
-        <f>AVERAGE(R57:R61)</f>
-        <v>3.2</v>
-      </c>
-      <c r="H17">
-        <f>AVERAGE(S57:S61)</f>
-        <v>16.2</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N17" s="7">
-        <v>2</v>
-      </c>
-      <c r="O17" s="7">
-        <v>9</v>
-      </c>
-      <c r="P17" s="7">
-        <v>178</v>
-      </c>
-      <c r="Q17" s="7">
-        <v>24234</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <f>AVERAGE(N62:N66)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D18">
-        <f>AVERAGE(O62:O66)</f>
-        <v>1.2</v>
-      </c>
-      <c r="E18">
-        <f>AVERAGE(P62:P66)</f>
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <f>AVERAGE(Q62:Q66)</f>
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <f>AVERAGE(R62:R66)</f>
-        <v>2.4</v>
-      </c>
-      <c r="H18">
-        <f>AVERAGE(S62:S66)</f>
-        <v>10.4</v>
-      </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N18" s="8">
-        <v>0</v>
-      </c>
-      <c r="O18" s="8">
-        <v>6</v>
-      </c>
-      <c r="P18" s="8">
-        <v>186</v>
-      </c>
-      <c r="Q18" s="8">
-        <v>24313</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19">
-        <f>AVERAGE(N67:N71)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D19">
-        <f>AVERAGE(O67:O71)</f>
-        <v>1.2</v>
-      </c>
-      <c r="E19">
-        <f>AVERAGE(P67:P71)</f>
-        <v>3.6</v>
-      </c>
-      <c r="F19">
-        <f>AVERAGE(Q67:Q71)</f>
-        <v>12.8</v>
-      </c>
-      <c r="G19">
-        <f>AVERAGE(R67:R71)</f>
-        <v>142.6</v>
-      </c>
-      <c r="H19">
-        <f>AVERAGE(S67:S71)</f>
-        <v>1334.2</v>
-      </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N19" s="8">
-        <v>1</v>
-      </c>
-      <c r="O19" s="8">
-        <v>2</v>
-      </c>
-      <c r="P19" s="8">
-        <v>125</v>
-      </c>
-      <c r="Q19" s="8">
-        <v>12675</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <f>AVERAGE(N72:N76)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D20">
-        <f>AVERAGE(O72:O76)</f>
-        <v>1.2</v>
-      </c>
-      <c r="E20">
-        <f>AVERAGE(P72:P76)</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F20">
-        <f>AVERAGE(Q72:Q76)</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G20">
-        <f>AVERAGE(R72:R76)</f>
-        <v>26.6</v>
-      </c>
-      <c r="H20">
-        <f>AVERAGE(S72:S76)</f>
-        <v>317.60000000000002</v>
-      </c>
-      <c r="L20" s="11"/>
-      <c r="M20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N20" s="8">
-        <v>1</v>
-      </c>
-      <c r="O20" s="8">
-        <v>1</v>
-      </c>
-      <c r="P20" s="8">
-        <v>173</v>
-      </c>
-      <c r="Q20" s="8">
-        <v>12459</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <f>AVERAGE(N77:N81)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D21">
-        <f>AVERAGE(O77:O81)</f>
-        <v>1.2</v>
-      </c>
-      <c r="E21">
-        <f>AVERAGE(P77:P81)</f>
-        <v>5.4</v>
-      </c>
-      <c r="F21">
-        <f>AVERAGE(Q77:Q81)</f>
-        <v>3.4</v>
-      </c>
-      <c r="G21">
-        <f>AVERAGE(R77:R81)</f>
-        <v>74.599999999999994</v>
-      </c>
-      <c r="H21">
-        <f>AVERAGE(S77:S81)</f>
-        <v>1426.6</v>
-      </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-      <c r="O21" s="5">
-        <v>2</v>
-      </c>
-      <c r="P21" s="5">
-        <v>168</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>12523</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <f>AVERAGE(N82:N86)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D22">
-        <f>AVERAGE(O82:O86)</f>
-        <v>1.4</v>
-      </c>
-      <c r="E22">
-        <f>AVERAGE(P82:P86)</f>
-        <v>1.6</v>
-      </c>
-      <c r="F22">
-        <f>AVERAGE(Q82:Q86)</f>
-        <v>3.2</v>
-      </c>
-      <c r="G22">
-        <f>AVERAGE(R82:R86)</f>
-        <v>29.6</v>
-      </c>
-      <c r="H22">
-        <f>AVERAGE(S82:S86)</f>
-        <v>317.8</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N22" s="8">
-        <v>1</v>
-      </c>
-      <c r="O22" s="8">
-        <v>2</v>
-      </c>
-      <c r="P22" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="8">
-        <v>20</v>
-      </c>
-      <c r="R22" s="8">
-        <v>218</v>
-      </c>
-      <c r="S22" s="8">
-        <v>2597</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="L23" s="11"/>
-      <c r="M23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N23" s="8">
-        <v>1</v>
-      </c>
-      <c r="O23" s="8">
-        <v>2</v>
-      </c>
-      <c r="P23" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>22</v>
-      </c>
-      <c r="R23" s="8">
-        <v>218</v>
-      </c>
-      <c r="S23" s="8">
-        <v>2607</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="L24" s="11"/>
-      <c r="M24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N24" s="8">
-        <v>1</v>
-      </c>
-      <c r="O24" s="8">
-        <v>1</v>
-      </c>
-      <c r="P24" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q24" s="8">
-        <v>14</v>
-      </c>
-      <c r="R24" s="8">
-        <v>139</v>
-      </c>
-      <c r="S24" s="8">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="L25" s="11"/>
-      <c r="M25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N25" s="8">
-        <v>1</v>
-      </c>
-      <c r="O25" s="8">
-        <v>0</v>
-      </c>
-      <c r="P25" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="8">
-        <v>12</v>
-      </c>
-      <c r="R25" s="8">
-        <v>140</v>
-      </c>
-      <c r="S25" s="8">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L26" s="12"/>
-      <c r="M26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N26" s="5">
-        <v>0</v>
-      </c>
-      <c r="O26" s="5">
-        <v>1</v>
-      </c>
-      <c r="P26" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="5">
-        <v>12</v>
-      </c>
-      <c r="R26" s="5">
-        <v>141</v>
-      </c>
-      <c r="S26" s="5">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L27" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N27" s="7">
-        <v>2</v>
-      </c>
-      <c r="O27" s="7">
-        <v>4</v>
-      </c>
-      <c r="P27" s="7">
-        <v>33</v>
-      </c>
-      <c r="Q27" s="7">
-        <v>1280</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="L28" s="11"/>
-      <c r="M28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N28" s="8">
-        <v>1</v>
-      </c>
-      <c r="O28" s="8">
-        <v>2</v>
-      </c>
-      <c r="P28" s="8">
-        <v>17</v>
-      </c>
-      <c r="Q28" s="8">
-        <v>1206</v>
-      </c>
-      <c r="R28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S28" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="L29" s="11"/>
-      <c r="M29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N29" s="8">
-        <v>1</v>
-      </c>
-      <c r="O29" s="8">
-        <v>1</v>
-      </c>
-      <c r="P29" s="8">
-        <v>21</v>
-      </c>
-      <c r="Q29" s="8">
-        <v>2125</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="L30" s="11"/>
-      <c r="M30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N30" s="8">
-        <v>1</v>
-      </c>
-      <c r="O30" s="8">
-        <v>1</v>
-      </c>
-      <c r="P30" s="8">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="8">
-        <v>2371</v>
-      </c>
-      <c r="R30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L31" s="12"/>
-      <c r="M31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N31" s="5">
-        <v>1</v>
-      </c>
-      <c r="O31" s="5">
-        <v>1</v>
-      </c>
-      <c r="P31" s="5">
-        <v>22</v>
-      </c>
-      <c r="Q31" s="5">
-        <v>2461</v>
-      </c>
-      <c r="R31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S31" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N32" s="7">
-        <v>2</v>
-      </c>
-      <c r="O32" s="7">
-        <v>2</v>
-      </c>
-      <c r="P32" s="7">
-        <v>11</v>
-      </c>
-      <c r="Q32" s="7">
-        <v>28</v>
-      </c>
-      <c r="R32" s="7">
-        <v>235</v>
-      </c>
-      <c r="S32" s="9">
-        <v>3373</v>
-      </c>
-    </row>
-    <row r="33" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L33" s="11"/>
-      <c r="M33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N33" s="8">
-        <v>1</v>
-      </c>
-      <c r="O33" s="8">
-        <v>1</v>
-      </c>
-      <c r="P33" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q33" s="8">
-        <v>21</v>
-      </c>
-      <c r="R33" s="8">
-        <v>229</v>
-      </c>
-      <c r="S33" s="8">
-        <v>3296</v>
-      </c>
-    </row>
-    <row r="34" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L34" s="11"/>
-      <c r="M34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N34" s="8">
-        <v>1</v>
-      </c>
-      <c r="O34" s="8">
-        <v>1</v>
-      </c>
-      <c r="P34" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="8">
-        <v>19</v>
-      </c>
-      <c r="R34" s="8">
-        <v>239</v>
-      </c>
-      <c r="S34" s="8">
-        <v>3280</v>
-      </c>
-    </row>
-    <row r="35" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L35" s="11"/>
-      <c r="M35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N35" s="8">
-        <v>1</v>
-      </c>
-      <c r="O35" s="8">
-        <v>1</v>
-      </c>
-      <c r="P35" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q35" s="8">
-        <v>17</v>
-      </c>
-      <c r="R35" s="8">
-        <v>230</v>
-      </c>
-      <c r="S35" s="8">
-        <v>3287</v>
-      </c>
-    </row>
-    <row r="36" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L36" s="12"/>
-      <c r="M36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N36" s="5">
-        <v>1</v>
-      </c>
-      <c r="O36" s="5">
-        <v>1</v>
-      </c>
-      <c r="P36" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q36" s="5">
-        <v>18</v>
-      </c>
-      <c r="R36" s="5">
-        <v>228</v>
-      </c>
-      <c r="S36" s="5">
-        <v>3402</v>
-      </c>
-    </row>
-    <row r="37" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L37" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N37" s="7">
-        <v>2</v>
-      </c>
-      <c r="O37" s="7">
-        <v>4</v>
-      </c>
-      <c r="P37" s="7">
-        <v>13</v>
-      </c>
-      <c r="Q37" s="7">
-        <v>22</v>
-      </c>
-      <c r="R37" s="7">
-        <v>127</v>
-      </c>
-      <c r="S37" s="8">
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="38" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L38" s="11"/>
-      <c r="M38" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N38" s="8">
-        <v>1</v>
-      </c>
-      <c r="O38" s="8">
-        <v>6</v>
-      </c>
-      <c r="P38" s="8">
-        <v>11</v>
-      </c>
-      <c r="Q38" s="8">
-        <v>15</v>
-      </c>
-      <c r="R38" s="8">
-        <v>119</v>
-      </c>
-      <c r="S38" s="8">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="39" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L39" s="11"/>
-      <c r="M39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N39" s="8">
-        <v>1</v>
-      </c>
-      <c r="O39" s="8">
-        <v>2</v>
-      </c>
-      <c r="P39" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q39" s="8">
-        <v>10</v>
-      </c>
-      <c r="R39" s="8">
-        <v>122</v>
-      </c>
-      <c r="S39" s="8">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="40" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L40" s="11"/>
-      <c r="M40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N40" s="8">
-        <v>1</v>
-      </c>
-      <c r="O40" s="8">
-        <v>1</v>
-      </c>
-      <c r="P40" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="8">
-        <v>10</v>
-      </c>
-      <c r="R40" s="8">
-        <v>120</v>
-      </c>
-      <c r="S40" s="8">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="41" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L41" s="12"/>
-      <c r="M41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N41" s="5">
-        <v>0</v>
-      </c>
-      <c r="O41" s="5">
-        <v>1</v>
-      </c>
-      <c r="P41" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="5">
-        <v>11</v>
-      </c>
-      <c r="R41" s="5">
-        <v>126</v>
-      </c>
-      <c r="S41" s="5">
-        <v>1319</v>
-      </c>
-    </row>
-    <row r="42" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L42" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M42" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N42" s="7">
-        <v>11</v>
-      </c>
-      <c r="O42" s="7">
-        <v>39</v>
-      </c>
-      <c r="P42" s="7">
-        <v>144</v>
-      </c>
-      <c r="Q42" s="7">
-        <v>234</v>
-      </c>
-      <c r="R42" s="7">
-        <v>497</v>
-      </c>
-      <c r="S42" s="8">
-        <v>3533</v>
-      </c>
-    </row>
-    <row r="43" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L43" s="11"/>
-      <c r="M43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N43" s="8">
-        <v>9</v>
-      </c>
-      <c r="O43" s="8">
-        <v>49</v>
-      </c>
-      <c r="P43" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q43" s="8">
-        <v>34</v>
-      </c>
-      <c r="R43" s="8">
-        <v>291</v>
-      </c>
-      <c r="S43" s="8">
-        <v>3242</v>
-      </c>
-    </row>
-    <row r="44" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L44" s="11"/>
-      <c r="M44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N44" s="8">
-        <v>5</v>
-      </c>
-      <c r="O44" s="8">
-        <v>60</v>
-      </c>
-      <c r="P44" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q44" s="8">
-        <v>37</v>
-      </c>
-      <c r="R44" s="8">
-        <v>337</v>
-      </c>
-      <c r="S44" s="8">
-        <v>3245</v>
-      </c>
-    </row>
-    <row r="45" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L45" s="11"/>
-      <c r="M45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N45" s="8">
-        <v>7</v>
-      </c>
-      <c r="O45" s="8">
-        <v>2</v>
-      </c>
-      <c r="P45" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q45" s="8">
-        <v>40</v>
-      </c>
-      <c r="R45" s="8">
-        <v>299</v>
-      </c>
-      <c r="S45" s="8">
-        <v>3263</v>
-      </c>
-    </row>
-    <row r="46" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L46" s="12"/>
-      <c r="M46" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N46" s="5">
-        <v>3</v>
-      </c>
-      <c r="O46" s="5">
-        <v>1</v>
       </c>
       <c r="P46" s="5">
         <v>3</v>
       </c>
       <c r="Q46" s="5">
+        <v>1</v>
+      </c>
+      <c r="R46" s="5">
+        <v>3</v>
+      </c>
+      <c r="S46" s="5">
         <v>41</v>
       </c>
-      <c r="R46" s="5">
+      <c r="T46" s="5">
         <v>296</v>
       </c>
-      <c r="S46" s="5">
+      <c r="U46" s="5">
         <v>3259</v>
       </c>
     </row>
-    <row r="47" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L47" s="10" t="s">
+    <row r="47" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47">
+        <f>AVERAGE(P67:P71)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D47">
+        <f>AVERAGE(Q67:Q71)</f>
+        <v>1.2</v>
+      </c>
+      <c r="E47">
+        <f>AVERAGE(R67:R71)</f>
+        <v>3.6</v>
+      </c>
+      <c r="F47">
+        <f>AVERAGE(S67:S71)</f>
+        <v>12.8</v>
+      </c>
+      <c r="G47">
+        <f>AVERAGE(T67:T71)</f>
+        <v>142.6</v>
+      </c>
+      <c r="H47">
+        <f>AVERAGE(U67:U71)</f>
+        <v>1334.2</v>
+      </c>
+      <c r="N47" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M47" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N47" s="7">
-        <v>1</v>
-      </c>
-      <c r="O47" s="7">
+      <c r="O47" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P47" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="7">
+        <v>2</v>
+      </c>
+      <c r="R47" s="7">
         <v>7</v>
       </c>
-      <c r="Q47" s="7">
+      <c r="S47" s="7">
         <v>41</v>
       </c>
-      <c r="R47" s="7">
+      <c r="T47" s="7">
         <v>282</v>
       </c>
-      <c r="S47" s="8">
+      <c r="U47" s="8">
         <v>1232</v>
       </c>
     </row>
-    <row r="48" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L48" s="11"/>
-      <c r="M48" s="2" t="s">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <f>AVERAGE(P72:P76)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D48">
+        <f>AVERAGE(Q72:Q76)</f>
+        <v>1.2</v>
+      </c>
+      <c r="E48">
+        <f>AVERAGE(R72:R76)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F48">
+        <f>AVERAGE(S72:S76)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G48">
+        <f>AVERAGE(T72:T76)</f>
+        <v>26.6</v>
+      </c>
+      <c r="H48">
+        <f>AVERAGE(U72:U76)</f>
+        <v>317.60000000000002</v>
+      </c>
+      <c r="N48" s="11"/>
+      <c r="O48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N48" s="8">
-        <v>1</v>
-      </c>
-      <c r="O48" s="8">
-        <v>1</v>
-      </c>
       <c r="P48" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="8">
+        <v>1</v>
+      </c>
+      <c r="R48" s="8">
+        <v>2</v>
+      </c>
+      <c r="S48" s="8">
         <v>18</v>
       </c>
-      <c r="R48" s="8">
+      <c r="T48" s="8">
         <v>106</v>
       </c>
-      <c r="S48" s="8">
+      <c r="U48" s="8">
         <v>1165</v>
       </c>
     </row>
-    <row r="49" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L49" s="11"/>
-      <c r="M49" s="2" t="s">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49">
+        <f>AVERAGE(P77:P81)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D49">
+        <f>AVERAGE(Q77:Q81)</f>
+        <v>1.2</v>
+      </c>
+      <c r="E49">
+        <f>AVERAGE(R77:R81)</f>
+        <v>5.4</v>
+      </c>
+      <c r="F49">
+        <f>AVERAGE(S77:S81)</f>
+        <v>3.4</v>
+      </c>
+      <c r="G49">
+        <f>AVERAGE(T77:T81)</f>
+        <v>74.599999999999994</v>
+      </c>
+      <c r="H49">
+        <f>AVERAGE(U77:U81)</f>
+        <v>1426.6</v>
+      </c>
+      <c r="N49" s="11"/>
+      <c r="O49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N49" s="8">
-        <v>1</v>
-      </c>
-      <c r="O49" s="8">
-        <v>1</v>
-      </c>
       <c r="P49" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="8">
+        <v>1</v>
+      </c>
+      <c r="R49" s="8">
+        <v>2</v>
+      </c>
+      <c r="S49" s="8">
         <v>16</v>
       </c>
-      <c r="R49" s="8">
+      <c r="T49" s="8">
         <v>105</v>
       </c>
-      <c r="S49" s="8">
+      <c r="U49" s="8">
         <v>1178</v>
       </c>
     </row>
-    <row r="50" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L50" s="11"/>
-      <c r="M50" s="2" t="s">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50">
+        <f>AVERAGE(P82:P86)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D50">
+        <f>AVERAGE(Q82:Q86)</f>
+        <v>1.4</v>
+      </c>
+      <c r="E50">
+        <f>AVERAGE(R82:R86)</f>
+        <v>1.6</v>
+      </c>
+      <c r="F50">
+        <f>AVERAGE(S82:S86)</f>
+        <v>3.2</v>
+      </c>
+      <c r="G50">
+        <f>AVERAGE(T82:T86)</f>
+        <v>29.6</v>
+      </c>
+      <c r="H50">
+        <f>AVERAGE(U82:U86)</f>
+        <v>317.8</v>
+      </c>
+      <c r="N50" s="11"/>
+      <c r="O50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N50" s="8">
-        <v>1</v>
-      </c>
-      <c r="O50" s="8">
-        <v>1</v>
-      </c>
       <c r="P50" s="8">
         <v>1</v>
       </c>
       <c r="Q50" s="8">
+        <v>1</v>
+      </c>
+      <c r="R50" s="8">
+        <v>1</v>
+      </c>
+      <c r="S50" s="8">
         <v>10</v>
       </c>
-      <c r="R50" s="8">
+      <c r="T50" s="8">
         <v>107</v>
       </c>
-      <c r="S50" s="8">
+      <c r="U50" s="8">
         <v>1176</v>
       </c>
     </row>
-    <row r="51" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L51" s="12"/>
-      <c r="M51" s="4" t="s">
+    <row r="51" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N51" s="12"/>
+      <c r="O51" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N51" s="5">
-        <v>1</v>
-      </c>
-      <c r="O51" s="5">
-        <v>1</v>
-      </c>
       <c r="P51" s="5">
         <v>1</v>
       </c>
       <c r="Q51" s="5">
+        <v>1</v>
+      </c>
+      <c r="R51" s="5">
+        <v>1</v>
+      </c>
+      <c r="S51" s="5">
         <v>9</v>
       </c>
-      <c r="R51" s="5">
+      <c r="T51" s="5">
         <v>103</v>
       </c>
-      <c r="S51" s="5">
+      <c r="U51" s="5">
         <v>1185</v>
       </c>
     </row>
-    <row r="52" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L52" s="10" t="s">
+    <row r="52" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N52" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M52" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N52" s="7">
-        <v>1</v>
-      </c>
-      <c r="O52" s="7">
+      <c r="O52" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P52" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>2</v>
+      </c>
+      <c r="R52" s="7">
         <v>3</v>
       </c>
-      <c r="Q52" s="7">
+      <c r="S52" s="7">
         <v>6</v>
       </c>
-      <c r="R52" s="7">
+      <c r="T52" s="7">
         <v>17</v>
       </c>
-      <c r="S52" s="7">
+      <c r="U52" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L53" s="11"/>
-      <c r="M53" s="2" t="s">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N53" s="11"/>
+      <c r="O53" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N53" s="8">
-        <v>1</v>
-      </c>
-      <c r="O53" s="8">
+      <c r="P53" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="8">
         <v>0</v>
       </c>
-      <c r="P53" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q53" s="8">
-        <v>2</v>
-      </c>
       <c r="R53" s="8">
+        <v>2</v>
+      </c>
+      <c r="S53" s="8">
+        <v>2</v>
+      </c>
+      <c r="T53" s="8">
         <v>11</v>
       </c>
-      <c r="S53" s="8">
+      <c r="U53" s="8">
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L54" s="11"/>
-      <c r="M54" s="2" t="s">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N54" s="11"/>
+      <c r="O54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N54" s="8">
+      <c r="P54" s="8">
         <v>0</v>
       </c>
-      <c r="O54" s="8">
+      <c r="Q54" s="8">
         <v>4</v>
       </c>
-      <c r="P54" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="8">
-        <v>1</v>
-      </c>
       <c r="R54" s="8">
+        <v>1</v>
+      </c>
+      <c r="S54" s="8">
+        <v>1</v>
+      </c>
+      <c r="T54" s="8">
         <v>3</v>
       </c>
-      <c r="S54" s="8">
+      <c r="U54" s="8">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L55" s="11"/>
-      <c r="M55" s="2" t="s">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N55" s="11"/>
+      <c r="O55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N55" s="8">
-        <v>1</v>
-      </c>
-      <c r="O55" s="8">
-        <v>1</v>
-      </c>
       <c r="P55" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q55" s="8">
+        <v>1</v>
+      </c>
+      <c r="R55" s="8">
+        <v>2</v>
+      </c>
+      <c r="S55" s="8">
         <v>0</v>
       </c>
-      <c r="R55" s="8">
-        <v>2</v>
-      </c>
-      <c r="S55" s="8">
+      <c r="T55" s="8">
+        <v>2</v>
+      </c>
+      <c r="U55" s="8">
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L56" s="12"/>
-      <c r="M56" s="4" t="s">
+    <row r="56" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N56" s="12"/>
+      <c r="O56" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N56" s="5">
-        <v>1</v>
-      </c>
-      <c r="O56" s="5">
+      <c r="P56" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="5">
         <v>0</v>
       </c>
-      <c r="P56" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q56" s="5">
-        <v>1</v>
-      </c>
       <c r="R56" s="5">
         <v>2</v>
       </c>
       <c r="S56" s="5">
+        <v>1</v>
+      </c>
+      <c r="T56" s="5">
+        <v>2</v>
+      </c>
+      <c r="U56" s="5">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L57" s="10" t="s">
+    <row r="57" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N57" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M57" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N57" s="7">
-        <v>1</v>
-      </c>
-      <c r="O57" s="7">
+      <c r="O57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P57" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="7">
         <v>4</v>
       </c>
-      <c r="P57" s="7">
+      <c r="R57" s="7">
         <v>3</v>
       </c>
-      <c r="Q57" s="7">
+      <c r="S57" s="7">
         <v>3</v>
       </c>
-      <c r="R57" s="7">
+      <c r="T57" s="7">
         <v>9</v>
       </c>
-      <c r="S57" s="8">
+      <c r="U57" s="8">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L58" s="11"/>
-      <c r="M58" s="2" t="s">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N58" s="11"/>
+      <c r="O58" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N58" s="8">
-        <v>1</v>
-      </c>
-      <c r="O58" s="8">
-        <v>1</v>
-      </c>
       <c r="P58" s="8">
         <v>1</v>
       </c>
       <c r="Q58" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R58" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S58" s="8">
+        <v>2</v>
+      </c>
+      <c r="T58" s="8">
+        <v>2</v>
+      </c>
+      <c r="U58" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L59" s="11"/>
-      <c r="M59" s="2" t="s">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N59" s="11"/>
+      <c r="O59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N59" s="8">
-        <v>1</v>
-      </c>
-      <c r="O59" s="8">
+      <c r="P59" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="8">
         <v>0</v>
       </c>
-      <c r="P59" s="8">
+      <c r="R59" s="8">
         <v>4</v>
       </c>
-      <c r="Q59" s="8">
-        <v>1</v>
-      </c>
-      <c r="R59" s="8">
-        <v>2</v>
-      </c>
       <c r="S59" s="8">
+        <v>1</v>
+      </c>
+      <c r="T59" s="8">
+        <v>2</v>
+      </c>
+      <c r="U59" s="8">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L60" s="11"/>
-      <c r="M60" s="2" t="s">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N60" s="11"/>
+      <c r="O60" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N60" s="8">
-        <v>1</v>
-      </c>
-      <c r="O60" s="8">
+      <c r="P60" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="8">
         <v>0</v>
       </c>
-      <c r="P60" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q60" s="8">
-        <v>1</v>
-      </c>
       <c r="R60" s="8">
         <v>1</v>
       </c>
       <c r="S60" s="8">
+        <v>1</v>
+      </c>
+      <c r="T60" s="8">
+        <v>1</v>
+      </c>
+      <c r="U60" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L61" s="12"/>
-      <c r="M61" s="4" t="s">
+    <row r="61" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N61" s="12"/>
+      <c r="O61" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N61" s="5">
-        <v>1</v>
-      </c>
-      <c r="O61" s="5">
+      <c r="P61" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="5">
         <v>0</v>
       </c>
-      <c r="P61" s="5">
+      <c r="R61" s="5">
         <v>0</v>
       </c>
-      <c r="Q61" s="5">
-        <v>1</v>
-      </c>
-      <c r="R61" s="5">
-        <v>2</v>
-      </c>
       <c r="S61" s="5">
+        <v>1</v>
+      </c>
+      <c r="T61" s="5">
+        <v>2</v>
+      </c>
+      <c r="U61" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L62" s="10" t="s">
+    <row r="62" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N62" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M62" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N62" s="7">
-        <v>1</v>
-      </c>
-      <c r="O62" s="7">
+      <c r="O62" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P62" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="7">
         <v>4</v>
       </c>
-      <c r="P62" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="7">
+      <c r="R62" s="7">
+        <v>1</v>
+      </c>
+      <c r="S62" s="7">
         <v>3</v>
       </c>
-      <c r="R62" s="7">
+      <c r="T62" s="7">
         <v>6</v>
       </c>
-      <c r="S62" s="8">
+      <c r="U62" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L63" s="11"/>
-      <c r="M63" s="2" t="s">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N63" s="11"/>
+      <c r="O63" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="N63" s="8">
-        <v>1</v>
-      </c>
-      <c r="O63" s="8">
-        <v>0</v>
       </c>
       <c r="P63" s="8">
         <v>1</v>
@@ -4755,23 +4753,23 @@
         <v>0</v>
       </c>
       <c r="R63" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S63" s="8">
+        <v>0</v>
+      </c>
+      <c r="T63" s="8">
+        <v>2</v>
+      </c>
+      <c r="U63" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L64" s="11"/>
-      <c r="M64" s="2" t="s">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="N64" s="11"/>
+      <c r="O64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N64" s="8">
-        <v>1</v>
-      </c>
-      <c r="O64" s="8">
-        <v>1</v>
-      </c>
       <c r="P64" s="8">
         <v>1</v>
       </c>
@@ -4779,23 +4777,23 @@
         <v>1</v>
       </c>
       <c r="R64" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S64" s="8">
+        <v>1</v>
+      </c>
+      <c r="T64" s="8">
+        <v>2</v>
+      </c>
+      <c r="U64" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L65" s="11"/>
-      <c r="M65" s="2" t="s">
+    <row r="65" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N65" s="11"/>
+      <c r="O65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N65" s="8">
-        <v>1</v>
-      </c>
-      <c r="O65" s="8">
-        <v>1</v>
-      </c>
       <c r="P65" s="8">
         <v>1</v>
       </c>
@@ -4806,22 +4804,22 @@
         <v>1</v>
       </c>
       <c r="S65" s="8">
+        <v>1</v>
+      </c>
+      <c r="T65" s="8">
+        <v>1</v>
+      </c>
+      <c r="U65" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L66" s="12"/>
-      <c r="M66" s="4" t="s">
+    <row r="66" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N66" s="12"/>
+      <c r="O66" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N66" s="5">
+      <c r="P66" s="5">
         <v>0</v>
-      </c>
-      <c r="O66" s="5">
-        <v>0</v>
-      </c>
-      <c r="P66" s="5">
-        <v>1</v>
       </c>
       <c r="Q66" s="5">
         <v>0</v>
@@ -4830,522 +4828,528 @@
         <v>1</v>
       </c>
       <c r="S66" s="5">
+        <v>0</v>
+      </c>
+      <c r="T66" s="5">
+        <v>1</v>
+      </c>
+      <c r="U66" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L67" s="10" t="s">
+    <row r="67" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N67" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M67" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N67" s="7">
-        <v>1</v>
-      </c>
-      <c r="O67" s="7">
+      <c r="O67" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P67" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="7">
+        <v>2</v>
+      </c>
+      <c r="R67" s="7">
         <v>11</v>
       </c>
-      <c r="Q67" s="7">
+      <c r="S67" s="7">
         <v>20</v>
       </c>
-      <c r="R67" s="7">
+      <c r="T67" s="7">
         <v>167</v>
       </c>
-      <c r="S67" s="8">
+      <c r="U67" s="8">
         <v>1387</v>
       </c>
     </row>
-    <row r="68" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L68" s="11"/>
-      <c r="M68" s="2" t="s">
+    <row r="68" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N68" s="11"/>
+      <c r="O68" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N68" s="8">
-        <v>1</v>
-      </c>
-      <c r="O68" s="8">
-        <v>1</v>
-      </c>
       <c r="P68" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q68" s="8">
+        <v>1</v>
+      </c>
+      <c r="R68" s="8">
+        <v>2</v>
+      </c>
+      <c r="S68" s="8">
         <v>13</v>
       </c>
-      <c r="R68" s="8">
+      <c r="T68" s="8">
         <v>132</v>
       </c>
-      <c r="S68" s="8">
+      <c r="U68" s="8">
         <v>1183</v>
       </c>
     </row>
-    <row r="69" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L69" s="11"/>
-      <c r="M69" s="2" t="s">
+    <row r="69" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N69" s="11"/>
+      <c r="O69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N69" s="8">
-        <v>1</v>
-      </c>
-      <c r="O69" s="8">
-        <v>1</v>
-      </c>
       <c r="P69" s="8">
         <v>1</v>
       </c>
       <c r="Q69" s="8">
+        <v>1</v>
+      </c>
+      <c r="R69" s="8">
+        <v>1</v>
+      </c>
+      <c r="S69" s="8">
         <v>11</v>
       </c>
-      <c r="R69" s="8">
+      <c r="T69" s="8">
         <v>141</v>
       </c>
-      <c r="S69" s="8">
+      <c r="U69" s="8">
         <v>1344</v>
       </c>
     </row>
-    <row r="70" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L70" s="11"/>
-      <c r="M70" s="2" t="s">
+    <row r="70" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N70" s="11"/>
+      <c r="O70" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N70" s="8">
-        <v>1</v>
-      </c>
-      <c r="O70" s="8">
-        <v>1</v>
-      </c>
       <c r="P70" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q70" s="8">
+        <v>1</v>
+      </c>
+      <c r="R70" s="8">
+        <v>2</v>
+      </c>
+      <c r="S70" s="8">
         <v>10</v>
       </c>
-      <c r="R70" s="8">
+      <c r="T70" s="8">
         <v>134</v>
       </c>
-      <c r="S70" s="8">
+      <c r="U70" s="8">
         <v>1384</v>
       </c>
     </row>
-    <row r="71" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L71" s="12"/>
-      <c r="M71" s="4" t="s">
+    <row r="71" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N71" s="12"/>
+      <c r="O71" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N71" s="5">
+      <c r="P71" s="5">
         <v>0</v>
       </c>
-      <c r="O71" s="5">
-        <v>1</v>
-      </c>
-      <c r="P71" s="5">
-        <v>2</v>
-      </c>
       <c r="Q71" s="5">
+        <v>1</v>
+      </c>
+      <c r="R71" s="5">
+        <v>2</v>
+      </c>
+      <c r="S71" s="5">
         <v>10</v>
       </c>
-      <c r="R71" s="5">
+      <c r="T71" s="5">
         <v>139</v>
       </c>
-      <c r="S71" s="5">
+      <c r="U71" s="5">
         <v>1373</v>
       </c>
     </row>
-    <row r="72" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L72" s="10" t="s">
+    <row r="72" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N72" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M72" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N72" s="7">
-        <v>1</v>
-      </c>
-      <c r="O72" s="7">
+      <c r="O72" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P72" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="7">
+        <v>2</v>
+      </c>
+      <c r="R72" s="7">
         <v>6</v>
       </c>
-      <c r="Q72" s="7">
+      <c r="S72" s="7">
         <v>8</v>
       </c>
-      <c r="R72" s="7">
+      <c r="T72" s="7">
         <v>35</v>
       </c>
-      <c r="S72" s="8">
+      <c r="U72" s="8">
         <v>319</v>
       </c>
     </row>
-    <row r="73" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L73" s="11"/>
-      <c r="M73" s="2" t="s">
+    <row r="73" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N73" s="11"/>
+      <c r="O73" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N73" s="8">
-        <v>1</v>
-      </c>
-      <c r="O73" s="8">
-        <v>1</v>
-      </c>
       <c r="P73" s="8">
         <v>1</v>
       </c>
       <c r="Q73" s="8">
+        <v>1</v>
+      </c>
+      <c r="R73" s="8">
+        <v>1</v>
+      </c>
+      <c r="S73" s="8">
         <v>8</v>
       </c>
-      <c r="R73" s="8">
+      <c r="T73" s="8">
         <v>33</v>
       </c>
-      <c r="S73" s="8">
+      <c r="U73" s="8">
         <v>310</v>
       </c>
     </row>
-    <row r="74" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L74" s="11"/>
-      <c r="M74" s="2" t="s">
+    <row r="74" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N74" s="11"/>
+      <c r="O74" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N74" s="8">
+      <c r="P74" s="8">
         <v>0</v>
       </c>
-      <c r="O74" s="8">
-        <v>1</v>
-      </c>
-      <c r="P74" s="8">
-        <v>1</v>
-      </c>
       <c r="Q74" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R74" s="8">
+        <v>1</v>
+      </c>
+      <c r="S74" s="8">
+        <v>2</v>
+      </c>
+      <c r="T74" s="8">
         <v>18</v>
       </c>
-      <c r="S74" s="8">
+      <c r="U74" s="8">
         <v>350</v>
       </c>
     </row>
-    <row r="75" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L75" s="11"/>
-      <c r="M75" s="2" t="s">
+    <row r="75" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N75" s="11"/>
+      <c r="O75" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N75" s="8">
-        <v>1</v>
-      </c>
-      <c r="O75" s="8">
-        <v>1</v>
-      </c>
       <c r="P75" s="8">
         <v>1</v>
       </c>
       <c r="Q75" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R75" s="8">
+        <v>1</v>
+      </c>
+      <c r="S75" s="8">
+        <v>2</v>
+      </c>
+      <c r="T75" s="8">
         <v>18</v>
       </c>
-      <c r="S75" s="8">
+      <c r="U75" s="8">
         <v>306</v>
       </c>
     </row>
-    <row r="76" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L76" s="12"/>
-      <c r="M76" s="4" t="s">
+    <row r="76" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N76" s="12"/>
+      <c r="O76" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N76" s="5">
-        <v>1</v>
-      </c>
-      <c r="O76" s="5">
-        <v>1</v>
-      </c>
       <c r="P76" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q76" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R76" s="5">
+        <v>2</v>
+      </c>
+      <c r="S76" s="5">
+        <v>2</v>
+      </c>
+      <c r="T76" s="5">
         <v>29</v>
       </c>
-      <c r="S76" s="5">
+      <c r="U76" s="5">
         <v>303</v>
       </c>
     </row>
-    <row r="77" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L77" s="10" t="s">
+    <row r="77" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N77" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M77" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N77" s="7">
-        <v>1</v>
-      </c>
-      <c r="O77" s="7">
+      <c r="O77" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P77" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q77" s="7">
         <v>4</v>
       </c>
-      <c r="P77" s="7">
+      <c r="R77" s="7">
         <v>5</v>
       </c>
-      <c r="Q77" s="7">
+      <c r="S77" s="7">
         <v>6</v>
       </c>
-      <c r="R77" s="7">
+      <c r="T77" s="7">
         <v>75</v>
       </c>
-      <c r="S77" s="8">
+      <c r="U77" s="8">
         <v>1438</v>
       </c>
     </row>
-    <row r="78" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L78" s="11"/>
-      <c r="M78" s="2" t="s">
+    <row r="78" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N78" s="11"/>
+      <c r="O78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N78" s="8">
-        <v>1</v>
-      </c>
-      <c r="O78" s="8">
+      <c r="P78" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="8">
         <v>0</v>
       </c>
-      <c r="P78" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q78" s="8">
+      <c r="R78" s="8">
+        <v>2</v>
+      </c>
+      <c r="S78" s="8">
         <v>6</v>
       </c>
-      <c r="R78" s="8">
+      <c r="T78" s="8">
         <v>99</v>
       </c>
-      <c r="S78" s="8">
+      <c r="U78" s="8">
         <v>1419</v>
       </c>
     </row>
-    <row r="79" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L79" s="11"/>
-      <c r="M79" s="2" t="s">
+    <row r="79" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N79" s="11"/>
+      <c r="O79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N79" s="8">
-        <v>1</v>
-      </c>
-      <c r="O79" s="8">
-        <v>1</v>
-      </c>
       <c r="P79" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q79" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R79" s="8">
+        <v>2</v>
+      </c>
+      <c r="S79" s="8">
+        <v>2</v>
+      </c>
+      <c r="T79" s="8">
         <v>90</v>
       </c>
-      <c r="S79" s="8">
+      <c r="U79" s="8">
         <v>1445</v>
       </c>
     </row>
-    <row r="80" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L80" s="11"/>
-      <c r="M80" s="2" t="s">
+    <row r="80" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N80" s="11"/>
+      <c r="O80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N80" s="8">
-        <v>1</v>
-      </c>
-      <c r="O80" s="8">
-        <v>1</v>
-      </c>
       <c r="P80" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="8">
+        <v>1</v>
+      </c>
+      <c r="R80" s="8">
         <v>8</v>
       </c>
-      <c r="Q80" s="8">
-        <v>1</v>
-      </c>
-      <c r="R80" s="8">
+      <c r="S80" s="8">
+        <v>1</v>
+      </c>
+      <c r="T80" s="8">
         <v>57</v>
       </c>
-      <c r="S80" s="8">
+      <c r="U80" s="8">
         <v>1416</v>
       </c>
     </row>
-    <row r="81" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L81" s="12"/>
-      <c r="M81" s="4" t="s">
+    <row r="81" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N81" s="12"/>
+      <c r="O81" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N81" s="5">
+      <c r="P81" s="5">
         <v>0</v>
       </c>
-      <c r="O81" s="5">
+      <c r="Q81" s="5">
         <v>0</v>
       </c>
-      <c r="P81" s="5">
+      <c r="R81" s="5">
         <v>10</v>
       </c>
-      <c r="Q81" s="5">
-        <v>2</v>
-      </c>
-      <c r="R81" s="5">
+      <c r="S81" s="5">
+        <v>2</v>
+      </c>
+      <c r="T81" s="5">
         <v>52</v>
       </c>
-      <c r="S81" s="5">
+      <c r="U81" s="5">
         <v>1415</v>
       </c>
     </row>
-    <row r="82" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L82" s="10" t="s">
+    <row r="82" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="N82" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M82" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N82" s="7">
-        <v>2</v>
-      </c>
-      <c r="O82" s="7">
+      <c r="O82" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P82" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q82" s="7">
         <v>4</v>
       </c>
-      <c r="P82" s="7">
+      <c r="R82" s="7">
         <v>3</v>
       </c>
-      <c r="Q82" s="7">
+      <c r="S82" s="7">
         <v>6</v>
       </c>
-      <c r="R82" s="7">
+      <c r="T82" s="7">
         <v>40</v>
       </c>
-      <c r="S82" s="8">
+      <c r="U82" s="8">
         <v>322</v>
       </c>
     </row>
-    <row r="83" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L83" s="11"/>
-      <c r="M83" s="2" t="s">
+    <row r="83" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N83" s="11"/>
+      <c r="O83" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N83" s="8">
-        <v>1</v>
-      </c>
-      <c r="O83" s="8">
+      <c r="P83" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="8">
         <v>0</v>
       </c>
-      <c r="P83" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q83" s="8">
+      <c r="R83" s="8">
+        <v>2</v>
+      </c>
+      <c r="S83" s="8">
         <v>4</v>
       </c>
-      <c r="R83" s="8">
+      <c r="T83" s="8">
         <v>42</v>
       </c>
-      <c r="S83" s="8">
+      <c r="U83" s="8">
         <v>359</v>
       </c>
     </row>
-    <row r="84" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L84" s="11"/>
-      <c r="M84" s="2" t="s">
+    <row r="84" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N84" s="11"/>
+      <c r="O84" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N84" s="8">
+      <c r="P84" s="8">
         <v>0</v>
       </c>
-      <c r="O84" s="8">
-        <v>1</v>
-      </c>
-      <c r="P84" s="8">
-        <v>1</v>
-      </c>
       <c r="Q84" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R84" s="8">
+        <v>1</v>
+      </c>
+      <c r="S84" s="8">
+        <v>2</v>
+      </c>
+      <c r="T84" s="8">
         <v>23</v>
       </c>
-      <c r="S84" s="8">
+      <c r="U84" s="8">
         <v>300</v>
       </c>
     </row>
-    <row r="85" spans="12:19" x14ac:dyDescent="0.35">
-      <c r="L85" s="11"/>
-      <c r="M85" s="2" t="s">
+    <row r="85" spans="14:21" x14ac:dyDescent="0.35">
+      <c r="N85" s="11"/>
+      <c r="O85" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N85" s="8">
-        <v>1</v>
-      </c>
-      <c r="O85" s="8">
-        <v>1</v>
-      </c>
       <c r="P85" s="8">
         <v>1</v>
       </c>
       <c r="Q85" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R85" s="8">
+        <v>1</v>
+      </c>
+      <c r="S85" s="8">
+        <v>2</v>
+      </c>
+      <c r="T85" s="8">
         <v>21</v>
       </c>
-      <c r="S85" s="8">
+      <c r="U85" s="8">
         <v>301</v>
       </c>
     </row>
-    <row r="86" spans="12:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L86" s="12"/>
-      <c r="M86" s="4" t="s">
+    <row r="86" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N86" s="12"/>
+      <c r="O86" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N86" s="5">
+      <c r="P86" s="5">
         <v>0</v>
       </c>
-      <c r="O86" s="5">
-        <v>1</v>
-      </c>
-      <c r="P86" s="5">
-        <v>1</v>
-      </c>
       <c r="Q86" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R86" s="5">
+        <v>1</v>
+      </c>
+      <c r="S86" s="5">
+        <v>2</v>
+      </c>
+      <c r="T86" s="5">
         <v>22</v>
       </c>
-      <c r="S86" s="5">
+      <c r="U86" s="5">
         <v>307</v>
       </c>
     </row>
-    <row r="87" spans="12:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N87" s="8"/>
+    <row r="87" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="P87" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="L72:L76"/>
-    <mergeCell ref="L77:L81"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="N72:N76"/>
+    <mergeCell ref="N77:N81"/>
     <mergeCell ref="B1:B4"/>
-    <mergeCell ref="L82:L86"/>
-    <mergeCell ref="L32:L36"/>
+    <mergeCell ref="N82:N86"/>
+    <mergeCell ref="N32:N36"/>
     <mergeCell ref="D1:I2"/>
-    <mergeCell ref="L52:L56"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="L17:L21"/>
-    <mergeCell ref="L27:L31"/>
-    <mergeCell ref="L37:L41"/>
-    <mergeCell ref="L42:L46"/>
-    <mergeCell ref="L47:L51"/>
-    <mergeCell ref="L12:L16"/>
-    <mergeCell ref="L22:L26"/>
-    <mergeCell ref="L57:L61"/>
-    <mergeCell ref="L62:L66"/>
-    <mergeCell ref="L67:L71"/>
+    <mergeCell ref="N52:N56"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="N7:N11"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="N27:N31"/>
+    <mergeCell ref="N37:N41"/>
+    <mergeCell ref="N42:N46"/>
+    <mergeCell ref="N47:N51"/>
+    <mergeCell ref="N12:N16"/>
+    <mergeCell ref="N22:N26"/>
+    <mergeCell ref="N57:N61"/>
+    <mergeCell ref="N62:N66"/>
+    <mergeCell ref="N67:N71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Use colors and dashed to improve legibility
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACD9A8F-D275-4F92-A22B-825CC485E123}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D88AF-A37A-4A17-98EF-F0616623EB8E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
   <si>
     <t>Input Size</t>
   </si>
@@ -113,6 +113,9 @@
       </rPr>
       <t>Input Size</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -334,10 +337,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -421,10 +425,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -508,10 +513,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -595,10 +601,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -682,10 +689,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
+              <a:prstDash val="dashDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -769,7 +777,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -856,12 +864,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -945,7 +954,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
@@ -1034,12 +1043,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1123,12 +1131,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd" cmpd="sng">
               <a:solidFill>
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1212,12 +1222,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1301,12 +1310,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1390,13 +1398,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1480,13 +1486,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1570,13 +1574,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1660,13 +1665,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1801,9 +1804,10 @@
       <c:valAx>
         <c:axId val="1687913903"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="18000"/>
+          <c:max val="4096"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1855,6 +1859,7 @@
         <c:crossAx val="1555000431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2835,8 +2840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:H50"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3560,6 +3565,9 @@
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
+      <c r="K33" t="s">
+        <v>25</v>
+      </c>
       <c r="N33" s="11"/>
       <c r="O33" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Use shapes in lines for legibility
Also significantly increase image resolution.
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D88AF-A37A-4A17-98EF-F0616623EB8E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B86E176-BE14-4FE9-B444-879353AD7C3B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -319,8 +320,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -337,18 +339,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -403,10 +402,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000000-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -425,18 +423,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -491,10 +486,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000001-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -513,18 +507,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -579,10 +570,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000002-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -601,18 +591,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -667,10 +654,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000003-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -689,18 +675,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:prstDash val="dashDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -755,10 +738,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000004-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -777,17 +759,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -842,10 +822,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000005-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -864,20 +843,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -932,10 +908,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000006-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -954,19 +929,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1021,10 +994,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000007-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1043,18 +1015,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1109,10 +1080,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000008-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1131,21 +1101,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1200,10 +1166,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{00000009-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1222,18 +1187,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1288,10 +1252,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{0000000A-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1310,18 +1273,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1376,10 +1338,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{0000000B-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1398,18 +1359,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1464,10 +1425,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{0000000C-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1486,18 +1446,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1552,10 +1512,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{0000000D-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1574,21 +1533,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1643,10 +1599,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{0000000E-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1665,18 +1620,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$34:$H$34</c:f>
@@ -1731,10 +1686,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+              <c16:uniqueId val="{0000000F-ABC6-411A-AD40-69D26F8115C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1746,12 +1700,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1555000431"/>
-        <c:axId val="1687913903"/>
-      </c:lineChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1559801535"/>
+        <c:axId val="1689482207"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="1555000431"/>
+        <c:axId val="1559801535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1749,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1687913903"/>
+        <c:crossAx val="1689482207"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1802,12 +1757,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1687913903"/>
+        <c:axId val="1689482207"/>
         <c:scaling>
-          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="4096"/>
-          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1856,10 +1808,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1555000431"/>
+        <c:crossAx val="1559801535"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1936,6 +1887,2036 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sorting Algorithm Times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$35:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4253.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heap Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$36:$H$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3546.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$37:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17240.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Comb Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$H$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>171.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048.1999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$39:$H$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1888.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$40:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>232.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3327.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$41:$H$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>122.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1352.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dot"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$42:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3308.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Java Default Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$43:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1187.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trump Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$44:$H$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bernie Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$45:$H$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hillary Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$46:$H$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Radix Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$47:$H$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>142.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1334.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bucket Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:prstDash val="lgDashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$48:$H$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>317.60000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Counting Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$49:$H$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1426.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pigeonhole Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$H$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>317.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-DD9C-4830-A7DD-7E3CEC8F7B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1555000431"/>
+        <c:axId val="1687913903"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1555000431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Inputs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1687913903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1687913903"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="4096"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1555000431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1984,8 +3965,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2093,11 +4114,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2108,11 +4124,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2144,9 +4155,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2500,7 +4508,572 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AB8D0AEB-B40B-41D5-A467-12EBB43F2672}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="84" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8655655" cy="6281964"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B6E91A4-DE7D-4C15-850C-8F8ED4A31A8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2512,8 +5085,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2840,8 +5413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add data for Slow Sort
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A271C84E-00CB-4362-B8D5-F483E1A9F127}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF33905-746D-48E9-B9A6-935D2C1DD833}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -248,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -286,6 +286,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2518,15 +2519,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:P11"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7265625" customWidth="1"/>
+    <col min="17" max="21" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2610,15 +2612,27 @@
       <c r="N7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
+      <c r="O7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C8">
@@ -2646,60 +2660,108 @@
         <v>10000000</v>
       </c>
       <c r="N8" s="16"/>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
+      <c r="P8" s="3">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="N9" s="16"/>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
+      <c r="P9" s="8">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="16"/>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
+      <c r="P10" s="8">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="N11" s="17"/>
-      <c r="O11" s="8" t="s">
+      <c r="O11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="P11" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
@@ -2708,75 +2770,75 @@
       <c r="N12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="O12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
+      <c r="O12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="N13" s="16"/>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="N14" s="16"/>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="N15" s="16"/>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
     </row>
     <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="N16" s="17"/>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
     </row>
     <row r="17" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -2785,75 +2847,75 @@
       <c r="N17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
+      <c r="O17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="N18" s="16"/>
-      <c r="O18" s="3" t="s">
+      <c r="O18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="N19" s="16"/>
-      <c r="O19" s="3" t="s">
+      <c r="O19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="N20" s="16"/>
-      <c r="O20" s="8" t="s">
+      <c r="O20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
     </row>
     <row r="21" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="N21" s="17"/>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
     </row>
     <row r="22" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -3237,10 +3299,10 @@
       <c r="O37" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
     </row>
@@ -3249,10 +3311,10 @@
       <c r="O38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
     </row>
@@ -3261,10 +3323,10 @@
       <c r="O39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
     </row>
@@ -3273,10 +3335,10 @@
       <c r="O40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
     </row>
@@ -3285,12 +3347,12 @@
       <c r="O41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
     </row>
     <row r="42" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N42" s="18" t="s">
@@ -3299,10 +3361,10 @@
       <c r="O42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
     </row>
@@ -3311,10 +3373,10 @@
       <c r="O43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
     </row>
@@ -3323,10 +3385,10 @@
       <c r="O44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
     </row>
@@ -3335,10 +3397,10 @@
       <c r="O45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
     </row>
@@ -3347,12 +3409,12 @@
       <c r="O46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
     </row>
     <row r="47" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N47" s="18" t="s">
@@ -4093,18 +4155,33 @@
       <c r="N77" s="18" t="s">
         <v>31</v>
       </c>
+      <c r="O77" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="78" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N78" s="16"/>
+      <c r="O78" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="79" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N79" s="16"/>
+      <c r="O79" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="80" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N80" s="16"/>
+      <c r="O80" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N81" s="17"/>
+      <c r="O81" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="82" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N82" s="18" t="s">

</xml_diff>

<commit_message>
Add Data for CycleSort
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF33905-746D-48E9-B9A6-935D2C1DD833}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEAFBDE-1FA7-4FCD-9509-6BF827F06089}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2773,12 +2773,24 @@
       <c r="O12" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
+      <c r="P12" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>159</v>
+      </c>
+      <c r="R12" s="8">
+        <v>113354</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
@@ -2788,12 +2800,24 @@
       <c r="O13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
+      <c r="P13" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>220</v>
+      </c>
+      <c r="R13" s="8">
+        <v>155473</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
@@ -2803,12 +2827,24 @@
       <c r="O14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+      <c r="P14" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>226</v>
+      </c>
+      <c r="R14" s="8">
+        <v>153142</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
@@ -2818,12 +2854,24 @@
       <c r="O15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
+      <c r="P15" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>228</v>
+      </c>
+      <c r="R15" s="8">
+        <v>147810</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
@@ -2833,12 +2881,24 @@
       <c r="O16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
+      <c r="P16" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>223</v>
+      </c>
+      <c r="R16" s="5">
+        <v>149324</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">

</xml_diff>

<commit_message>
Data for Cycle Sort
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6ACAAB-FC38-4C57-9162-80E2621B217D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846BD69E-F4B5-41D6-BA53-76207CBEC1DC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2773,6 +2773,24 @@
       <c r="O12" s="19" t="s">
         <v>2</v>
       </c>
+      <c r="P12" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>9</v>
+      </c>
+      <c r="R12">
+        <v>277</v>
+      </c>
+      <c r="S12">
+        <v>26488</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
@@ -2782,6 +2800,24 @@
       <c r="O13" s="19" t="s">
         <v>3</v>
       </c>
+      <c r="P13" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="R13">
+        <v>258</v>
+      </c>
+      <c r="S13">
+        <v>26815</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
@@ -2791,6 +2827,24 @@
       <c r="O14" s="19" t="s">
         <v>4</v>
       </c>
+      <c r="P14" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>233</v>
+      </c>
+      <c r="S14">
+        <v>23822</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
@@ -2800,6 +2854,24 @@
       <c r="O15" s="19" t="s">
         <v>5</v>
       </c>
+      <c r="P15" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>234</v>
+      </c>
+      <c r="S15">
+        <v>23903</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
@@ -2809,12 +2881,24 @@
       <c r="O16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
+      <c r="P16" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>3</v>
+      </c>
+      <c r="R16" s="5">
+        <v>236</v>
+      </c>
+      <c r="S16" s="5">
+        <v>23665</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">

</xml_diff>

<commit_message>
Data for Cocktail Sort
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846BD69E-F4B5-41D6-BA53-76207CBEC1DC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8C242E-B9F2-4520-BB18-61489CC41133}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3419,60 +3419,120 @@
       <c r="O37" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
+      <c r="P37" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>8</v>
+      </c>
+      <c r="R37" s="7">
+        <v>126</v>
+      </c>
+      <c r="S37" s="7">
+        <v>13569</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="38" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N38" s="16"/>
       <c r="O38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
+      <c r="P38" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>3</v>
+      </c>
+      <c r="R38" s="8">
+        <v>109</v>
+      </c>
+      <c r="S38" s="8">
+        <v>13801</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="39" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N39" s="16"/>
       <c r="O39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
+      <c r="P39" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>2</v>
+      </c>
+      <c r="R39" s="8">
+        <v>109</v>
+      </c>
+      <c r="S39" s="8">
+        <v>12396</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="40" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N40" s="16"/>
       <c r="O40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
+      <c r="P40" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>3</v>
+      </c>
+      <c r="R40" s="8">
+        <v>113</v>
+      </c>
+      <c r="S40" s="8">
+        <v>12261</v>
+      </c>
+      <c r="T40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="41" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N41" s="17"/>
       <c r="O41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
+      <c r="P41" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>2</v>
+      </c>
+      <c r="R41" s="5">
+        <v>116</v>
+      </c>
+      <c r="S41" s="5">
+        <v>12393</v>
+      </c>
+      <c r="T41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U41" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="42" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N42" s="18" t="s">

</xml_diff>

<commit_message>
Aashish Sort 1 data
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A31EA80-60C5-4341-8288-68E5408AC316}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5E95BB-4920-4723-93E6-FC79CC22ABA3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W79" sqref="W79"/>
+    <sheetView tabSelected="1" topLeftCell="I103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U122" sqref="U122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5374,60 +5374,120 @@
       <c r="O117" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P117" s="7"/>
-      <c r="Q117" s="7"/>
-      <c r="R117" s="7"/>
-      <c r="S117" s="7"/>
-      <c r="T117" s="7"/>
-      <c r="U117" s="8"/>
+      <c r="P117" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q117" s="7">
+        <v>4</v>
+      </c>
+      <c r="R117" s="7">
+        <v>9</v>
+      </c>
+      <c r="S117" s="7">
+        <v>78</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1084</v>
+      </c>
+      <c r="U117" s="8">
+        <v>4684</v>
+      </c>
     </row>
     <row r="118" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N118" s="16"/>
       <c r="O118" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P118" s="8"/>
-      <c r="Q118" s="8"/>
-      <c r="R118" s="8"/>
-      <c r="S118" s="8"/>
-      <c r="T118" s="8"/>
-      <c r="U118" s="8"/>
+      <c r="P118" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q118" s="8">
+        <v>3</v>
+      </c>
+      <c r="R118" s="8">
+        <v>15</v>
+      </c>
+      <c r="S118" s="8">
+        <v>113</v>
+      </c>
+      <c r="T118" s="8">
+        <v>961</v>
+      </c>
+      <c r="U118" s="8">
+        <v>9842</v>
+      </c>
     </row>
     <row r="119" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N119" s="16"/>
       <c r="O119" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P119" s="8"/>
-      <c r="Q119" s="8"/>
-      <c r="R119" s="8"/>
-      <c r="S119" s="8"/>
-      <c r="T119" s="8"/>
-      <c r="U119" s="8"/>
+      <c r="P119" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q119" s="8">
+        <v>1</v>
+      </c>
+      <c r="R119" s="8">
+        <v>8</v>
+      </c>
+      <c r="S119" s="8">
+        <v>58</v>
+      </c>
+      <c r="T119" s="8">
+        <v>375</v>
+      </c>
+      <c r="U119" s="8">
+        <v>9862</v>
+      </c>
     </row>
     <row r="120" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N120" s="16"/>
       <c r="O120" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P120" s="8"/>
-      <c r="Q120" s="8"/>
-      <c r="R120" s="8"/>
-      <c r="S120" s="8"/>
-      <c r="T120" s="8"/>
-      <c r="U120" s="8"/>
+      <c r="P120" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q120" s="8">
+        <v>1</v>
+      </c>
+      <c r="R120" s="8">
+        <v>20</v>
+      </c>
+      <c r="S120" s="8">
+        <v>46</v>
+      </c>
+      <c r="T120" s="8">
+        <v>903</v>
+      </c>
+      <c r="U120" s="8">
+        <v>9694</v>
+      </c>
     </row>
     <row r="121" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N121" s="17"/>
       <c r="O121" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P121" s="5"/>
-      <c r="Q121" s="5"/>
-      <c r="R121" s="5"/>
-      <c r="S121" s="5"/>
-      <c r="T121" s="5"/>
-      <c r="U121" s="5"/>
+      <c r="P121" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q121" s="5">
+        <v>1</v>
+      </c>
+      <c r="R121" s="5">
+        <v>27</v>
+      </c>
+      <c r="S121" s="5">
+        <v>48</v>
+      </c>
+      <c r="T121" s="5">
+        <v>916</v>
+      </c>
+      <c r="U121" s="5">
+        <v>4127</v>
+      </c>
     </row>
     <row r="122" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N122" s="18" t="s">

</xml_diff>

<commit_message>
Data for Aashish Sort 2
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5E95BB-4920-4723-93E6-FC79CC22ABA3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B2643A-D924-4566-8427-7A3CF08CD377}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U122" sqref="U122"/>
+    <sheetView tabSelected="1" topLeftCell="I115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W126" sqref="W126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5496,60 +5496,120 @@
       <c r="O122" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P122" s="7"/>
-      <c r="Q122" s="7"/>
-      <c r="R122" s="7"/>
-      <c r="S122" s="7"/>
-      <c r="T122" s="7"/>
-      <c r="U122" s="8"/>
+      <c r="P122" s="7">
+        <v>7</v>
+      </c>
+      <c r="Q122" s="7">
+        <v>74</v>
+      </c>
+      <c r="R122" s="7">
+        <v>42289</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T122" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="123" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N123" s="16"/>
       <c r="O123" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P123" s="8"/>
-      <c r="Q123" s="8"/>
-      <c r="R123" s="8"/>
-      <c r="S123" s="8"/>
-      <c r="T123" s="8"/>
-      <c r="U123" s="8"/>
+      <c r="P123" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q123" s="8">
+        <v>57</v>
+      </c>
+      <c r="R123" s="8">
+        <v>43745</v>
+      </c>
+      <c r="S123" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T123" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U123" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="124" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N124" s="16"/>
       <c r="O124" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P124" s="8"/>
-      <c r="Q124" s="8"/>
-      <c r="R124" s="8"/>
-      <c r="S124" s="8"/>
-      <c r="T124" s="8"/>
-      <c r="U124" s="8"/>
+      <c r="P124" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q124" s="8">
+        <v>52</v>
+      </c>
+      <c r="R124" s="8">
+        <v>42572</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T124" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="125" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N125" s="16"/>
       <c r="O125" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P125" s="8"/>
-      <c r="Q125" s="8"/>
-      <c r="R125" s="8"/>
-      <c r="S125" s="8"/>
-      <c r="T125" s="8"/>
-      <c r="U125" s="8"/>
+      <c r="P125" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q125" s="8">
+        <v>52</v>
+      </c>
+      <c r="R125" s="8">
+        <v>42238</v>
+      </c>
+      <c r="S125" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T125" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U125" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="126" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N126" s="17"/>
       <c r="O126" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P126" s="5"/>
-      <c r="Q126" s="5"/>
-      <c r="R126" s="5"/>
-      <c r="S126" s="5"/>
-      <c r="T126" s="5"/>
-      <c r="U126" s="5"/>
+      <c r="P126" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q126" s="5">
+        <v>53</v>
+      </c>
+      <c r="R126" s="5">
+        <v>62600</v>
+      </c>
+      <c r="S126" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T126" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U126" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="127" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N127" s="18" t="s">

</xml_diff>

<commit_message>
Data for Aashish Sort 5
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B2643A-D924-4566-8427-7A3CF08CD377}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25137C55-565B-4142-8C75-10805B0EE1AD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W126" sqref="W126"/>
+    <sheetView tabSelected="1" topLeftCell="I112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V129" sqref="V129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5618,60 +5618,120 @@
       <c r="O127" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P127" s="7"/>
-      <c r="Q127" s="7"/>
-      <c r="R127" s="7"/>
-      <c r="S127" s="7"/>
-      <c r="T127" s="7"/>
-      <c r="U127" s="8"/>
+      <c r="P127" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q127" s="7">
+        <v>11</v>
+      </c>
+      <c r="R127" s="7">
+        <v>164</v>
+      </c>
+      <c r="S127" s="7">
+        <v>7250</v>
+      </c>
+      <c r="T127" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U127" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="128" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N128" s="16"/>
       <c r="O128" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P128" s="8"/>
-      <c r="Q128" s="8"/>
-      <c r="R128" s="8"/>
-      <c r="S128" s="8"/>
-      <c r="T128" s="8"/>
-      <c r="U128" s="8"/>
+      <c r="P128" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q128" s="8">
+        <v>2</v>
+      </c>
+      <c r="R128" s="8">
+        <v>108</v>
+      </c>
+      <c r="S128" s="8">
+        <v>6997</v>
+      </c>
+      <c r="T128" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="129" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N129" s="16"/>
       <c r="O129" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P129" s="8"/>
-      <c r="Q129" s="8"/>
-      <c r="R129" s="8"/>
-      <c r="S129" s="8"/>
-      <c r="T129" s="8"/>
-      <c r="U129" s="8"/>
+      <c r="P129" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q129" s="8">
+        <v>3</v>
+      </c>
+      <c r="R129" s="8">
+        <v>90</v>
+      </c>
+      <c r="S129" s="8">
+        <v>7124</v>
+      </c>
+      <c r="T129" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U129" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="130" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N130" s="16"/>
       <c r="O130" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P130" s="8"/>
-      <c r="Q130" s="8"/>
-      <c r="R130" s="8"/>
-      <c r="S130" s="8"/>
-      <c r="T130" s="8"/>
-      <c r="U130" s="8"/>
+      <c r="P130" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="8">
+        <v>1</v>
+      </c>
+      <c r="R130" s="8">
+        <v>78</v>
+      </c>
+      <c r="S130" s="8">
+        <v>6951</v>
+      </c>
+      <c r="T130" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="131" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N131" s="17"/>
       <c r="O131" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P131" s="5"/>
-      <c r="Q131" s="5"/>
-      <c r="R131" s="5"/>
-      <c r="S131" s="5"/>
-      <c r="T131" s="5"/>
-      <c r="U131" s="5"/>
+      <c r="P131" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q131" s="5">
+        <v>1</v>
+      </c>
+      <c r="R131" s="5">
+        <v>72</v>
+      </c>
+      <c r="S131" s="5">
+        <v>6908</v>
+      </c>
+      <c r="T131" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U131" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="132" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N132" s="18" t="s">

</xml_diff>

<commit_message>
Add data for Aashish Sort 4
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25137C55-565B-4142-8C75-10805B0EE1AD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DBC0BC-7055-4D21-8D44-A5F3C55C2904}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="1" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="36">
   <si>
     <t>Input Size</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V129" sqref="V129"/>
+    <sheetView tabSelected="1" topLeftCell="I118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T139" sqref="T139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5740,60 +5740,120 @@
       <c r="O132" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P132" s="7"/>
-      <c r="Q132" s="7"/>
-      <c r="R132" s="7"/>
-      <c r="S132" s="7"/>
-      <c r="T132" s="7"/>
-      <c r="U132" s="8"/>
+      <c r="P132" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q132" s="7">
+        <v>11</v>
+      </c>
+      <c r="R132" s="7">
+        <v>349</v>
+      </c>
+      <c r="S132" s="7">
+        <v>29788</v>
+      </c>
+      <c r="T132" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="133" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N133" s="16"/>
       <c r="O133" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P133" s="8"/>
-      <c r="Q133" s="8"/>
-      <c r="R133" s="8"/>
-      <c r="S133" s="8"/>
-      <c r="T133" s="8"/>
-      <c r="U133" s="8"/>
+      <c r="P133" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q133" s="8">
+        <v>6</v>
+      </c>
+      <c r="R133" s="8">
+        <v>286</v>
+      </c>
+      <c r="S133" s="8">
+        <v>29873</v>
+      </c>
+      <c r="T133" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U133" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="134" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N134" s="16"/>
       <c r="O134" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P134" s="8"/>
-      <c r="Q134" s="8"/>
-      <c r="R134" s="8"/>
-      <c r="S134" s="8"/>
-      <c r="T134" s="8"/>
-      <c r="U134" s="8"/>
+      <c r="P134" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q134" s="8">
+        <v>3</v>
+      </c>
+      <c r="R134" s="8">
+        <v>185</v>
+      </c>
+      <c r="S134" s="8">
+        <v>21541</v>
+      </c>
+      <c r="T134" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="135" spans="14:21" x14ac:dyDescent="0.35">
       <c r="N135" s="16"/>
       <c r="O135" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P135" s="8"/>
-      <c r="Q135" s="8"/>
-      <c r="R135" s="8"/>
-      <c r="S135" s="8"/>
-      <c r="T135" s="8"/>
-      <c r="U135" s="8"/>
+      <c r="P135" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q135" s="8">
+        <v>3</v>
+      </c>
+      <c r="R135" s="8">
+        <v>193</v>
+      </c>
+      <c r="S135" s="8">
+        <v>21286</v>
+      </c>
+      <c r="T135" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U135" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="136" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N136" s="17"/>
       <c r="O136" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P136" s="5"/>
-      <c r="Q136" s="5"/>
-      <c r="R136" s="5"/>
-      <c r="S136" s="5"/>
-      <c r="T136" s="5"/>
-      <c r="U136" s="5"/>
+      <c r="P136" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q136" s="5">
+        <v>3</v>
+      </c>
+      <c r="R136" s="5">
+        <v>188</v>
+      </c>
+      <c r="S136" s="5">
+        <v>21406</v>
+      </c>
+      <c r="T136" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U136" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="137" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="P137" s="8"/>

</xml_diff>

<commit_message>
Make y-axis start at 1
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5665C8D-3188-4DF9-9D9C-140DA04B7F81}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A12616-89CF-4A69-BF8C-FABD3D9A33D2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -277,6 +277,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,18 +291,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,7 +1294,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
@@ -1400,7 +1400,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
@@ -3243,6 +3243,7 @@
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4326,7 +4327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -4341,7 +4342,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="19" t="s">
@@ -4358,7 +4359,7 @@
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B2" s="18"/>
+      <c r="B2" s="21"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
@@ -4371,10 +4372,10 @@
       <c r="M2" s="11"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B3" s="18"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" s="18"/>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="13"/>
@@ -4463,13 +4464,13 @@
     <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="N33" s="10"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="20" t="s">
+      <c r="P33" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="N34" s="3"/>
@@ -4494,15 +4495,15 @@
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="N35" s="15" t="s">
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="N35" s="17" t="s">
         <v>26</v>
       </c>
       <c r="O35" s="2" t="s">
@@ -4528,31 +4529,31 @@
       </c>
     </row>
     <row r="36" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C36" s="21">
+      <c r="C36" s="14">
         <f t="shared" ref="C36:H36" si="0">P34</f>
         <v>100</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="14">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="14">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="14">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="14">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="H36" s="21">
+      <c r="H36" s="14">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="N36" s="15"/>
+      <c r="N36" s="17"/>
       <c r="O36" s="2" t="s">
         <v>3</v>
       </c>
@@ -4598,7 +4599,7 @@
       <c r="H37">
         <v>99999999</v>
       </c>
-      <c r="N37" s="15"/>
+      <c r="N37" s="17"/>
       <c r="O37" s="2" t="s">
         <v>4</v>
       </c>
@@ -4630,7 +4631,7 @@
         <v>1.4</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:H38" si="1">AVERAGE(Q40:Q44)</f>
+        <f t="shared" ref="D38:F38" si="1">AVERAGE(Q40:Q44)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="E38">
@@ -4647,7 +4648,7 @@
       <c r="H38">
         <v>99999999</v>
       </c>
-      <c r="N38" s="15"/>
+      <c r="N38" s="17"/>
       <c r="O38" s="12" t="s">
         <v>5</v>
       </c>
@@ -4679,7 +4680,7 @@
         <v>1.8</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:H39" si="2">AVERAGE(Q45:Q49)</f>
+        <f t="shared" ref="D39:E39" si="2">AVERAGE(Q45:Q49)</f>
         <v>211.2</v>
       </c>
       <c r="E39">
@@ -4695,7 +4696,7 @@
       <c r="H39">
         <v>99999999</v>
       </c>
-      <c r="N39" s="16"/>
+      <c r="N39" s="18"/>
       <c r="O39" s="4" t="s">
         <v>6</v>
       </c>
@@ -4727,7 +4728,7 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:H40" si="3">AVERAGE(Q50:Q54)</f>
+        <f t="shared" ref="D40:F40" si="3">AVERAGE(Q50:Q54)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="E40">
@@ -4744,7 +4745,7 @@
       <c r="H40">
         <v>99999999</v>
       </c>
-      <c r="N40" s="14" t="s">
+      <c r="N40" s="16" t="s">
         <v>27</v>
       </c>
       <c r="O40" s="12" t="s">
@@ -4797,7 +4798,7 @@
         <f t="shared" si="4"/>
         <v>3546.8</v>
       </c>
-      <c r="N41" s="15"/>
+      <c r="N41" s="17"/>
       <c r="O41" s="12" t="s">
         <v>3</v>
       </c>
@@ -4829,7 +4830,7 @@
         <v>0.8</v>
       </c>
       <c r="D42">
-        <f t="shared" ref="D42:H42" si="5">AVERAGE(Q60:Q64)</f>
+        <f t="shared" ref="D42:F42" si="5">AVERAGE(Q60:Q64)</f>
         <v>4</v>
       </c>
       <c r="E42">
@@ -4846,7 +4847,7 @@
       <c r="H42">
         <v>99999999</v>
       </c>
-      <c r="N42" s="15"/>
+      <c r="N42" s="17"/>
       <c r="O42" s="12" t="s">
         <v>4</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>1.2</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:H43" si="6">AVERAGE(Q65:Q69)</f>
+        <f t="shared" ref="D43:F43" si="6">AVERAGE(Q65:Q69)</f>
         <v>3.6</v>
       </c>
       <c r="E43">
@@ -4895,7 +4896,7 @@
       <c r="H43">
         <v>99999999</v>
       </c>
-      <c r="N43" s="15"/>
+      <c r="N43" s="17"/>
       <c r="O43" s="12" t="s">
         <v>5</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44:H44" si="7">AVERAGE(Q70:Q74)</f>
+        <f t="shared" ref="D44:F44" si="7">AVERAGE(Q70:Q74)</f>
         <v>2.6</v>
       </c>
       <c r="E44">
@@ -4944,7 +4945,7 @@
       <c r="H44">
         <v>99999999</v>
       </c>
-      <c r="N44" s="16"/>
+      <c r="N44" s="18"/>
       <c r="O44" s="4" t="s">
         <v>6</v>
       </c>
@@ -4995,7 +4996,7 @@
         <f t="shared" si="8"/>
         <v>2048.1999999999998</v>
       </c>
-      <c r="N45" s="14" t="s">
+      <c r="N45" s="16" t="s">
         <v>28</v>
       </c>
       <c r="O45" s="2" t="s">
@@ -5029,7 +5030,7 @@
         <v>1.2</v>
       </c>
       <c r="D46">
-        <f t="shared" ref="D46:H46" si="9">AVERAGE(Q80:Q84)</f>
+        <f t="shared" ref="D46:F46" si="9">AVERAGE(Q80:Q84)</f>
         <v>1.8</v>
       </c>
       <c r="E46">
@@ -5046,7 +5047,7 @@
       <c r="H46">
         <v>99999999</v>
       </c>
-      <c r="N46" s="15"/>
+      <c r="N46" s="17"/>
       <c r="O46" s="2" t="s">
         <v>3</v>
       </c>
@@ -5097,7 +5098,7 @@
         <f t="shared" si="10"/>
         <v>3327.6</v>
       </c>
-      <c r="N47" s="15"/>
+      <c r="N47" s="17"/>
       <c r="O47" s="2" t="s">
         <v>4</v>
       </c>
@@ -5148,7 +5149,7 @@
         <f t="shared" si="11"/>
         <v>1352.8</v>
       </c>
-      <c r="N48" s="15"/>
+      <c r="N48" s="17"/>
       <c r="O48" s="12" t="s">
         <v>5</v>
       </c>
@@ -5199,7 +5200,7 @@
         <f t="shared" si="12"/>
         <v>3308.4</v>
       </c>
-      <c r="N49" s="16"/>
+      <c r="N49" s="18"/>
       <c r="O49" s="4" t="s">
         <v>6</v>
       </c>
@@ -5250,7 +5251,7 @@
         <f t="shared" si="13"/>
         <v>1187.2</v>
       </c>
-      <c r="N50" s="14" t="s">
+      <c r="N50" s="16" t="s">
         <v>1</v>
       </c>
       <c r="O50" s="2" t="s">
@@ -5303,7 +5304,7 @@
         <f t="shared" si="14"/>
         <v>29.4</v>
       </c>
-      <c r="N51" s="15"/>
+      <c r="N51" s="17"/>
       <c r="O51" s="2" t="s">
         <v>3</v>
       </c>
@@ -5354,7 +5355,7 @@
         <f t="shared" si="15"/>
         <v>16.2</v>
       </c>
-      <c r="N52" s="15"/>
+      <c r="N52" s="17"/>
       <c r="O52" s="2" t="s">
         <v>4</v>
       </c>
@@ -5405,7 +5406,7 @@
         <f t="shared" si="16"/>
         <v>10.4</v>
       </c>
-      <c r="N53" s="15"/>
+      <c r="N53" s="17"/>
       <c r="O53" s="2" t="s">
         <v>5</v>
       </c>
@@ -5437,7 +5438,7 @@
         <v>1.6</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:H54" si="17">AVERAGE(Q120:Q124)</f>
+        <f t="shared" ref="D54:F54" si="17">AVERAGE(Q120:Q124)</f>
         <v>1.2</v>
       </c>
       <c r="E54">
@@ -5454,7 +5455,7 @@
       <c r="H54">
         <v>99999999</v>
       </c>
-      <c r="N54" s="16"/>
+      <c r="N54" s="18"/>
       <c r="O54" s="4" t="s">
         <v>6</v>
       </c>
@@ -5505,7 +5506,7 @@
         <f t="shared" si="18"/>
         <v>1334.2</v>
       </c>
-      <c r="N55" s="14" t="s">
+      <c r="N55" s="16" t="s">
         <v>20</v>
       </c>
       <c r="O55" s="2" t="s">
@@ -5558,7 +5559,7 @@
         <f t="shared" si="19"/>
         <v>317.60000000000002</v>
       </c>
-      <c r="N56" s="15"/>
+      <c r="N56" s="17"/>
       <c r="O56" s="2" t="s">
         <v>3</v>
       </c>
@@ -5609,7 +5610,7 @@
         <f t="shared" si="20"/>
         <v>1426.6</v>
       </c>
-      <c r="N57" s="15"/>
+      <c r="N57" s="17"/>
       <c r="O57" s="2" t="s">
         <v>4</v>
       </c>
@@ -5660,7 +5661,7 @@
         <f t="shared" si="21"/>
         <v>317.8</v>
       </c>
-      <c r="N58" s="15"/>
+      <c r="N58" s="17"/>
       <c r="O58" s="2" t="s">
         <v>5</v>
       </c>
@@ -5711,7 +5712,7 @@
         <f t="shared" si="22"/>
         <v>7641.8</v>
       </c>
-      <c r="N59" s="16"/>
+      <c r="N59" s="18"/>
       <c r="O59" s="4" t="s">
         <v>6</v>
       </c>
@@ -5743,7 +5744,7 @@
         <v>2.4</v>
       </c>
       <c r="D60">
-        <f t="shared" ref="D60:H60" si="23">AVERAGE(Q150:Q154)</f>
+        <f t="shared" ref="D60:E60" si="23">AVERAGE(Q150:Q154)</f>
         <v>57.6</v>
       </c>
       <c r="E60">
@@ -5759,7 +5760,7 @@
       <c r="H60">
         <v>99999999</v>
       </c>
-      <c r="N60" s="14" t="s">
+      <c r="N60" s="16" t="s">
         <v>7</v>
       </c>
       <c r="O60" s="6" t="s">
@@ -5793,7 +5794,7 @@
         <v>1.2</v>
       </c>
       <c r="D61">
-        <f t="shared" ref="D61:H61" si="24">AVERAGE(Q155:Q159)</f>
+        <f t="shared" ref="D61:F61" si="24">AVERAGE(Q155:Q159)</f>
         <v>3.6</v>
       </c>
       <c r="E61">
@@ -5810,7 +5811,7 @@
       <c r="H61">
         <v>99999999</v>
       </c>
-      <c r="N61" s="15"/>
+      <c r="N61" s="17"/>
       <c r="O61" s="2" t="s">
         <v>3</v>
       </c>
@@ -5842,7 +5843,7 @@
         <v>1.6</v>
       </c>
       <c r="D62">
-        <f t="shared" ref="D62:H62" si="25">AVERAGE(Q160:Q164)</f>
+        <f t="shared" ref="D62:F62" si="25">AVERAGE(Q160:Q164)</f>
         <v>5.2</v>
       </c>
       <c r="E62">
@@ -5859,7 +5860,7 @@
       <c r="H62">
         <v>99999999</v>
       </c>
-      <c r="N62" s="15"/>
+      <c r="N62" s="17"/>
       <c r="O62" s="2" t="s">
         <v>4</v>
       </c>
@@ -5883,7 +5884,7 @@
       </c>
     </row>
     <row r="63" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="N63" s="15"/>
+      <c r="N63" s="17"/>
       <c r="O63" s="2" t="s">
         <v>5</v>
       </c>
@@ -5907,7 +5908,7 @@
       </c>
     </row>
     <row r="64" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N64" s="16"/>
+      <c r="N64" s="18"/>
       <c r="O64" s="4" t="s">
         <v>6</v>
       </c>
@@ -5931,7 +5932,7 @@
       </c>
     </row>
     <row r="65" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N65" s="14" t="s">
+      <c r="N65" s="16" t="s">
         <v>29</v>
       </c>
       <c r="O65" s="6" t="s">
@@ -5957,7 +5958,7 @@
       </c>
     </row>
     <row r="66" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N66" s="15"/>
+      <c r="N66" s="17"/>
       <c r="O66" s="2" t="s">
         <v>3</v>
       </c>
@@ -5981,7 +5982,7 @@
       </c>
     </row>
     <row r="67" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N67" s="15"/>
+      <c r="N67" s="17"/>
       <c r="O67" s="2" t="s">
         <v>4</v>
       </c>
@@ -6005,7 +6006,7 @@
       </c>
     </row>
     <row r="68" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N68" s="15"/>
+      <c r="N68" s="17"/>
       <c r="O68" s="2" t="s">
         <v>5</v>
       </c>
@@ -6029,7 +6030,7 @@
       </c>
     </row>
     <row r="69" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N69" s="16"/>
+      <c r="N69" s="18"/>
       <c r="O69" s="4" t="s">
         <v>6</v>
       </c>
@@ -6053,7 +6054,7 @@
       </c>
     </row>
     <row r="70" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N70" s="14" t="s">
+      <c r="N70" s="16" t="s">
         <v>30</v>
       </c>
       <c r="O70" s="6" t="s">
@@ -6079,7 +6080,7 @@
       </c>
     </row>
     <row r="71" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N71" s="15"/>
+      <c r="N71" s="17"/>
       <c r="O71" s="2" t="s">
         <v>3</v>
       </c>
@@ -6103,7 +6104,7 @@
       </c>
     </row>
     <row r="72" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N72" s="15"/>
+      <c r="N72" s="17"/>
       <c r="O72" s="2" t="s">
         <v>4</v>
       </c>
@@ -6127,7 +6128,7 @@
       </c>
     </row>
     <row r="73" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N73" s="15"/>
+      <c r="N73" s="17"/>
       <c r="O73" s="2" t="s">
         <v>5</v>
       </c>
@@ -6151,7 +6152,7 @@
       </c>
     </row>
     <row r="74" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N74" s="16"/>
+      <c r="N74" s="18"/>
       <c r="O74" s="4" t="s">
         <v>6</v>
       </c>
@@ -6175,7 +6176,7 @@
       </c>
     </row>
     <row r="75" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N75" s="14" t="s">
+      <c r="N75" s="16" t="s">
         <v>21</v>
       </c>
       <c r="O75" s="2" t="s">
@@ -6201,7 +6202,7 @@
       </c>
     </row>
     <row r="76" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N76" s="15"/>
+      <c r="N76" s="17"/>
       <c r="O76" s="2" t="s">
         <v>3</v>
       </c>
@@ -6225,7 +6226,7 @@
       </c>
     </row>
     <row r="77" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N77" s="15"/>
+      <c r="N77" s="17"/>
       <c r="O77" s="2" t="s">
         <v>4</v>
       </c>
@@ -6249,7 +6250,7 @@
       </c>
     </row>
     <row r="78" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N78" s="15"/>
+      <c r="N78" s="17"/>
       <c r="O78" s="2" t="s">
         <v>5</v>
       </c>
@@ -6273,7 +6274,7 @@
       </c>
     </row>
     <row r="79" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N79" s="16"/>
+      <c r="N79" s="18"/>
       <c r="O79" s="4" t="s">
         <v>6</v>
       </c>
@@ -6297,7 +6298,7 @@
       </c>
     </row>
     <row r="80" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N80" s="14" t="s">
+      <c r="N80" s="16" t="s">
         <v>8</v>
       </c>
       <c r="O80" s="6" t="s">
@@ -6323,7 +6324,7 @@
       </c>
     </row>
     <row r="81" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N81" s="15"/>
+      <c r="N81" s="17"/>
       <c r="O81" s="2" t="s">
         <v>3</v>
       </c>
@@ -6347,7 +6348,7 @@
       </c>
     </row>
     <row r="82" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N82" s="15"/>
+      <c r="N82" s="17"/>
       <c r="O82" s="2" t="s">
         <v>4</v>
       </c>
@@ -6371,7 +6372,7 @@
       </c>
     </row>
     <row r="83" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N83" s="15"/>
+      <c r="N83" s="17"/>
       <c r="O83" s="2" t="s">
         <v>5</v>
       </c>
@@ -6395,7 +6396,7 @@
       </c>
     </row>
     <row r="84" spans="11:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N84" s="16"/>
+      <c r="N84" s="18"/>
       <c r="O84" s="4" t="s">
         <v>6</v>
       </c>
@@ -6419,7 +6420,7 @@
       </c>
     </row>
     <row r="85" spans="11:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N85" s="14" t="s">
+      <c r="N85" s="16" t="s">
         <v>19</v>
       </c>
       <c r="O85" s="6" t="s">
@@ -6448,7 +6449,7 @@
       <c r="K86" t="s">
         <v>25</v>
       </c>
-      <c r="N86" s="15"/>
+      <c r="N86" s="17"/>
       <c r="O86" s="2" t="s">
         <v>3</v>
       </c>
@@ -6472,7 +6473,7 @@
       </c>
     </row>
     <row r="87" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N87" s="15"/>
+      <c r="N87" s="17"/>
       <c r="O87" s="2" t="s">
         <v>4</v>
       </c>
@@ -6496,7 +6497,7 @@
       </c>
     </row>
     <row r="88" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N88" s="15"/>
+      <c r="N88" s="17"/>
       <c r="O88" s="2" t="s">
         <v>5</v>
       </c>
@@ -6520,7 +6521,7 @@
       </c>
     </row>
     <row r="89" spans="11:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N89" s="16"/>
+      <c r="N89" s="18"/>
       <c r="O89" s="4" t="s">
         <v>6</v>
       </c>
@@ -6544,7 +6545,7 @@
       </c>
     </row>
     <row r="90" spans="11:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N90" s="14" t="s">
+      <c r="N90" s="16" t="s">
         <v>9</v>
       </c>
       <c r="O90" s="6" t="s">
@@ -6570,7 +6571,7 @@
       </c>
     </row>
     <row r="91" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N91" s="15"/>
+      <c r="N91" s="17"/>
       <c r="O91" s="2" t="s">
         <v>3</v>
       </c>
@@ -6594,7 +6595,7 @@
       </c>
     </row>
     <row r="92" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N92" s="15"/>
+      <c r="N92" s="17"/>
       <c r="O92" s="2" t="s">
         <v>4</v>
       </c>
@@ -6618,7 +6619,7 @@
       </c>
     </row>
     <row r="93" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N93" s="15"/>
+      <c r="N93" s="17"/>
       <c r="O93" s="2" t="s">
         <v>5</v>
       </c>
@@ -6642,7 +6643,7 @@
       </c>
     </row>
     <row r="94" spans="11:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N94" s="16"/>
+      <c r="N94" s="18"/>
       <c r="O94" s="4" t="s">
         <v>6</v>
       </c>
@@ -6666,7 +6667,7 @@
       </c>
     </row>
     <row r="95" spans="11:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N95" s="14" t="s">
+      <c r="N95" s="16" t="s">
         <v>10</v>
       </c>
       <c r="O95" s="6" t="s">
@@ -6692,7 +6693,7 @@
       </c>
     </row>
     <row r="96" spans="11:21" x14ac:dyDescent="0.35">
-      <c r="N96" s="15"/>
+      <c r="N96" s="17"/>
       <c r="O96" s="2" t="s">
         <v>3</v>
       </c>
@@ -6716,7 +6717,7 @@
       </c>
     </row>
     <row r="97" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N97" s="15"/>
+      <c r="N97" s="17"/>
       <c r="O97" s="2" t="s">
         <v>4</v>
       </c>
@@ -6740,7 +6741,7 @@
       </c>
     </row>
     <row r="98" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N98" s="15"/>
+      <c r="N98" s="17"/>
       <c r="O98" s="2" t="s">
         <v>5</v>
       </c>
@@ -6764,7 +6765,7 @@
       </c>
     </row>
     <row r="99" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N99" s="16"/>
+      <c r="N99" s="18"/>
       <c r="O99" s="4" t="s">
         <v>6</v>
       </c>
@@ -6788,7 +6789,7 @@
       </c>
     </row>
     <row r="100" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N100" s="14" t="s">
+      <c r="N100" s="16" t="s">
         <v>11</v>
       </c>
       <c r="O100" s="6" t="s">
@@ -6814,7 +6815,7 @@
       </c>
     </row>
     <row r="101" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N101" s="15"/>
+      <c r="N101" s="17"/>
       <c r="O101" s="2" t="s">
         <v>3</v>
       </c>
@@ -6838,7 +6839,7 @@
       </c>
     </row>
     <row r="102" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N102" s="15"/>
+      <c r="N102" s="17"/>
       <c r="O102" s="2" t="s">
         <v>4</v>
       </c>
@@ -6862,7 +6863,7 @@
       </c>
     </row>
     <row r="103" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N103" s="15"/>
+      <c r="N103" s="17"/>
       <c r="O103" s="2" t="s">
         <v>5</v>
       </c>
@@ -6886,7 +6887,7 @@
       </c>
     </row>
     <row r="104" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N104" s="16"/>
+      <c r="N104" s="18"/>
       <c r="O104" s="4" t="s">
         <v>6</v>
       </c>
@@ -6910,7 +6911,7 @@
       </c>
     </row>
     <row r="105" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N105" s="14" t="s">
+      <c r="N105" s="16" t="s">
         <v>12</v>
       </c>
       <c r="O105" s="6" t="s">
@@ -6936,7 +6937,7 @@
       </c>
     </row>
     <row r="106" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N106" s="15"/>
+      <c r="N106" s="17"/>
       <c r="O106" s="2" t="s">
         <v>3</v>
       </c>
@@ -6960,7 +6961,7 @@
       </c>
     </row>
     <row r="107" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N107" s="15"/>
+      <c r="N107" s="17"/>
       <c r="O107" s="2" t="s">
         <v>4</v>
       </c>
@@ -6984,7 +6985,7 @@
       </c>
     </row>
     <row r="108" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N108" s="15"/>
+      <c r="N108" s="17"/>
       <c r="O108" s="2" t="s">
         <v>5</v>
       </c>
@@ -7008,7 +7009,7 @@
       </c>
     </row>
     <row r="109" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N109" s="16"/>
+      <c r="N109" s="18"/>
       <c r="O109" s="4" t="s">
         <v>6</v>
       </c>
@@ -7032,7 +7033,7 @@
       </c>
     </row>
     <row r="110" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N110" s="14" t="s">
+      <c r="N110" s="16" t="s">
         <v>13</v>
       </c>
       <c r="O110" s="6" t="s">
@@ -7058,7 +7059,7 @@
       </c>
     </row>
     <row r="111" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N111" s="15"/>
+      <c r="N111" s="17"/>
       <c r="O111" s="2" t="s">
         <v>3</v>
       </c>
@@ -7082,7 +7083,7 @@
       </c>
     </row>
     <row r="112" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N112" s="15"/>
+      <c r="N112" s="17"/>
       <c r="O112" s="2" t="s">
         <v>4</v>
       </c>
@@ -7106,7 +7107,7 @@
       </c>
     </row>
     <row r="113" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N113" s="15"/>
+      <c r="N113" s="17"/>
       <c r="O113" s="2" t="s">
         <v>5</v>
       </c>
@@ -7130,7 +7131,7 @@
       </c>
     </row>
     <row r="114" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N114" s="16"/>
+      <c r="N114" s="18"/>
       <c r="O114" s="4" t="s">
         <v>6</v>
       </c>
@@ -7154,7 +7155,7 @@
       </c>
     </row>
     <row r="115" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N115" s="14" t="s">
+      <c r="N115" s="16" t="s">
         <v>14</v>
       </c>
       <c r="O115" s="6" t="s">
@@ -7180,7 +7181,7 @@
       </c>
     </row>
     <row r="116" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N116" s="15"/>
+      <c r="N116" s="17"/>
       <c r="O116" s="2" t="s">
         <v>3</v>
       </c>
@@ -7204,7 +7205,7 @@
       </c>
     </row>
     <row r="117" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N117" s="15"/>
+      <c r="N117" s="17"/>
       <c r="O117" s="2" t="s">
         <v>4</v>
       </c>
@@ -7228,7 +7229,7 @@
       </c>
     </row>
     <row r="118" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N118" s="15"/>
+      <c r="N118" s="17"/>
       <c r="O118" s="2" t="s">
         <v>5</v>
       </c>
@@ -7252,7 +7253,7 @@
       </c>
     </row>
     <row r="119" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N119" s="16"/>
+      <c r="N119" s="18"/>
       <c r="O119" s="4" t="s">
         <v>6</v>
       </c>
@@ -7276,7 +7277,7 @@
       </c>
     </row>
     <row r="120" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N120" s="14" t="s">
+      <c r="N120" s="16" t="s">
         <v>31</v>
       </c>
       <c r="O120" s="6" t="s">
@@ -7302,7 +7303,7 @@
       </c>
     </row>
     <row r="121" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N121" s="15"/>
+      <c r="N121" s="17"/>
       <c r="O121" s="2" t="s">
         <v>3</v>
       </c>
@@ -7326,7 +7327,7 @@
       </c>
     </row>
     <row r="122" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N122" s="15"/>
+      <c r="N122" s="17"/>
       <c r="O122" s="2" t="s">
         <v>4</v>
       </c>
@@ -7350,7 +7351,7 @@
       </c>
     </row>
     <row r="123" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N123" s="15"/>
+      <c r="N123" s="17"/>
       <c r="O123" s="2" t="s">
         <v>5</v>
       </c>
@@ -7374,7 +7375,7 @@
       </c>
     </row>
     <row r="124" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N124" s="16"/>
+      <c r="N124" s="18"/>
       <c r="O124" s="4" t="s">
         <v>6</v>
       </c>
@@ -7398,7 +7399,7 @@
       </c>
     </row>
     <row r="125" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N125" s="14" t="s">
+      <c r="N125" s="16" t="s">
         <v>15</v>
       </c>
       <c r="O125" s="6" t="s">
@@ -7424,7 +7425,7 @@
       </c>
     </row>
     <row r="126" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N126" s="15"/>
+      <c r="N126" s="17"/>
       <c r="O126" s="2" t="s">
         <v>3</v>
       </c>
@@ -7448,7 +7449,7 @@
       </c>
     </row>
     <row r="127" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N127" s="15"/>
+      <c r="N127" s="17"/>
       <c r="O127" s="2" t="s">
         <v>4</v>
       </c>
@@ -7472,7 +7473,7 @@
       </c>
     </row>
     <row r="128" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N128" s="15"/>
+      <c r="N128" s="17"/>
       <c r="O128" s="2" t="s">
         <v>5</v>
       </c>
@@ -7496,7 +7497,7 @@
       </c>
     </row>
     <row r="129" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N129" s="16"/>
+      <c r="N129" s="18"/>
       <c r="O129" s="4" t="s">
         <v>6</v>
       </c>
@@ -7520,7 +7521,7 @@
       </c>
     </row>
     <row r="130" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N130" s="14" t="s">
+      <c r="N130" s="16" t="s">
         <v>16</v>
       </c>
       <c r="O130" s="6" t="s">
@@ -7546,7 +7547,7 @@
       </c>
     </row>
     <row r="131" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N131" s="15"/>
+      <c r="N131" s="17"/>
       <c r="O131" s="2" t="s">
         <v>3</v>
       </c>
@@ -7570,7 +7571,7 @@
       </c>
     </row>
     <row r="132" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N132" s="15"/>
+      <c r="N132" s="17"/>
       <c r="O132" s="2" t="s">
         <v>4</v>
       </c>
@@ -7594,7 +7595,7 @@
       </c>
     </row>
     <row r="133" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N133" s="15"/>
+      <c r="N133" s="17"/>
       <c r="O133" s="2" t="s">
         <v>5</v>
       </c>
@@ -7618,7 +7619,7 @@
       </c>
     </row>
     <row r="134" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N134" s="16"/>
+      <c r="N134" s="18"/>
       <c r="O134" s="4" t="s">
         <v>6</v>
       </c>
@@ -7642,7 +7643,7 @@
       </c>
     </row>
     <row r="135" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N135" s="14" t="s">
+      <c r="N135" s="16" t="s">
         <v>17</v>
       </c>
       <c r="O135" s="6" t="s">
@@ -7668,7 +7669,7 @@
       </c>
     </row>
     <row r="136" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N136" s="15"/>
+      <c r="N136" s="17"/>
       <c r="O136" s="2" t="s">
         <v>3</v>
       </c>
@@ -7692,7 +7693,7 @@
       </c>
     </row>
     <row r="137" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N137" s="15"/>
+      <c r="N137" s="17"/>
       <c r="O137" s="2" t="s">
         <v>4</v>
       </c>
@@ -7716,7 +7717,7 @@
       </c>
     </row>
     <row r="138" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N138" s="15"/>
+      <c r="N138" s="17"/>
       <c r="O138" s="2" t="s">
         <v>5</v>
       </c>
@@ -7740,7 +7741,7 @@
       </c>
     </row>
     <row r="139" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N139" s="16"/>
+      <c r="N139" s="18"/>
       <c r="O139" s="4" t="s">
         <v>6</v>
       </c>
@@ -7764,7 +7765,7 @@
       </c>
     </row>
     <row r="140" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N140" s="14" t="s">
+      <c r="N140" s="16" t="s">
         <v>22</v>
       </c>
       <c r="O140" s="6" t="s">
@@ -7790,7 +7791,7 @@
       </c>
     </row>
     <row r="141" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N141" s="15"/>
+      <c r="N141" s="17"/>
       <c r="O141" s="2" t="s">
         <v>3</v>
       </c>
@@ -7814,7 +7815,7 @@
       </c>
     </row>
     <row r="142" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N142" s="15"/>
+      <c r="N142" s="17"/>
       <c r="O142" s="2" t="s">
         <v>4</v>
       </c>
@@ -7838,7 +7839,7 @@
       </c>
     </row>
     <row r="143" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N143" s="15"/>
+      <c r="N143" s="17"/>
       <c r="O143" s="2" t="s">
         <v>5</v>
       </c>
@@ -7862,7 +7863,7 @@
       </c>
     </row>
     <row r="144" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N144" s="16"/>
+      <c r="N144" s="18"/>
       <c r="O144" s="4" t="s">
         <v>6</v>
       </c>
@@ -7886,7 +7887,7 @@
       </c>
     </row>
     <row r="145" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N145" s="14" t="s">
+      <c r="N145" s="16" t="s">
         <v>32</v>
       </c>
       <c r="O145" s="6" t="s">
@@ -7912,7 +7913,7 @@
       </c>
     </row>
     <row r="146" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N146" s="15"/>
+      <c r="N146" s="17"/>
       <c r="O146" s="2" t="s">
         <v>3</v>
       </c>
@@ -7936,7 +7937,7 @@
       </c>
     </row>
     <row r="147" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N147" s="15"/>
+      <c r="N147" s="17"/>
       <c r="O147" s="2" t="s">
         <v>4</v>
       </c>
@@ -7960,7 +7961,7 @@
       </c>
     </row>
     <row r="148" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N148" s="15"/>
+      <c r="N148" s="17"/>
       <c r="O148" s="2" t="s">
         <v>5</v>
       </c>
@@ -7984,7 +7985,7 @@
       </c>
     </row>
     <row r="149" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N149" s="16"/>
+      <c r="N149" s="18"/>
       <c r="O149" s="4" t="s">
         <v>6</v>
       </c>
@@ -8008,7 +8009,7 @@
       </c>
     </row>
     <row r="150" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N150" s="14" t="s">
+      <c r="N150" s="16" t="s">
         <v>33</v>
       </c>
       <c r="O150" s="6" t="s">
@@ -8034,7 +8035,7 @@
       </c>
     </row>
     <row r="151" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N151" s="15"/>
+      <c r="N151" s="17"/>
       <c r="O151" s="2" t="s">
         <v>3</v>
       </c>
@@ -8058,7 +8059,7 @@
       </c>
     </row>
     <row r="152" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N152" s="15"/>
+      <c r="N152" s="17"/>
       <c r="O152" s="2" t="s">
         <v>4</v>
       </c>
@@ -8082,7 +8083,7 @@
       </c>
     </row>
     <row r="153" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N153" s="15"/>
+      <c r="N153" s="17"/>
       <c r="O153" s="2" t="s">
         <v>5</v>
       </c>
@@ -8106,7 +8107,7 @@
       </c>
     </row>
     <row r="154" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N154" s="16"/>
+      <c r="N154" s="18"/>
       <c r="O154" s="4" t="s">
         <v>6</v>
       </c>
@@ -8130,7 +8131,7 @@
       </c>
     </row>
     <row r="155" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N155" s="14" t="s">
+      <c r="N155" s="16" t="s">
         <v>35</v>
       </c>
       <c r="O155" s="6" t="s">
@@ -8156,7 +8157,7 @@
       </c>
     </row>
     <row r="156" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N156" s="15"/>
+      <c r="N156" s="17"/>
       <c r="O156" s="2" t="s">
         <v>3</v>
       </c>
@@ -8180,7 +8181,7 @@
       </c>
     </row>
     <row r="157" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N157" s="15"/>
+      <c r="N157" s="17"/>
       <c r="O157" s="2" t="s">
         <v>4</v>
       </c>
@@ -8204,7 +8205,7 @@
       </c>
     </row>
     <row r="158" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N158" s="15"/>
+      <c r="N158" s="17"/>
       <c r="O158" s="2" t="s">
         <v>5</v>
       </c>
@@ -8228,7 +8229,7 @@
       </c>
     </row>
     <row r="159" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N159" s="16"/>
+      <c r="N159" s="18"/>
       <c r="O159" s="4" t="s">
         <v>6</v>
       </c>
@@ -8252,7 +8253,7 @@
       </c>
     </row>
     <row r="160" spans="14:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N160" s="14" t="s">
+      <c r="N160" s="16" t="s">
         <v>34</v>
       </c>
       <c r="O160" s="6" t="s">
@@ -8278,7 +8279,7 @@
       </c>
     </row>
     <row r="161" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N161" s="15"/>
+      <c r="N161" s="17"/>
       <c r="O161" s="2" t="s">
         <v>3</v>
       </c>
@@ -8302,7 +8303,7 @@
       </c>
     </row>
     <row r="162" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N162" s="15"/>
+      <c r="N162" s="17"/>
       <c r="O162" s="2" t="s">
         <v>4</v>
       </c>
@@ -8326,7 +8327,7 @@
       </c>
     </row>
     <row r="163" spans="14:21" x14ac:dyDescent="0.35">
-      <c r="N163" s="15"/>
+      <c r="N163" s="17"/>
       <c r="O163" s="2" t="s">
         <v>5</v>
       </c>
@@ -8350,7 +8351,7 @@
       </c>
     </row>
     <row r="164" spans="14:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N164" s="16"/>
+      <c r="N164" s="18"/>
       <c r="O164" s="4" t="s">
         <v>6</v>
       </c>
@@ -8378,20 +8379,7 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="P33:T33"/>
-    <mergeCell ref="N85:N89"/>
-    <mergeCell ref="N95:N99"/>
-    <mergeCell ref="N90:N94"/>
-    <mergeCell ref="N100:N104"/>
-    <mergeCell ref="N35:N39"/>
-    <mergeCell ref="N40:N44"/>
-    <mergeCell ref="N45:N49"/>
-    <mergeCell ref="N50:N54"/>
-    <mergeCell ref="N55:N59"/>
-    <mergeCell ref="N60:N64"/>
-    <mergeCell ref="N65:N69"/>
-    <mergeCell ref="N70:N74"/>
-    <mergeCell ref="N75:N79"/>
+    <mergeCell ref="B1:B4"/>
     <mergeCell ref="N160:N164"/>
     <mergeCell ref="D1:I2"/>
     <mergeCell ref="N130:N134"/>
@@ -8407,7 +8395,20 @@
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="N150:N154"/>
     <mergeCell ref="N155:N159"/>
-    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="P33:T33"/>
+    <mergeCell ref="N85:N89"/>
+    <mergeCell ref="N95:N99"/>
+    <mergeCell ref="N90:N94"/>
+    <mergeCell ref="N100:N104"/>
+    <mergeCell ref="N35:N39"/>
+    <mergeCell ref="N40:N44"/>
+    <mergeCell ref="N45:N49"/>
+    <mergeCell ref="N50:N54"/>
+    <mergeCell ref="N55:N59"/>
+    <mergeCell ref="N60:N64"/>
+    <mergeCell ref="N65:N69"/>
+    <mergeCell ref="N70:N74"/>
+    <mergeCell ref="N75:N79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Make lines slightly more legible
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A12616-89CF-4A69-BF8C-FABD3D9A33D2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BCA84B-2619-4AD9-89FB-3A422899B619}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -387,7 +387,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1401438403497362E-2"/>
+          <c:y val="0.43235075621890146"/>
+          <c:w val="0.88081389386530395"/>
+          <c:h val="0.52339586791518633"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -406,7 +416,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -487,7 +497,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000000-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -506,7 +516,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -587,7 +597,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000001-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -606,7 +616,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -687,7 +697,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000002-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -706,7 +716,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -785,7 +795,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000003-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -804,10 +814,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -883,7 +894,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000004-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -902,7 +913,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -983,7 +994,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000005-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1002,12 +1013,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1085,7 +1097,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000006-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1104,12 +1116,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1191,7 +1204,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000007-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1210,12 +1223,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1297,7 +1311,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000008-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1316,7 +1330,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4">
                   <a:lumMod val="60000"/>
@@ -1403,7 +1417,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000009-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1422,12 +1436,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1509,7 +1522,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{0000000A-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1528,12 +1541,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1615,7 +1627,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{0000000B-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1634,12 +1646,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1719,7 +1728,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{0000000C-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1738,13 +1747,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1823,7 +1830,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{0000000D-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1842,7 +1849,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3">
                   <a:lumMod val="80000"/>
@@ -1932,7 +1939,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{0000000E-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1951,7 +1958,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4">
                   <a:lumMod val="80000"/>
@@ -2036,7 +2043,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{0000000F-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2055,7 +2062,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5">
                   <a:lumMod val="80000"/>
@@ -2145,7 +2152,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000010-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2164,7 +2171,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6">
                   <a:lumMod val="80000"/>
@@ -2254,7 +2261,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000011-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2273,12 +2280,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2360,7 +2366,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000012-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2379,12 +2385,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2466,7 +2473,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000013-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2485,11 +2492,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2572,7 +2577,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000014-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000014-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2591,12 +2596,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2674,7 +2678,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000015-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000015-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2693,7 +2697,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5">
                   <a:lumMod val="80000"/>
@@ -2776,7 +2780,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000016-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000016-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2795,7 +2799,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6">
                   <a:lumMod val="80000"/>
@@ -2882,7 +2886,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000017-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000017-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2901,7 +2905,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
@@ -2986,7 +2990,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000018-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000018-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3005,13 +3009,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="002060"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3095,7 +3097,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000019-A953-42C8-8CD2-4C6FC4AEA9AF}"/>
+              <c16:uniqueId val="{00000019-D497-4DEB-AA01-7755E50130A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3109,11 +3111,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1045938671"/>
-        <c:axId val="1044506415"/>
+        <c:axId val="1455736143"/>
+        <c:axId val="1318478671"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1045938671"/>
+        <c:axId val="1455736143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3154,16 +3156,24 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Input</a:t>
+                  <a:t>Number</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> size</a:t>
+                  <a:t> of inputs</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.49915932562481313"/>
+              <c:y val="0.93159470504083497"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3230,7 +3240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1044506415"/>
+        <c:crossAx val="1318478671"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3238,7 +3248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1044506415"/>
+        <c:axId val="1318478671"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3339,7 +3349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1045938671"/>
+        <c:crossAx val="1455736143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3992,22 +4002,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>441324</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>155574</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>568779</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12698</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6D0BE9-305C-443B-AF63-CD6958882DD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F43C777E-8ABA-440B-ABC1-29F0EEE39E57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4327,8 +4337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Make chart more legible
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BCA84B-2619-4AD9-89FB-3A422899B619}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3BF777-46A4-4F21-8D80-1716DB7085FB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -1545,7 +1545,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:prstDash val="sysDot"/>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1760,7 +1760,14 @@
             <c:symbol val="star"/>
             <c:size val="6"/>
             <c:spPr>
-              <a:noFill/>
+              <a:pattFill prst="pct5">
+                <a:fgClr>
+                  <a:schemeClr val="accent1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
@@ -2173,10 +2180,7 @@
           <c:spPr>
             <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2387,9 +2391,7 @@
           <c:spPr>
             <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
               <a:round/>
@@ -2598,7 +2600,7 @@
           <c:spPr>
             <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:prstDash val="dash"/>
               <a:round/>
@@ -3250,10 +3252,10 @@
       <c:valAx>
         <c:axId val="1318478671"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="10000"/>
-          <c:min val="1"/>
+          <c:max val="1024"/>
+          <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3352,6 +3354,8 @@
         <c:crossAx val="1455736143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4337,7 +4341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Move chart to not overlap headers
</commit_message>
<xml_diff>
--- a/Time Analysis.xlsx
+++ b/Time Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashi\Google Drive\Other\Programming\Java\Sorting-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3BF777-46A4-4F21-8D80-1716DB7085FB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17CBEEB-A05F-4C76-9718-19B379E45A79}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{1C7ACAA4-707A-4904-B8C4-4E7DBE1FFB51}"/>
   </bookViews>
@@ -278,8 +278,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,8 +296,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,8 +392,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.1401438403497362E-2"/>
-          <c:y val="0.43235075621890146"/>
+          <c:x val="8.9668578480354408E-2"/>
+          <c:y val="0.37139479082797267"/>
           <c:w val="0.88081389386530395"/>
           <c:h val="0.52339586791518633"/>
         </c:manualLayout>
@@ -4006,15 +4006,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>85480</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>24424</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>568779</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>12698</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>43682</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>37122</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4341,7 +4341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69077E36-5233-4F55-84DC-B14A1170E353}">
   <dimension ref="B1:U165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -4356,7 +4356,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="19" t="s">
@@ -4373,7 +4373,7 @@
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B2" s="21"/>
+      <c r="B2" s="15"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
@@ -4386,10 +4386,10 @@
       <c r="M2" s="11"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B3" s="21"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" s="21"/>
+      <c r="B4" s="15"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="13"/>
@@ -4478,13 +4478,13 @@
     <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="N33" s="10"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="15" t="s">
+      <c r="P33" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="N34" s="3"/>
@@ -8393,6 +8393,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="P33:T33"/>
+    <mergeCell ref="N85:N89"/>
+    <mergeCell ref="N95:N99"/>
+    <mergeCell ref="N90:N94"/>
+    <mergeCell ref="N100:N104"/>
+    <mergeCell ref="N35:N39"/>
+    <mergeCell ref="N40:N44"/>
+    <mergeCell ref="N45:N49"/>
+    <mergeCell ref="N50:N54"/>
+    <mergeCell ref="N55:N59"/>
+    <mergeCell ref="N60:N64"/>
+    <mergeCell ref="N65:N69"/>
+    <mergeCell ref="N70:N74"/>
+    <mergeCell ref="N75:N79"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="N160:N164"/>
     <mergeCell ref="D1:I2"/>
@@ -8409,20 +8423,6 @@
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="N150:N154"/>
     <mergeCell ref="N155:N159"/>
-    <mergeCell ref="P33:T33"/>
-    <mergeCell ref="N85:N89"/>
-    <mergeCell ref="N95:N99"/>
-    <mergeCell ref="N90:N94"/>
-    <mergeCell ref="N100:N104"/>
-    <mergeCell ref="N35:N39"/>
-    <mergeCell ref="N40:N44"/>
-    <mergeCell ref="N45:N49"/>
-    <mergeCell ref="N50:N54"/>
-    <mergeCell ref="N55:N59"/>
-    <mergeCell ref="N60:N64"/>
-    <mergeCell ref="N65:N69"/>
-    <mergeCell ref="N70:N74"/>
-    <mergeCell ref="N75:N79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>